<commit_message>
Correção dos metadados para matérias de 41 a 50
</commit_message>
<xml_diff>
--- a/projeto final/1 - levantamento/Matérias CD.xlsx
+++ b/projeto final/1 - levantamento/Matérias CD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caris\Desktop\IA024_deep_learning_nlp\projeto final\1 - levantamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4517880C-2E67-40F8-8191-AAD2DCF08A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0343715A-B69F-41A1-8B90-8CADFEE90A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="660" windowWidth="20730" windowHeight="11040" xr2:uid="{A25B0F39-AFD6-49AD-BAE6-0169C11C595E}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="638">
   <si>
     <t>Matéria</t>
   </si>
@@ -1998,9 +1998,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2338,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7617A561-B2B5-4674-8694-EA4F3B3BAE78}">
   <dimension ref="A1:E212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2540,6 +2541,9 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>637</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
@@ -2554,6 +2558,9 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>637</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2568,6 +2575,9 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>637</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
@@ -2582,6 +2592,9 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>637</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2596,6 +2609,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>637</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
@@ -2610,6 +2626,9 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>637</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
@@ -2624,6 +2643,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>637</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>51</v>
       </c>
@@ -2635,6 +2657,9 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>637</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>52</v>
       </c>
@@ -2649,6 +2674,9 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>637</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
@@ -2663,6 +2691,9 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>637</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>58</v>
       </c>
@@ -2677,6 +2708,9 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>637</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>61</v>
       </c>
@@ -2691,6 +2725,9 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>637</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>64</v>
       </c>
@@ -2705,6 +2742,9 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" t="s">
+        <v>637</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>67</v>
       </c>
@@ -2719,6 +2759,9 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>637</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>70</v>
       </c>
@@ -2733,6 +2776,9 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>637</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>73</v>
       </c>
@@ -2747,6 +2793,9 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>637</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>76</v>
       </c>
@@ -2761,6 +2810,9 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>637</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>79</v>
       </c>
@@ -2775,6 +2827,9 @@
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>637</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>82</v>
       </c>
@@ -2789,6 +2844,9 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>637</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>85</v>
       </c>
@@ -2803,6 +2861,9 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>637</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>88</v>
       </c>
@@ -2817,6 +2878,9 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>91</v>
       </c>
@@ -2831,6 +2895,9 @@
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>94</v>
       </c>
@@ -2845,6 +2912,9 @@
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C34" s="1" t="s">
         <v>97</v>
       </c>
@@ -2859,6 +2929,9 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C35" s="1" t="s">
         <v>100</v>
       </c>
@@ -2873,6 +2946,9 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C36" s="1" t="s">
         <v>103</v>
       </c>
@@ -2887,6 +2963,9 @@
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C37" s="1" t="s">
         <v>106</v>
       </c>
@@ -2901,6 +2980,9 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>109</v>
       </c>
@@ -2915,6 +2997,9 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C39" s="1" t="s">
         <v>112</v>
       </c>
@@ -2929,6 +3014,9 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C40" s="1" t="s">
         <v>115</v>
       </c>
@@ -2940,6 +3028,9 @@
       <c r="A41">
         <v>40</v>
       </c>
+      <c r="B41" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C41" s="1" t="s">
         <v>117</v>
       </c>
@@ -2954,6 +3045,9 @@
       <c r="A42">
         <v>41</v>
       </c>
+      <c r="B42" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C42" s="1" t="s">
         <v>120</v>
       </c>
@@ -2968,6 +3062,9 @@
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="B43" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C43" s="1" t="s">
         <v>123</v>
       </c>
@@ -2982,6 +3079,9 @@
       <c r="A44">
         <v>43</v>
       </c>
+      <c r="B44" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C44" s="1" t="s">
         <v>126</v>
       </c>
@@ -2996,6 +3096,9 @@
       <c r="A45">
         <v>44</v>
       </c>
+      <c r="B45" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C45" s="1" t="s">
         <v>129</v>
       </c>
@@ -3010,6 +3113,9 @@
       <c r="A46">
         <v>45</v>
       </c>
+      <c r="B46" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C46" s="1" t="s">
         <v>132</v>
       </c>
@@ -3024,6 +3130,9 @@
       <c r="A47">
         <v>46</v>
       </c>
+      <c r="B47" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C47" s="1" t="s">
         <v>135</v>
       </c>
@@ -3038,6 +3147,9 @@
       <c r="A48">
         <v>47</v>
       </c>
+      <c r="B48" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C48" s="1" t="s">
         <v>138</v>
       </c>
@@ -3052,6 +3164,9 @@
       <c r="A49">
         <v>48</v>
       </c>
+      <c r="B49" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C49" s="1" t="s">
         <v>141</v>
       </c>
@@ -3066,6 +3181,9 @@
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="C50" s="1" t="s">
         <v>144</v>
       </c>
@@ -3079,6 +3197,9 @@
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>637</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>147</v>
@@ -5960,6 +6081,7 @@
     <hyperlink ref="E212" r:id="rId626" xr:uid="{BF7B36EC-2642-4F9B-A942-FC7DA39117FB}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId627"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Corrige metadados das matérias 61-70. Apaga a matéria 54 (não há dados suficientes) e a substitui pela 211. A base agora passa a ter 210 matérias.
</commit_message>
<xml_diff>
--- a/projeto final/1 - levantamento/Matérias CD.xlsx
+++ b/projeto final/1 - levantamento/Matérias CD.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caris\Desktop\IA024_deep_learning_nlp\projeto final\1 - levantamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0343715A-B69F-41A1-8B90-8CADFEE90A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B98F8F-E94C-4F8B-93F8-BBE884BDD345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="660" windowWidth="20730" windowHeight="11040" xr2:uid="{A25B0F39-AFD6-49AD-BAE6-0169C11C595E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A25B0F39-AFD6-49AD-BAE6-0169C11C595E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tem transcrição" sheetId="1" r:id="rId1"/>
     <sheet name="Aguardando" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tem transcrição'!$C$1:$E$212</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tem transcrição'!$C$1:$E$211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="635">
   <si>
     <t>Matéria</t>
   </si>
@@ -517,15 +517,6 @@
   </si>
   <si>
     <t>https://www.camara.leg.br/internet/ordemdodia/integras/2273244.htm</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/noticias/956540-DEBATEDORES-APONTAM-ABUSOS-EM-CADASTROS-DE-CONSUMIDORES-FEITOS-POR-FARMACIAS</t>
-  </si>
-  <si>
-    <t>https://escriba.camara.leg.br/escriba-servicosweb/html/67618</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/internet/ordemdodia/integras/2264792.htm</t>
   </si>
   <si>
     <t>https://www.camara.leg.br/noticias/955138-SINDICATOS-CRITICAM-INCIDENCIA-DE-CONTRIBUICAO-DE-INATIVOS-SOBRE-VALORES-ACIMA-DO-MINIMO</t>
@@ -1998,10 +1989,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2337,14 +2327,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7617A561-B2B5-4674-8694-EA4F3B3BAE78}">
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" customWidth="1"/>
     <col min="4" max="4" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.140625" bestFit="1" customWidth="1"/>
@@ -2352,19 +2343,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B1" t="s">
+        <v>633</v>
+      </c>
+      <c r="C1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D1" t="s">
+        <v>631</v>
+      </c>
+      <c r="E1" t="s">
         <v>632</v>
-      </c>
-      <c r="B1" t="s">
-        <v>636</v>
-      </c>
-      <c r="C1" t="s">
-        <v>633</v>
-      </c>
-      <c r="D1" t="s">
-        <v>634</v>
-      </c>
-      <c r="E1" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2372,7 +2363,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -2389,7 +2380,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -2406,7 +2397,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -2423,7 +2414,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -2440,7 +2431,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -2457,7 +2448,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -2474,7 +2465,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -2491,7 +2482,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
@@ -2508,7 +2499,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -2525,7 +2516,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>31</v>
@@ -2542,7 +2533,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2559,7 +2550,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
@@ -2576,7 +2567,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
@@ -2593,7 +2584,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>41</v>
@@ -2610,7 +2601,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>44</v>
@@ -2627,7 +2618,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
@@ -2644,7 +2635,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>51</v>
@@ -2658,7 +2649,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>52</v>
@@ -2675,7 +2666,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>55</v>
@@ -2692,7 +2683,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>58</v>
@@ -2709,7 +2700,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>61</v>
@@ -2726,7 +2717,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>64</v>
@@ -2743,7 +2734,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>67</v>
@@ -2760,7 +2751,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>70</v>
@@ -2777,7 +2768,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>73</v>
@@ -2794,7 +2785,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>76</v>
@@ -2811,7 +2802,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>79</v>
@@ -2828,7 +2819,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>82</v>
@@ -2845,7 +2836,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>85</v>
@@ -2862,7 +2853,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>88</v>
@@ -2878,8 +2869,8 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>637</v>
+      <c r="B32" t="s">
+        <v>634</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>91</v>
@@ -2895,8 +2886,8 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>637</v>
+      <c r="B33" t="s">
+        <v>634</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>94</v>
@@ -2912,8 +2903,8 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>637</v>
+      <c r="B34" t="s">
+        <v>634</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>97</v>
@@ -2929,8 +2920,8 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>637</v>
+      <c r="B35" t="s">
+        <v>634</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>100</v>
@@ -2946,8 +2937,8 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>637</v>
+      <c r="B36" t="s">
+        <v>634</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>103</v>
@@ -2963,8 +2954,8 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>637</v>
+      <c r="B37" t="s">
+        <v>634</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>106</v>
@@ -2980,8 +2971,8 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>637</v>
+      <c r="B38" t="s">
+        <v>634</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>109</v>
@@ -2997,8 +2988,8 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>637</v>
+      <c r="B39" t="s">
+        <v>634</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>112</v>
@@ -3014,8 +3005,8 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>637</v>
+      <c r="B40" t="s">
+        <v>634</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>115</v>
@@ -3028,8 +3019,8 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>637</v>
+      <c r="B41" t="s">
+        <v>634</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>117</v>
@@ -3045,8 +3036,8 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>637</v>
+      <c r="B42" t="s">
+        <v>634</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>120</v>
@@ -3062,8 +3053,8 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>637</v>
+      <c r="B43" t="s">
+        <v>634</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>123</v>
@@ -3079,8 +3070,8 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>637</v>
+      <c r="B44" t="s">
+        <v>634</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>126</v>
@@ -3096,8 +3087,8 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>637</v>
+      <c r="B45" t="s">
+        <v>634</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>129</v>
@@ -3113,8 +3104,8 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>637</v>
+      <c r="B46" t="s">
+        <v>634</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>132</v>
@@ -3130,8 +3121,8 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>637</v>
+      <c r="B47" t="s">
+        <v>634</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>135</v>
@@ -3147,8 +3138,8 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>637</v>
+      <c r="B48" t="s">
+        <v>634</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>138</v>
@@ -3164,8 +3155,8 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>637</v>
+      <c r="B49" t="s">
+        <v>634</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>141</v>
@@ -3181,8 +3172,8 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>637</v>
+      <c r="B50" t="s">
+        <v>634</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>144</v>
@@ -3198,8 +3189,8 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>637</v>
+      <c r="B51" t="s">
+        <v>634</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>147</v>
@@ -3215,6 +3206,9 @@
       <c r="A52">
         <v>51</v>
       </c>
+      <c r="B52" t="s">
+        <v>634</v>
+      </c>
       <c r="C52" s="1" t="s">
         <v>150</v>
       </c>
@@ -3229,6 +3223,9 @@
       <c r="A53">
         <v>52</v>
       </c>
+      <c r="B53" t="s">
+        <v>634</v>
+      </c>
       <c r="C53" s="1" t="s">
         <v>155</v>
       </c>
@@ -3243,6 +3240,9 @@
       <c r="A54">
         <v>53</v>
       </c>
+      <c r="B54" t="s">
+        <v>634</v>
+      </c>
       <c r="C54" s="1" t="s">
         <v>156</v>
       </c>
@@ -3257,229 +3257,280 @@
       <c r="A55">
         <v>54</v>
       </c>
+      <c r="B55" t="s">
+        <v>634</v>
+      </c>
       <c r="C55" s="1" t="s">
-        <v>159</v>
+        <v>626</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>160</v>
+        <v>627</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>161</v>
+        <v>628</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
+      <c r="B56" t="s">
+        <v>634</v>
+      </c>
       <c r="C56" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
+      <c r="B57" t="s">
+        <v>634</v>
+      </c>
       <c r="C57" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
+      <c r="B58" t="s">
+        <v>634</v>
+      </c>
       <c r="C58" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
+      <c r="B59" t="s">
+        <v>634</v>
+      </c>
       <c r="C59" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
+      <c r="B60" t="s">
+        <v>634</v>
+      </c>
       <c r="C60" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
+      <c r="B61" t="s">
+        <v>634</v>
+      </c>
       <c r="C61" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
+      <c r="B62" t="s">
+        <v>634</v>
+      </c>
       <c r="C62" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
+      <c r="B63" t="s">
+        <v>634</v>
+      </c>
       <c r="C63" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
+      <c r="B64" t="s">
+        <v>634</v>
+      </c>
       <c r="C64" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
+      <c r="B65" t="s">
+        <v>634</v>
+      </c>
       <c r="C65" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
+      <c r="B66" t="s">
+        <v>634</v>
+      </c>
       <c r="C66" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
+      <c r="B67" t="s">
+        <v>634</v>
+      </c>
       <c r="C67" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
+      <c r="B68" t="s">
+        <v>634</v>
+      </c>
       <c r="C68" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
+      <c r="B69" t="s">
+        <v>634</v>
+      </c>
       <c r="C69" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
+      <c r="B70" t="s">
+        <v>634</v>
+      </c>
       <c r="C70" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
+      <c r="B71" t="s">
+        <v>634</v>
+      </c>
       <c r="C71" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3487,13 +3538,13 @@
         <v>71</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3501,13 +3552,13 @@
         <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3515,13 +3566,13 @@
         <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3529,13 +3580,13 @@
         <v>74</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3543,13 +3594,13 @@
         <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3557,13 +3608,13 @@
         <v>76</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3571,13 +3622,13 @@
         <v>77</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3585,13 +3636,13 @@
         <v>78</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3599,13 +3650,13 @@
         <v>79</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3613,13 +3664,13 @@
         <v>80</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3627,13 +3678,13 @@
         <v>81</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3641,13 +3692,13 @@
         <v>82</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3655,13 +3706,13 @@
         <v>83</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3669,13 +3720,13 @@
         <v>84</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3683,10 +3734,10 @@
         <v>85</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3694,13 +3745,13 @@
         <v>86</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3708,13 +3759,13 @@
         <v>87</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3722,13 +3773,13 @@
         <v>88</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3736,13 +3787,13 @@
         <v>89</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3750,13 +3801,13 @@
         <v>90</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3764,13 +3815,13 @@
         <v>91</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3778,13 +3829,13 @@
         <v>92</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3792,13 +3843,13 @@
         <v>93</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3806,13 +3857,13 @@
         <v>94</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3820,13 +3871,13 @@
         <v>95</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3834,13 +3885,13 @@
         <v>96</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3848,13 +3899,13 @@
         <v>97</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3862,10 +3913,10 @@
         <v>98</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3873,13 +3924,13 @@
         <v>99</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3887,13 +3938,13 @@
         <v>100</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3901,13 +3952,13 @@
         <v>101</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3915,13 +3966,13 @@
         <v>102</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3929,13 +3980,13 @@
         <v>103</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3943,13 +3994,13 @@
         <v>104</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3957,13 +4008,13 @@
         <v>105</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3971,13 +4022,13 @@
         <v>106</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3985,13 +4036,13 @@
         <v>107</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3999,13 +4050,13 @@
         <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -4013,13 +4064,13 @@
         <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4027,13 +4078,13 @@
         <v>110</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4041,13 +4092,13 @@
         <v>111</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4055,13 +4106,13 @@
         <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4069,13 +4120,13 @@
         <v>113</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4083,13 +4134,13 @@
         <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4097,13 +4148,13 @@
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4111,13 +4162,13 @@
         <v>116</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4125,13 +4176,13 @@
         <v>117</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4139,13 +4190,13 @@
         <v>118</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4153,13 +4204,13 @@
         <v>119</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4167,13 +4218,13 @@
         <v>120</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4181,13 +4232,13 @@
         <v>121</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4195,13 +4246,13 @@
         <v>122</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4209,13 +4260,13 @@
         <v>123</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4223,13 +4274,13 @@
         <v>124</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4237,13 +4288,13 @@
         <v>125</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4251,13 +4302,13 @@
         <v>126</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4265,13 +4316,13 @@
         <v>127</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4279,13 +4330,13 @@
         <v>128</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4293,13 +4344,13 @@
         <v>129</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4307,13 +4358,13 @@
         <v>130</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4321,13 +4372,13 @@
         <v>131</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4335,13 +4386,13 @@
         <v>132</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4349,13 +4400,13 @@
         <v>133</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4363,13 +4414,13 @@
         <v>134</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4377,13 +4428,13 @@
         <v>135</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4391,13 +4442,13 @@
         <v>136</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4405,13 +4456,13 @@
         <v>137</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4419,13 +4470,13 @@
         <v>138</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4433,13 +4484,13 @@
         <v>139</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4447,13 +4498,13 @@
         <v>140</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4461,13 +4512,13 @@
         <v>141</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4475,13 +4526,13 @@
         <v>142</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4489,13 +4540,13 @@
         <v>143</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4503,13 +4554,13 @@
         <v>144</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4517,13 +4568,13 @@
         <v>145</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4531,13 +4582,13 @@
         <v>146</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4545,13 +4596,13 @@
         <v>147</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4559,13 +4610,13 @@
         <v>148</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4573,13 +4624,13 @@
         <v>149</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4587,13 +4638,13 @@
         <v>150</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4601,13 +4652,13 @@
         <v>151</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4615,13 +4666,13 @@
         <v>152</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4629,13 +4680,13 @@
         <v>153</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4643,13 +4694,13 @@
         <v>154</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4657,13 +4708,13 @@
         <v>155</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4671,13 +4722,13 @@
         <v>156</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4685,13 +4736,13 @@
         <v>157</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4699,13 +4750,13 @@
         <v>158</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4713,13 +4764,13 @@
         <v>159</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4727,13 +4778,13 @@
         <v>160</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4741,13 +4792,13 @@
         <v>161</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4755,13 +4806,13 @@
         <v>162</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4769,13 +4820,13 @@
         <v>163</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4783,13 +4834,13 @@
         <v>164</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4797,13 +4848,13 @@
         <v>165</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4811,13 +4862,13 @@
         <v>166</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4825,13 +4876,13 @@
         <v>167</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4839,13 +4890,13 @@
         <v>168</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4853,13 +4904,13 @@
         <v>169</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4867,13 +4918,13 @@
         <v>170</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4881,13 +4932,13 @@
         <v>171</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4895,13 +4946,13 @@
         <v>172</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4909,13 +4960,13 @@
         <v>173</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4923,13 +4974,13 @@
         <v>174</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4937,13 +4988,13 @@
         <v>175</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4951,13 +5002,13 @@
         <v>176</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4965,13 +5016,13 @@
         <v>177</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4979,13 +5030,13 @@
         <v>178</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -4993,13 +5044,13 @@
         <v>179</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -5007,13 +5058,13 @@
         <v>180</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -5021,13 +5072,13 @@
         <v>181</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5035,13 +5086,13 @@
         <v>182</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5049,13 +5100,13 @@
         <v>183</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5063,13 +5114,13 @@
         <v>184</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5077,13 +5128,13 @@
         <v>185</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5091,13 +5142,13 @@
         <v>186</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5105,13 +5156,13 @@
         <v>187</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5119,13 +5170,13 @@
         <v>188</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5133,13 +5184,13 @@
         <v>189</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5147,13 +5198,13 @@
         <v>190</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5161,13 +5212,13 @@
         <v>191</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5175,13 +5226,13 @@
         <v>192</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5189,13 +5240,13 @@
         <v>193</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -5203,13 +5254,13 @@
         <v>194</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5217,13 +5268,13 @@
         <v>195</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -5231,13 +5282,13 @@
         <v>196</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5245,13 +5296,13 @@
         <v>197</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5259,13 +5310,13 @@
         <v>198</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5273,13 +5324,13 @@
         <v>199</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5287,13 +5338,13 @@
         <v>200</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5301,13 +5352,13 @@
         <v>201</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5315,13 +5366,13 @@
         <v>202</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5329,13 +5380,13 @@
         <v>203</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5343,13 +5394,13 @@
         <v>204</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5357,13 +5408,13 @@
         <v>205</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5371,13 +5422,13 @@
         <v>206</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5385,13 +5436,13 @@
         <v>207</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5399,13 +5450,13 @@
         <v>208</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5413,13 +5464,13 @@
         <v>209</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5427,27 +5478,13 @@
         <v>210</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212">
-        <v>211</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -5608,480 +5645,477 @@
     <hyperlink ref="C54" r:id="rId153" xr:uid="{9CBADF16-C123-4B5E-AB60-16AF747E8EF8}"/>
     <hyperlink ref="D54" r:id="rId154" xr:uid="{B92FE25E-6ECF-4065-94DC-0751F2096070}"/>
     <hyperlink ref="E54" r:id="rId155" xr:uid="{EE97DEB6-FBA7-4FC5-8857-01EC7D3DEB28}"/>
-    <hyperlink ref="C55" r:id="rId156" xr:uid="{0AED98B6-EEE9-4C14-8A51-BCC178E1283D}"/>
-    <hyperlink ref="D55" r:id="rId157" xr:uid="{3EBD29BF-9581-4C6F-B3F6-ACFE90C27CAF}"/>
-    <hyperlink ref="E55" r:id="rId158" xr:uid="{578BBD40-96E6-4281-B282-E68FB013238C}"/>
-    <hyperlink ref="C56" r:id="rId159" xr:uid="{93A3A603-A9B2-4D19-812A-74A36F16D1BC}"/>
-    <hyperlink ref="D56" r:id="rId160" xr:uid="{F3F43F43-E791-4A68-9487-58DD42F5F7B7}"/>
-    <hyperlink ref="E56" r:id="rId161" xr:uid="{E53FDCD2-A870-487C-83BB-B2F9355F084C}"/>
-    <hyperlink ref="E57" r:id="rId162" xr:uid="{95776386-802C-4E31-AB88-27B8CDF0F98E}"/>
-    <hyperlink ref="D57" r:id="rId163" xr:uid="{273B5CFE-28E9-4D37-8E20-9EEEFD512062}"/>
-    <hyperlink ref="C57" r:id="rId164" xr:uid="{CB726674-3850-4498-868B-9706F994615D}"/>
-    <hyperlink ref="C58" r:id="rId165" xr:uid="{B663A24C-0B6C-401D-AC91-CEDD5CC4C7B7}"/>
-    <hyperlink ref="D58" r:id="rId166" xr:uid="{2E990E0F-4E98-4C50-9D71-1E1591F61C5C}"/>
-    <hyperlink ref="E58" r:id="rId167" xr:uid="{A890A3C2-DD7A-4D54-AAD4-DE19A02AB080}"/>
-    <hyperlink ref="D59" r:id="rId168" xr:uid="{6B6FDF6B-3060-4EA4-A538-A32130409E58}"/>
-    <hyperlink ref="E59" r:id="rId169" xr:uid="{0B4BA579-1251-419C-83B7-16A2DE374221}"/>
-    <hyperlink ref="C59" r:id="rId170" xr:uid="{9FE2E172-5C41-4230-84CF-F6E914414453}"/>
-    <hyperlink ref="C60" r:id="rId171" xr:uid="{A3A1E70E-3606-43AB-959D-42D475EC026C}"/>
-    <hyperlink ref="D60" r:id="rId172" xr:uid="{05D726A8-B397-4927-9858-8A6F1E8C2C34}"/>
-    <hyperlink ref="E60" r:id="rId173" xr:uid="{E3E92A65-878C-4396-A979-259192CFE3FB}"/>
-    <hyperlink ref="C61" r:id="rId174" xr:uid="{9CDDC3F7-461B-41F6-A604-8C9AAF323690}"/>
-    <hyperlink ref="D61" r:id="rId175" xr:uid="{F9BD9FD8-27F4-433F-85B6-5B88A8B0B2EA}"/>
-    <hyperlink ref="E61" r:id="rId176" xr:uid="{036D4EDF-20C3-46C1-B910-16EFF6E50BBF}"/>
-    <hyperlink ref="C64" r:id="rId177" xr:uid="{2E1566B2-0D33-4DAB-8479-3FEEB5CD0159}"/>
-    <hyperlink ref="D64" r:id="rId178" xr:uid="{117EEFAC-1BA9-40E7-BF81-427F4E2C074D}"/>
-    <hyperlink ref="E64" r:id="rId179" xr:uid="{352858DF-5707-44F4-A4DD-C9D46E1C9188}"/>
-    <hyperlink ref="C65" r:id="rId180" xr:uid="{F83364B1-EDCD-40AE-B3E5-ADB81A08EB7C}"/>
-    <hyperlink ref="D65" r:id="rId181" xr:uid="{C78C668C-C893-42CE-89BA-9C9DC1B04B03}"/>
-    <hyperlink ref="E65" r:id="rId182" xr:uid="{E8577748-C8CE-4E73-BB98-1BB03AD9686A}"/>
-    <hyperlink ref="C66" r:id="rId183" xr:uid="{A58DB200-4FFE-4BF3-B93F-D7D768D15010}"/>
-    <hyperlink ref="D66" r:id="rId184" xr:uid="{63426EA7-EE17-4830-AD2C-B92AB219EFC9}"/>
-    <hyperlink ref="E66" r:id="rId185" xr:uid="{A528D6F6-6F96-4FDE-969E-517AEE4FDE49}"/>
-    <hyperlink ref="C67" r:id="rId186" xr:uid="{80D9D7A9-DD44-4211-9955-F61D7176460D}"/>
-    <hyperlink ref="D67" r:id="rId187" xr:uid="{D4A9E17D-57B2-46AE-8198-9B6AE21635E2}"/>
-    <hyperlink ref="E67" r:id="rId188" xr:uid="{714D4749-2A7B-491D-9FB8-1BF21E9A93A1}"/>
-    <hyperlink ref="C68" r:id="rId189" xr:uid="{B4C331B2-82CE-4B4E-94B3-88D151FEA07C}"/>
-    <hyperlink ref="D68" r:id="rId190" xr:uid="{C1C28575-633C-4333-AE20-6E34F0D2C138}"/>
-    <hyperlink ref="E68" r:id="rId191" xr:uid="{FE501029-2FFD-40EF-A6D2-E4F0980CB07B}"/>
-    <hyperlink ref="D69" r:id="rId192" xr:uid="{4E5BE45A-EE70-4A55-8813-6234D4AC22C3}"/>
-    <hyperlink ref="E69" r:id="rId193" xr:uid="{B6845F8F-30C8-434A-9566-8828D3FACB44}"/>
-    <hyperlink ref="C69" r:id="rId194" xr:uid="{42EC5C33-69F0-46DF-855B-9082D27FA37E}"/>
-    <hyperlink ref="C70" r:id="rId195" xr:uid="{B9C25BBF-2F1C-43AB-81D9-BA7D962E4B80}"/>
-    <hyperlink ref="D70" r:id="rId196" xr:uid="{7FAC267F-3E9F-431E-A5F7-E593B7A351C3}"/>
-    <hyperlink ref="E70" r:id="rId197" xr:uid="{931EEA1E-08EA-45E0-9646-E9D6D48A4F19}"/>
-    <hyperlink ref="C72" r:id="rId198" xr:uid="{2B570C9B-5283-429F-A6C6-071211DDB4CD}"/>
-    <hyperlink ref="D72" r:id="rId199" xr:uid="{DE416E21-0088-4A69-BD6D-D1C470435319}"/>
-    <hyperlink ref="E72" r:id="rId200" xr:uid="{D8837C3B-A0F9-4ED9-AA44-C440FB07A20C}"/>
-    <hyperlink ref="C73" r:id="rId201" xr:uid="{D6BD5389-04F2-4B58-9F33-AAA93C71092F}"/>
-    <hyperlink ref="D73" r:id="rId202" xr:uid="{7C93FBAB-8242-4810-A221-B083FC1513C1}"/>
-    <hyperlink ref="E73" r:id="rId203" xr:uid="{F0338AD3-0E74-4F5E-8444-AB3C55B8A664}"/>
-    <hyperlink ref="D74" r:id="rId204" xr:uid="{594C1034-31CE-4449-83AE-862B6480A46D}"/>
-    <hyperlink ref="E74" r:id="rId205" xr:uid="{30DAC341-1E00-4295-9B09-88B418393100}"/>
-    <hyperlink ref="C74" r:id="rId206" xr:uid="{4E97E308-91E7-4668-9B7F-2338C5857A08}"/>
-    <hyperlink ref="C75" r:id="rId207" xr:uid="{066BA063-0C85-4162-B074-0AAED730B020}"/>
-    <hyperlink ref="D75" r:id="rId208" xr:uid="{22128F9A-D8EF-4482-873E-5AB7553BCF20}"/>
-    <hyperlink ref="E75" r:id="rId209" xr:uid="{730102A0-62A5-4CA6-9C35-CB7BE66653A7}"/>
-    <hyperlink ref="D76" r:id="rId210" xr:uid="{92DE723E-DC1E-4E35-9F8A-DFC81658094A}"/>
-    <hyperlink ref="E76" r:id="rId211" xr:uid="{88C9AD40-1118-49F6-A915-7EAC16F870A2}"/>
-    <hyperlink ref="C76" r:id="rId212" xr:uid="{0DBA37A8-7096-4807-AC1B-4BEEFD66EA84}"/>
-    <hyperlink ref="C77" r:id="rId213" xr:uid="{83838767-AE02-4E24-9364-758023852C1B}"/>
-    <hyperlink ref="D77" r:id="rId214" xr:uid="{3C1F43CF-1207-4D08-A29C-EF841A48722C}"/>
-    <hyperlink ref="E77" r:id="rId215" xr:uid="{9D1B210A-0896-4875-B2FE-48517A0CA7F8}"/>
-    <hyperlink ref="D78" r:id="rId216" xr:uid="{A272A680-03CE-4750-A5EA-13B9BAD1DDA3}"/>
-    <hyperlink ref="E78" r:id="rId217" xr:uid="{F984F963-EDFC-4A31-BC8C-DE2561D61832}"/>
-    <hyperlink ref="C78" r:id="rId218" xr:uid="{68F9921C-BE67-40B9-8D57-068F721C5F32}"/>
-    <hyperlink ref="D79" r:id="rId219" xr:uid="{48B07033-F32B-4E27-9F43-BBA692FC8D29}"/>
-    <hyperlink ref="E79" r:id="rId220" xr:uid="{69916E72-32B0-4D28-9637-0EEFFADF74E8}"/>
-    <hyperlink ref="C79" r:id="rId221" xr:uid="{C8B9A133-0888-4E11-A670-EFF7CAC4ABFE}"/>
-    <hyperlink ref="D80" r:id="rId222" xr:uid="{0E15DC38-6EC8-4D48-8A86-F4AEB986ECDF}"/>
-    <hyperlink ref="E80" r:id="rId223" xr:uid="{36C1DDB0-E1FC-4E5D-949E-8F56A1E2E8FF}"/>
-    <hyperlink ref="C80" r:id="rId224" xr:uid="{B925BBDF-760B-4CD2-A22B-DB576A318F97}"/>
-    <hyperlink ref="D81" r:id="rId225" xr:uid="{5E1CFEEC-121E-4A0C-8D6E-1BE66A180602}"/>
-    <hyperlink ref="E81" r:id="rId226" xr:uid="{766EF454-F43A-4F23-8B1F-175DFBFA66C4}"/>
-    <hyperlink ref="C81" r:id="rId227" xr:uid="{F85622CB-5CD0-48DC-A9C2-D3B6BED83625}"/>
-    <hyperlink ref="D82" r:id="rId228" xr:uid="{022B4862-9904-438C-888E-088EFA87DF90}"/>
-    <hyperlink ref="E82" r:id="rId229" xr:uid="{DB096912-4591-4CA7-89B5-81A0A35646CE}"/>
-    <hyperlink ref="C82" r:id="rId230" xr:uid="{1DDD2058-A4A9-44F5-BA2A-2FC1A103A9F9}"/>
-    <hyperlink ref="C83" r:id="rId231" xr:uid="{3B08A944-BE8A-4F11-A43D-772558AE96DD}"/>
-    <hyperlink ref="D83" r:id="rId232" xr:uid="{27AB88EB-9DAF-4FA2-AA3A-E724287C8F93}"/>
-    <hyperlink ref="E83" r:id="rId233" xr:uid="{5BE5BE86-194D-42C1-86C0-0EB255719069}"/>
-    <hyperlink ref="D84" r:id="rId234" xr:uid="{70156D30-FCC6-4159-9748-163AA7650BFF}"/>
-    <hyperlink ref="E84" r:id="rId235" xr:uid="{AB61F21B-2647-4188-86EB-7A9EF52EAD4E}"/>
-    <hyperlink ref="C84" r:id="rId236" xr:uid="{AB845C66-110A-4E17-BA35-49424C8D9DB8}"/>
-    <hyperlink ref="C85" r:id="rId237" xr:uid="{4BEB7309-0983-4E2A-8044-81A5248547AD}"/>
-    <hyperlink ref="D85" r:id="rId238" xr:uid="{B47FB409-ABDE-45DB-91C0-653606E6F1FE}"/>
-    <hyperlink ref="E85" r:id="rId239" xr:uid="{9C948BFA-EE5F-4B1A-89B4-BF6DD4933F34}"/>
-    <hyperlink ref="D87" r:id="rId240" xr:uid="{A671B004-D342-45B8-BAA5-3E49FE2DE8BD}"/>
-    <hyperlink ref="E87" r:id="rId241" xr:uid="{C4019578-43D7-4898-AFB3-EAF1FF26E40C}"/>
-    <hyperlink ref="C87" r:id="rId242" xr:uid="{44B49121-69C0-4CB8-99B4-1D3604703C20}"/>
-    <hyperlink ref="D88" r:id="rId243" xr:uid="{9FB0C34A-F587-4BAE-9F2E-6FB5C63D9D1F}"/>
-    <hyperlink ref="E88" r:id="rId244" xr:uid="{F4E6ACF3-DFAA-477B-BE00-0211EEF43CD5}"/>
-    <hyperlink ref="C88" r:id="rId245" xr:uid="{77539DF1-1D8C-420E-8D0F-988850275481}"/>
-    <hyperlink ref="D89" r:id="rId246" xr:uid="{CB844098-58B7-4F8E-9B26-9BF7BCA817A0}"/>
-    <hyperlink ref="E89" r:id="rId247" xr:uid="{27CA033B-C8BD-4632-8C3B-BF86115051BF}"/>
-    <hyperlink ref="C89" r:id="rId248" xr:uid="{90338A87-20AE-4C6E-98E9-85613D1C7589}"/>
-    <hyperlink ref="D90" r:id="rId249" xr:uid="{A2814B89-6B87-4365-9C51-229D20F3F148}"/>
-    <hyperlink ref="E90" r:id="rId250" xr:uid="{880F7943-3A52-496B-A7C1-7EF72DDC2689}"/>
-    <hyperlink ref="C90" r:id="rId251" xr:uid="{0D7A2F28-4643-47C9-B897-7323740734E4}"/>
-    <hyperlink ref="C91" r:id="rId252" xr:uid="{6FAD943F-0A69-4BAF-AB56-35651FB59547}"/>
-    <hyperlink ref="D91" r:id="rId253" xr:uid="{1DE20C76-625A-4F4C-8C81-8D9C072645AF}"/>
-    <hyperlink ref="E91" r:id="rId254" xr:uid="{DB534690-3B61-4958-B81D-B687C80AA2E6}"/>
-    <hyperlink ref="C92" r:id="rId255" xr:uid="{F8F36C90-CCC9-4055-8BFD-CA71908A98D0}"/>
-    <hyperlink ref="D92" r:id="rId256" xr:uid="{7257BD60-D08C-4CBB-B7E5-8086A9C62A70}"/>
-    <hyperlink ref="E92" r:id="rId257" xr:uid="{57CB7722-444C-4E22-B23F-13AC9D1792A5}"/>
-    <hyperlink ref="C93" r:id="rId258" xr:uid="{7D8FD390-7977-4F5A-A4AE-D8AFF1779260}"/>
-    <hyperlink ref="D93" r:id="rId259" xr:uid="{C1952C13-045C-461F-8BC0-C9C86F08CAAE}"/>
-    <hyperlink ref="E93" r:id="rId260" xr:uid="{6593CB6B-985B-4C06-8E0B-4DD2A95CFB8C}"/>
-    <hyperlink ref="E94" r:id="rId261" xr:uid="{2033DE9C-AB68-4337-9666-E036632B48E9}"/>
-    <hyperlink ref="D94" r:id="rId262" xr:uid="{BC335142-CEB5-45DC-A6D5-CB1E1226051F}"/>
-    <hyperlink ref="C94" r:id="rId263" xr:uid="{373F113B-04B2-431D-8E11-05B90B52D390}"/>
-    <hyperlink ref="C95" r:id="rId264" xr:uid="{E3539E81-DF93-4A39-9945-36CEC9E34CF4}"/>
-    <hyperlink ref="D95" r:id="rId265" xr:uid="{D669F179-1AC6-4E08-96C5-C7BE89D41875}"/>
-    <hyperlink ref="E95" r:id="rId266" xr:uid="{CBC521FB-9833-4D60-918B-F3038613EC49}"/>
-    <hyperlink ref="D96" r:id="rId267" xr:uid="{1487A3FD-94F4-4C63-B36B-1C6236ACCCAA}"/>
-    <hyperlink ref="E96" r:id="rId268" xr:uid="{5F631273-96B3-48BB-A5C6-A8077E8EC752}"/>
-    <hyperlink ref="C96" r:id="rId269" xr:uid="{ADE8BEEA-ABC6-474A-A950-FF38898D34D2}"/>
-    <hyperlink ref="D97" r:id="rId270" xr:uid="{4DD3F6B0-4B1E-451C-9857-7B840584705D}"/>
-    <hyperlink ref="E97" r:id="rId271" xr:uid="{6DA9CE9D-442F-4DC5-BE8C-7745B1745575}"/>
-    <hyperlink ref="C97" r:id="rId272" xr:uid="{E59BA18D-2DA1-4FDF-9C1E-CD6D1A2620C7}"/>
-    <hyperlink ref="D98" r:id="rId273" xr:uid="{5C95BE55-05A0-4BE2-A224-2C4A40579DEE}"/>
-    <hyperlink ref="E98" r:id="rId274" xr:uid="{E2F28665-F304-48EB-AEE8-E289F7A4FC5A}"/>
-    <hyperlink ref="C98" r:id="rId275" xr:uid="{55201C98-C656-4EE7-A35F-CE17F44473C3}"/>
-    <hyperlink ref="C100" r:id="rId276" xr:uid="{79EA69E5-FEAB-4C20-B0DE-70A81655B6D4}"/>
-    <hyperlink ref="D100" r:id="rId277" xr:uid="{ED375E0D-1308-4908-9149-A0315A582320}"/>
-    <hyperlink ref="E100" r:id="rId278" xr:uid="{D46B35C8-21A4-4B52-ABFA-8A94A326F9D7}"/>
-    <hyperlink ref="C101" r:id="rId279" xr:uid="{E7ACECEC-3A28-4599-84B8-59BC02BF4FED}"/>
-    <hyperlink ref="D101" r:id="rId280" xr:uid="{465047FF-1256-4E45-AE8D-E5CEDB95F73F}"/>
-    <hyperlink ref="E101" r:id="rId281" xr:uid="{F30A2FC8-5BF5-487F-A934-EC4AC77FE211}"/>
-    <hyperlink ref="C102" r:id="rId282" xr:uid="{178FA5E3-E6A3-4365-9928-DC4296B031B7}"/>
-    <hyperlink ref="D102" r:id="rId283" xr:uid="{2487C55D-36B0-497C-8E7F-76864E5D2337}"/>
-    <hyperlink ref="E102" r:id="rId284" xr:uid="{9ABF0A5D-385F-4E38-95DF-7739D7794FCD}"/>
-    <hyperlink ref="C103" r:id="rId285" xr:uid="{5D123A8D-D901-4600-9E13-23B4081222A0}"/>
-    <hyperlink ref="D103" r:id="rId286" xr:uid="{B41BE957-8100-409E-8F6C-9FFF07208823}"/>
-    <hyperlink ref="E103" r:id="rId287" xr:uid="{7417B276-5872-4090-A0D9-C56E6230AB29}"/>
-    <hyperlink ref="C104" r:id="rId288" xr:uid="{2AC02C2A-F7B1-4CDE-8106-C0D377FFD10A}"/>
-    <hyperlink ref="D104" r:id="rId289" xr:uid="{CF5FB671-CD80-457E-9A5C-55AC19128002}"/>
-    <hyperlink ref="E104" r:id="rId290" xr:uid="{7EB7712F-F3D4-4CD0-928D-AA08612DA711}"/>
-    <hyperlink ref="C105" r:id="rId291" xr:uid="{3A98A613-5247-4EDD-9ED8-FFB31D28F72C}"/>
-    <hyperlink ref="D105" r:id="rId292" xr:uid="{B0F0B342-1498-46A9-BD50-0660E9657C90}"/>
-    <hyperlink ref="E105" r:id="rId293" xr:uid="{0B67D960-696C-427C-A875-D3B85CFF0762}"/>
-    <hyperlink ref="C106" r:id="rId294" xr:uid="{1DA3041A-7728-4026-B61E-A1AB5F15F5A8}"/>
-    <hyperlink ref="D106" r:id="rId295" xr:uid="{451E6F75-0E8E-49A5-8A5B-87255F93DD33}"/>
-    <hyperlink ref="E106" r:id="rId296" xr:uid="{D49DC68C-742B-425B-881B-A83AF4714EE4}"/>
-    <hyperlink ref="C107" r:id="rId297" xr:uid="{D226CEDC-443D-41F7-AD26-0AAF1BD9DB3F}"/>
-    <hyperlink ref="D107" r:id="rId298" xr:uid="{EF0F660D-62B8-4AA4-A272-57AB44F0E9CF}"/>
-    <hyperlink ref="E107" r:id="rId299" xr:uid="{3F4019C0-9C15-4B90-B9D3-90908DBCF849}"/>
-    <hyperlink ref="C108" r:id="rId300" xr:uid="{8B746AED-6ACC-4850-8828-FB6F0374D303}"/>
-    <hyperlink ref="D108" r:id="rId301" xr:uid="{F9014A66-3EE9-40DC-B87E-5D9054B50E5D}"/>
-    <hyperlink ref="E108" r:id="rId302" xr:uid="{4EE6DB51-0C8B-400C-A838-15E4BD633EE2}"/>
-    <hyperlink ref="C109" r:id="rId303" xr:uid="{FA69422B-0C15-4C8B-B074-46A3869AC7C9}"/>
-    <hyperlink ref="D109" r:id="rId304" xr:uid="{621EC68A-7ACE-45FB-88A3-06F720875DD7}"/>
-    <hyperlink ref="E109" r:id="rId305" xr:uid="{554DED57-0D82-433F-987B-1B34E1214C78}"/>
-    <hyperlink ref="C110" r:id="rId306" xr:uid="{4117E483-CA3B-487C-94D0-D68E8DB43993}"/>
-    <hyperlink ref="D110" r:id="rId307" xr:uid="{8AAA2CF2-8CC2-4067-AAC9-FA2A4EFE32DD}"/>
-    <hyperlink ref="E110" r:id="rId308" xr:uid="{66B74877-14BB-4AD3-8761-E581180779E3}"/>
-    <hyperlink ref="C111" r:id="rId309" xr:uid="{C527C048-13AF-4166-AAC3-24C05E9E601E}"/>
-    <hyperlink ref="D111" r:id="rId310" xr:uid="{2965799F-E19D-4831-A7B4-10AC9AAC4229}"/>
-    <hyperlink ref="E111" r:id="rId311" xr:uid="{44E6383F-DB4B-4F5D-BA87-405239E1E5E0}"/>
-    <hyperlink ref="C112" r:id="rId312" xr:uid="{714BC743-EB75-42ED-AF6E-B8B31923740F}"/>
-    <hyperlink ref="D112" r:id="rId313" xr:uid="{C53CEA57-5AB8-4F8D-BE5E-9B4CB9BD9BF5}"/>
-    <hyperlink ref="E112" r:id="rId314" xr:uid="{B6767105-A075-4865-AAC5-BF568E26C3DC}"/>
-    <hyperlink ref="C113" r:id="rId315" xr:uid="{DA3469AE-90EC-41E3-9216-B1C0BDA33A67}"/>
-    <hyperlink ref="D113" r:id="rId316" xr:uid="{557307AD-C5A9-4652-888D-A94FDF80009E}"/>
-    <hyperlink ref="E113" r:id="rId317" xr:uid="{C3DCCA91-9FBC-47D2-A94E-C1B437125A9A}"/>
-    <hyperlink ref="C114" r:id="rId318" xr:uid="{2906FCEE-6A7F-45B3-8BF5-7B231A0D23DB}"/>
-    <hyperlink ref="D114" r:id="rId319" xr:uid="{CBE1D2EA-6123-4939-A2F6-07C30E28EEE0}"/>
-    <hyperlink ref="E114" r:id="rId320" xr:uid="{31DAEDC2-35C0-48F5-A25B-93D7BF3A7450}"/>
-    <hyperlink ref="C115" r:id="rId321" xr:uid="{9E70ABF8-EABB-4B06-80D0-153AB8E19A7B}"/>
-    <hyperlink ref="D115" r:id="rId322" xr:uid="{327C9817-CBEE-4C9A-AAC6-464A863BEF9D}"/>
-    <hyperlink ref="E115" r:id="rId323" xr:uid="{A96FDAEB-0252-432D-A050-64EE5BE04F6D}"/>
-    <hyperlink ref="C116" r:id="rId324" xr:uid="{A4745FA3-0838-4B0A-8AF1-C0E8A9318E7A}"/>
-    <hyperlink ref="D116" r:id="rId325" xr:uid="{D592EA88-2676-4594-A3F8-755BA2197B17}"/>
-    <hyperlink ref="E116" r:id="rId326" xr:uid="{43298315-6704-4543-B6A3-1D12ED3BD89B}"/>
-    <hyperlink ref="C117" r:id="rId327" xr:uid="{4F507A97-E64C-4FA2-827D-A97B68F6502C}"/>
-    <hyperlink ref="D117" r:id="rId328" xr:uid="{89E85572-0309-4ECD-9E6F-6A8BFBDD0475}"/>
-    <hyperlink ref="E117" r:id="rId329" xr:uid="{6C735EE1-5379-4E04-87DC-61981092F13A}"/>
-    <hyperlink ref="C118" r:id="rId330" xr:uid="{DCB2DDD8-CEA1-4A83-927E-AA880D5F2465}"/>
-    <hyperlink ref="D118" r:id="rId331" xr:uid="{87B4582B-3A51-46CB-A7AA-14A53BEF2877}"/>
-    <hyperlink ref="E118" r:id="rId332" xr:uid="{95F3F337-662F-4DEB-899F-8B106C6AD582}"/>
-    <hyperlink ref="D119" r:id="rId333" xr:uid="{C6E03219-8688-46D5-858A-2C3BB7AC04D7}"/>
-    <hyperlink ref="E119" r:id="rId334" xr:uid="{222C944B-0CA2-4AA1-BFF7-664ED828CA3B}"/>
-    <hyperlink ref="C119" r:id="rId335" xr:uid="{50F33598-73F6-4B9D-8478-4AC6890A025A}"/>
-    <hyperlink ref="D120" r:id="rId336" xr:uid="{4AED68E4-2779-4CB0-B7AE-44AFAECA4499}"/>
-    <hyperlink ref="E120" r:id="rId337" xr:uid="{20510976-5BE1-4F80-89F3-DC95303A5BBF}"/>
-    <hyperlink ref="C120" r:id="rId338" xr:uid="{3842BBC2-0FE4-402C-A871-BFB50EE32BA0}"/>
-    <hyperlink ref="C121" r:id="rId339" xr:uid="{89D31CD8-B8E5-49D6-8FA5-D7A42F6CB540}"/>
-    <hyperlink ref="D121" r:id="rId340" xr:uid="{AC74A6C1-41F5-4315-92E2-A3C7ED59EBBD}"/>
-    <hyperlink ref="E121" r:id="rId341" xr:uid="{B1F093AF-7F7F-460F-A4F0-ADB6490D731B}"/>
-    <hyperlink ref="C122" r:id="rId342" xr:uid="{D4F65573-20F5-43D1-80BF-2795F41D9F57}"/>
-    <hyperlink ref="D122" r:id="rId343" xr:uid="{B88C2559-C22D-41ED-8F15-469DB6777B84}"/>
-    <hyperlink ref="E122" r:id="rId344" xr:uid="{EEA137CE-31F7-415B-94AB-CA2A55462E5C}"/>
-    <hyperlink ref="C123" r:id="rId345" xr:uid="{D997E317-1F11-4A83-B7F1-CF5217F8F4ED}"/>
-    <hyperlink ref="D123" r:id="rId346" xr:uid="{C9088CDA-1F58-4681-9DAD-82F7D0583EE5}"/>
-    <hyperlink ref="E123" r:id="rId347" xr:uid="{830325FC-B5CA-4053-8D5D-6DA5A0E9CEB3}"/>
-    <hyperlink ref="C124" r:id="rId348" xr:uid="{5AC4D217-D8FE-4409-862F-FAA5A86520AC}"/>
-    <hyperlink ref="D124" r:id="rId349" xr:uid="{CE468356-AB38-423F-ACE7-04587D99102E}"/>
-    <hyperlink ref="E124" r:id="rId350" xr:uid="{611001F6-2221-481D-AFA1-35DB4D386424}"/>
-    <hyperlink ref="C125" r:id="rId351" xr:uid="{FCC30E1C-7F83-4581-822A-7F2ACF21B208}"/>
-    <hyperlink ref="D125" r:id="rId352" xr:uid="{3A097561-C99B-452A-B5F9-14E12478CA8E}"/>
-    <hyperlink ref="E125" r:id="rId353" xr:uid="{5847BD3E-972F-4164-8556-AAACBBA355DB}"/>
-    <hyperlink ref="C126" r:id="rId354" xr:uid="{3BCC14C6-3272-4FB5-B30F-233B0FFAA229}"/>
-    <hyperlink ref="D126" r:id="rId355" xr:uid="{D87B0C63-927A-423F-9DEE-FB163765706A}"/>
-    <hyperlink ref="E126" r:id="rId356" xr:uid="{8D18C038-05BE-41FB-9589-349C2DB35EB6}"/>
-    <hyperlink ref="C127" r:id="rId357" xr:uid="{212AE7B7-8417-4613-9B01-457D5FAD32E2}"/>
-    <hyperlink ref="D127" r:id="rId358" xr:uid="{16169750-2789-41D4-92EE-8370C62CF1BA}"/>
-    <hyperlink ref="E127" r:id="rId359" xr:uid="{EF236839-B3F1-4D2A-8793-A6E0A9D52328}"/>
-    <hyperlink ref="C128" r:id="rId360" xr:uid="{13F5A019-E7BD-473A-8BFB-051E885B1146}"/>
-    <hyperlink ref="D128" r:id="rId361" xr:uid="{C06C249C-A9D7-4BAE-AD6C-0ECED61AA088}"/>
-    <hyperlink ref="E128" r:id="rId362" xr:uid="{C2493638-1F36-426C-A65E-9BA0E883C835}"/>
-    <hyperlink ref="C129" r:id="rId363" xr:uid="{7F246417-F2E2-4CEF-ACB8-0C0E87FFBD79}"/>
-    <hyperlink ref="D129" r:id="rId364" xr:uid="{77141049-FDE6-4B29-8926-A7256E4C0505}"/>
-    <hyperlink ref="E129" r:id="rId365" xr:uid="{F98DCA20-9796-418E-B8CA-A3E005647A01}"/>
-    <hyperlink ref="C130" r:id="rId366" xr:uid="{0BA229B0-06A2-4C48-9914-A5374B32A34F}"/>
-    <hyperlink ref="D130" r:id="rId367" xr:uid="{3F506EBE-0BD0-4794-87C1-953206B16CD4}"/>
-    <hyperlink ref="E130" r:id="rId368" xr:uid="{A615BCEB-72DE-43C7-8A07-693C54D3A0C4}"/>
-    <hyperlink ref="C131" r:id="rId369" xr:uid="{07FCC78B-BF39-43FB-A89D-700B9FB2D824}"/>
-    <hyperlink ref="D131" r:id="rId370" xr:uid="{12B43D3A-B1AA-41D0-8A47-1DDC5FBC02CC}"/>
-    <hyperlink ref="E131" r:id="rId371" xr:uid="{E1EB98C2-E2CA-4E94-8439-8B789E3754E7}"/>
-    <hyperlink ref="D132" r:id="rId372" xr:uid="{63468E1D-F523-48BF-8225-D649FBE847EC}"/>
-    <hyperlink ref="E132" r:id="rId373" xr:uid="{4D681694-A038-4227-BC2E-F2651367ACF3}"/>
-    <hyperlink ref="C132" r:id="rId374" xr:uid="{D7ECE862-4574-486D-A9A4-78F8E4FC1681}"/>
-    <hyperlink ref="C133" r:id="rId375" xr:uid="{B156B9CD-29C4-4D78-8EBA-515A4C1B6B5A}"/>
-    <hyperlink ref="D133" r:id="rId376" xr:uid="{DA45D1F5-4AD3-4F4C-8A29-855166DF6940}"/>
-    <hyperlink ref="E133" r:id="rId377" xr:uid="{596A4EF2-4527-401B-A2CE-FA6A6AE241FF}"/>
-    <hyperlink ref="C134" r:id="rId378" xr:uid="{DC92B3C9-52B9-4D63-AC4A-1FE80AD38A7B}"/>
-    <hyperlink ref="D134" r:id="rId379" xr:uid="{6653B8D2-7773-4FD1-8AB6-76B074FA4AAA}"/>
-    <hyperlink ref="E134" r:id="rId380" xr:uid="{58D58C73-9A50-44A9-A0EA-5592206BB72F}"/>
-    <hyperlink ref="C135" r:id="rId381" xr:uid="{CF269375-1231-4422-9D05-86CA9413B1AD}"/>
-    <hyperlink ref="D135" r:id="rId382" xr:uid="{7AF85C45-2D0F-4BF2-8039-612435A7F999}"/>
-    <hyperlink ref="E135" r:id="rId383" xr:uid="{B39AC57D-61C7-4384-92C0-FA4D3C141F31}"/>
-    <hyperlink ref="C136" r:id="rId384" xr:uid="{F5D55CD9-3B76-4FD8-AC67-16192C305D26}"/>
-    <hyperlink ref="D136" r:id="rId385" xr:uid="{48D8B605-74CE-472F-AFDD-08EC6689007C}"/>
-    <hyperlink ref="E136" r:id="rId386" xr:uid="{44FF3624-E323-438F-8CAB-68D1CB08688C}"/>
-    <hyperlink ref="C137" r:id="rId387" xr:uid="{CE592AC5-E5D6-495B-BB1B-85E6B7EE95DA}"/>
-    <hyperlink ref="D137" r:id="rId388" xr:uid="{D0AD0ECF-67E1-4B11-91F5-AA23D31475D4}"/>
-    <hyperlink ref="E137" r:id="rId389" xr:uid="{CA7CD45E-3E5B-4C2E-93A9-84848C1A52F2}"/>
-    <hyperlink ref="C138" r:id="rId390" xr:uid="{971AEABA-C26E-4CD2-B617-7E7AEFA79225}"/>
-    <hyperlink ref="D138" r:id="rId391" xr:uid="{E838D43A-FA34-4E17-A12D-60A467F149C2}"/>
-    <hyperlink ref="E138" r:id="rId392" xr:uid="{31F37E78-12DF-444E-A3FB-EF00403D39D4}"/>
-    <hyperlink ref="C139" r:id="rId393" xr:uid="{7DC70FA2-2641-4F66-B9F8-01F68ED70F02}"/>
-    <hyperlink ref="D139" r:id="rId394" xr:uid="{B963012C-FACA-4A11-B1C4-313CF3F6387F}"/>
-    <hyperlink ref="E139" r:id="rId395" xr:uid="{E1DCAB4B-878B-4C50-97B6-B5A5D2A2FADD}"/>
-    <hyperlink ref="C140" r:id="rId396" xr:uid="{60F58296-9148-4312-9D0C-BF4DE0690B91}"/>
-    <hyperlink ref="D140" r:id="rId397" xr:uid="{8DBCCAC8-BC9E-442F-A475-9F8639697DB9}"/>
-    <hyperlink ref="E140" r:id="rId398" xr:uid="{0B4BC81F-7CB5-41BC-88B0-3B2BBBE80A3F}"/>
-    <hyperlink ref="D141" r:id="rId399" xr:uid="{9A0BB159-B669-435C-9CB1-A2BA4C4091A9}"/>
-    <hyperlink ref="E141" r:id="rId400" xr:uid="{0055782C-E077-4204-8FF9-57BE6F8FED26}"/>
-    <hyperlink ref="C141" r:id="rId401" xr:uid="{FE323C66-30FE-40E0-8F0E-4108D9EC2713}"/>
-    <hyperlink ref="C142" r:id="rId402" xr:uid="{666B5CC7-4AFE-4EE4-93A2-099371C034E3}"/>
-    <hyperlink ref="D142" r:id="rId403" xr:uid="{A9DFF398-3782-4606-A5AD-16EB49874249}"/>
-    <hyperlink ref="E142" r:id="rId404" xr:uid="{CB3B62B3-3706-4AEA-B831-85D12973AAFB}"/>
-    <hyperlink ref="C143" r:id="rId405" xr:uid="{5B3C3EC4-7E86-40AB-980C-956D883C0DE8}"/>
-    <hyperlink ref="D143" r:id="rId406" xr:uid="{E58660DA-18E4-456D-AE6E-157A8C791640}"/>
-    <hyperlink ref="E143" r:id="rId407" xr:uid="{30D38FD6-524A-4260-A893-C02ABC8FD7D8}"/>
-    <hyperlink ref="C144" r:id="rId408" xr:uid="{EAA73046-9047-4BE9-A054-E3310DE63E1A}"/>
-    <hyperlink ref="D144" r:id="rId409" xr:uid="{54E7A160-9887-4A15-A5E4-7E98C3B546B1}"/>
-    <hyperlink ref="E144" r:id="rId410" xr:uid="{5BA4E4AA-D08F-40BB-B211-CD81B18FF87A}"/>
-    <hyperlink ref="C145" r:id="rId411" xr:uid="{E57FE190-B789-4567-B86E-2D8DD5BB470A}"/>
-    <hyperlink ref="D145" r:id="rId412" xr:uid="{303EC3AA-5A58-4C68-97E5-480D5E8B49ED}"/>
-    <hyperlink ref="E145" r:id="rId413" xr:uid="{111A682B-10E9-494F-BA71-FEC4F7FB0BD6}"/>
-    <hyperlink ref="C146" r:id="rId414" xr:uid="{E353A765-41EF-43C2-AB89-89DFAEA7EAB7}"/>
-    <hyperlink ref="D146" r:id="rId415" xr:uid="{6DB31883-29E3-4B37-A5BC-B8A2B95FBC29}"/>
-    <hyperlink ref="E146" r:id="rId416" xr:uid="{FCF11283-83AE-42A7-BB7D-85631FD6E8B9}"/>
-    <hyperlink ref="C147" r:id="rId417" xr:uid="{2CA57331-C3C7-4E12-82CB-C628ECE4CCAB}"/>
-    <hyperlink ref="D147" r:id="rId418" xr:uid="{B5E1FE84-C98A-420D-837D-C3DCBB95E91F}"/>
-    <hyperlink ref="E147" r:id="rId419" xr:uid="{20932CE8-F8AE-4689-9CD7-3D080869A55D}"/>
-    <hyperlink ref="C148" r:id="rId420" xr:uid="{7618A490-B688-42C9-94E0-4F8540FF40DB}"/>
-    <hyperlink ref="D148" r:id="rId421" xr:uid="{668BB9C5-109F-4A7E-868C-D2732EFA34A2}"/>
-    <hyperlink ref="E148" r:id="rId422" xr:uid="{0F731946-786D-4814-BAE4-8D0C99005D78}"/>
-    <hyperlink ref="C149" r:id="rId423" xr:uid="{51F53306-B34E-472A-B470-69B8029C9ED4}"/>
-    <hyperlink ref="D149" r:id="rId424" xr:uid="{F2FEECB1-F3BC-4C78-B544-613C7FF5E436}"/>
-    <hyperlink ref="E149" r:id="rId425" xr:uid="{343909DC-77D4-4FBB-BE02-DCD4EC0C20EB}"/>
-    <hyperlink ref="C150" r:id="rId426" xr:uid="{F187FD4D-E765-4937-9701-2C58603180AE}"/>
-    <hyperlink ref="D150" r:id="rId427" xr:uid="{31FB4D76-B008-46DB-9637-691B1894CE21}"/>
-    <hyperlink ref="E150" r:id="rId428" xr:uid="{03572D9E-807D-4918-B128-29411ACBB625}"/>
-    <hyperlink ref="C151" r:id="rId429" xr:uid="{5130DE5E-46EF-4B05-8FE0-179C2E7E6948}"/>
-    <hyperlink ref="D151" r:id="rId430" xr:uid="{97742F59-5F59-4D68-996E-0A272575FADC}"/>
-    <hyperlink ref="E151" r:id="rId431" xr:uid="{2355B201-6EF9-4A6A-A9B9-BF166EC28606}"/>
-    <hyperlink ref="C152" r:id="rId432" xr:uid="{407F15B9-9D77-4AFB-B5E8-1B163C7E370E}"/>
-    <hyperlink ref="D152" r:id="rId433" xr:uid="{7A5EB5DE-BDC8-4E93-9761-A6603D00EFAD}"/>
-    <hyperlink ref="E152" r:id="rId434" xr:uid="{097CE107-4BA7-4CF3-996A-093477F670F6}"/>
-    <hyperlink ref="D153" r:id="rId435" xr:uid="{51B6FCED-FA56-433D-BA3D-445C0F2FE651}"/>
-    <hyperlink ref="E153" r:id="rId436" xr:uid="{26C3E259-1ACD-4F3A-B70D-194C131947DB}"/>
-    <hyperlink ref="C153" r:id="rId437" xr:uid="{3A114C26-8E8C-45B9-94BD-FCD3CAA9597E}"/>
-    <hyperlink ref="C154" r:id="rId438" xr:uid="{9AA9391F-DE63-4135-A127-DF0F47F7D8C7}"/>
-    <hyperlink ref="D154" r:id="rId439" xr:uid="{2BF42871-0750-440A-A243-619A1C20CC7F}"/>
-    <hyperlink ref="E154" r:id="rId440" xr:uid="{D39D1674-E469-410B-9639-99835CA9A908}"/>
-    <hyperlink ref="C155" r:id="rId441" xr:uid="{5F3DC677-1855-4283-B201-795E598B8917}"/>
-    <hyperlink ref="D155" r:id="rId442" xr:uid="{97F71AB0-0556-481D-B3A2-984C5AB5ED3A}"/>
-    <hyperlink ref="E155" r:id="rId443" xr:uid="{F4091531-5EEE-42BF-9549-D3422C21479A}"/>
-    <hyperlink ref="C156" r:id="rId444" xr:uid="{09680C2A-D8C5-41B4-9F07-96FF1792918C}"/>
-    <hyperlink ref="D156" r:id="rId445" xr:uid="{B9850E60-1546-4D20-8BF8-E8A5C91504C9}"/>
-    <hyperlink ref="E156" r:id="rId446" xr:uid="{CB7D6C00-6A72-4633-A0C4-CA7AD5F7CA43}"/>
-    <hyperlink ref="C157" r:id="rId447" xr:uid="{80024236-A643-48BC-A603-88E4C61F39E9}"/>
-    <hyperlink ref="D157" r:id="rId448" xr:uid="{120C8743-AA48-4C9A-AE55-5610BE126DC3}"/>
-    <hyperlink ref="E157" r:id="rId449" xr:uid="{2D5BB430-5FE3-453B-A9D2-87D25EF175BD}"/>
-    <hyperlink ref="C158" r:id="rId450" xr:uid="{4DFB4F67-145A-44E0-BE4E-70236393A673}"/>
-    <hyperlink ref="D158" r:id="rId451" xr:uid="{63643BC2-FC62-42D6-82C6-75379B5F7031}"/>
-    <hyperlink ref="E158" r:id="rId452" xr:uid="{6CF4B868-96BA-46BA-B87F-853852F4531D}"/>
-    <hyperlink ref="C159" r:id="rId453" xr:uid="{352410C9-FE4B-4A2C-BC1F-750169232690}"/>
-    <hyperlink ref="D159" r:id="rId454" xr:uid="{AFE88A43-637E-4B75-B37A-1F57451F4619}"/>
-    <hyperlink ref="E159" r:id="rId455" xr:uid="{7535847A-C949-43A9-93A4-F0EC6DDF68DA}"/>
-    <hyperlink ref="C160" r:id="rId456" xr:uid="{4C1038DE-1D54-48E4-8E66-F691E40DCC63}"/>
-    <hyperlink ref="D160" r:id="rId457" xr:uid="{41172669-0845-43AD-9650-8B8A62925666}"/>
-    <hyperlink ref="E160" r:id="rId458" xr:uid="{B16881C8-92C0-4AA1-B859-DBDCB15AD570}"/>
-    <hyperlink ref="C161" r:id="rId459" xr:uid="{39A2F065-2C25-448A-8687-9F2149D01184}"/>
-    <hyperlink ref="D161" r:id="rId460" xr:uid="{F2ED0C3A-0135-4147-AEFF-DC4B8ED0D685}"/>
-    <hyperlink ref="E161" r:id="rId461" xr:uid="{8DF3594C-0BF9-448B-A503-24794FCECEA3}"/>
-    <hyperlink ref="D162" r:id="rId462" xr:uid="{2D27BDFB-D4B5-44B9-965C-A93682BCB150}"/>
-    <hyperlink ref="E162" r:id="rId463" xr:uid="{744A7EC5-AEB8-42E3-A556-E4E16C245E49}"/>
-    <hyperlink ref="C162" r:id="rId464" xr:uid="{1A5BE688-8DAF-46EE-BE55-B56FA387D60A}"/>
-    <hyperlink ref="C163" r:id="rId465" xr:uid="{A2A8969B-E67C-4C42-9F40-97418205870F}"/>
-    <hyperlink ref="D163" r:id="rId466" xr:uid="{8C15BC14-EB1D-4AFA-82A9-D7F5FEB92B34}"/>
-    <hyperlink ref="E163" r:id="rId467" xr:uid="{C1AF09A0-75AC-415B-AEAA-FFE6CDF5282B}"/>
-    <hyperlink ref="C164" r:id="rId468" xr:uid="{97A7FD74-2B85-4FD7-96FD-C28091A20A4D}"/>
-    <hyperlink ref="D164" r:id="rId469" xr:uid="{8C7ACE0C-84B0-4967-A6EA-73EBBBCA6E3A}"/>
-    <hyperlink ref="E164" r:id="rId470" xr:uid="{63C7876B-76A9-4A33-B78B-52C0CA2D8D5E}"/>
-    <hyperlink ref="C165" r:id="rId471" xr:uid="{06B4DEBF-7C8E-4884-91BE-A793EE0F62CC}"/>
-    <hyperlink ref="D165" r:id="rId472" xr:uid="{A9147945-5306-4AE5-BE85-C90C7FC7EC3C}"/>
-    <hyperlink ref="E165" r:id="rId473" xr:uid="{77243768-5B39-4BB1-BA96-960A09265D09}"/>
-    <hyperlink ref="D166" r:id="rId474" xr:uid="{0D2C4551-5A3A-4398-A3D2-99FB0401A7D1}"/>
-    <hyperlink ref="E166" r:id="rId475" xr:uid="{38A6A660-830B-4694-A398-A9DE1011AC6B}"/>
-    <hyperlink ref="C166" r:id="rId476" xr:uid="{5228C198-AF2C-40F8-B2F5-057085C54F0D}"/>
-    <hyperlink ref="C167" r:id="rId477" xr:uid="{A08507FD-CA4F-44FD-80EA-F0484A51F904}"/>
-    <hyperlink ref="D167" r:id="rId478" xr:uid="{F9694B45-4A2C-4F66-8EE4-DA8EE40951ED}"/>
-    <hyperlink ref="E167" r:id="rId479" xr:uid="{C3119FB8-069B-4D3F-B5C3-5883D3A505F1}"/>
-    <hyperlink ref="C168" r:id="rId480" xr:uid="{AA2D388E-48CF-41C9-B888-4F64BFF2ACC5}"/>
-    <hyperlink ref="D168" r:id="rId481" xr:uid="{136A9ACA-B873-408C-877B-B88BEDEE02DE}"/>
-    <hyperlink ref="E168" r:id="rId482" xr:uid="{45143C2B-0CE5-460D-8C8C-7BDD7391EC20}"/>
-    <hyperlink ref="C169" r:id="rId483" xr:uid="{412AABCD-D11B-4C1F-BAE3-8E9B5314FEFE}"/>
-    <hyperlink ref="D169" r:id="rId484" xr:uid="{52143DB4-9220-420E-9325-C79A91D3E77F}"/>
-    <hyperlink ref="E169" r:id="rId485" xr:uid="{EBD5079E-6759-45C1-A040-15A1D7EFA833}"/>
-    <hyperlink ref="C170" r:id="rId486" xr:uid="{D9EDA746-00FA-479B-BBF8-E6EA24906B94}"/>
-    <hyperlink ref="D170" r:id="rId487" xr:uid="{F2F02B4C-A61F-48DB-B4B9-B590F1EAE1A5}"/>
-    <hyperlink ref="E170" r:id="rId488" xr:uid="{4EF3DEB5-F631-42E5-BF23-8FD5BD7C5726}"/>
-    <hyperlink ref="C171" r:id="rId489" xr:uid="{C7AC3295-F2D7-4B73-81FE-CE9DD8908E72}"/>
-    <hyperlink ref="D171" r:id="rId490" xr:uid="{13A8A69F-88CE-42AE-A904-E26015719290}"/>
-    <hyperlink ref="E171" r:id="rId491" xr:uid="{69E9CB21-248F-4A60-986D-523E9D222CCD}"/>
-    <hyperlink ref="C172" r:id="rId492" xr:uid="{7627DCB7-8878-43A8-B6E9-AA0B9A8AA69D}"/>
-    <hyperlink ref="D172" r:id="rId493" xr:uid="{FCCBB0CF-B9DD-4759-BBA3-76BD72CDE47E}"/>
-    <hyperlink ref="E172" r:id="rId494" xr:uid="{3E811DA2-3C40-4364-9266-6773CDEE5611}"/>
-    <hyperlink ref="C173" r:id="rId495" xr:uid="{FC27C7F6-56D3-4353-B218-AEDBD69411BE}"/>
-    <hyperlink ref="D173" r:id="rId496" xr:uid="{1FAEEA19-C0F2-4B64-AB53-5CE1FCFD3EED}"/>
-    <hyperlink ref="E173" r:id="rId497" xr:uid="{9AFEB9F6-C42C-4F69-BAB9-0F96228BAB75}"/>
-    <hyperlink ref="C174" r:id="rId498" xr:uid="{782E6140-94C3-407F-BEAF-9C0D976620EB}"/>
-    <hyperlink ref="D174" r:id="rId499" xr:uid="{B6A4BB4A-CEE1-4126-85FD-8A0A92A86F6C}"/>
-    <hyperlink ref="E174" r:id="rId500" xr:uid="{4DE847BB-899E-400F-B0A1-5368BD326435}"/>
-    <hyperlink ref="C175" r:id="rId501" xr:uid="{550B60D7-37BE-42DF-A0A6-234EE2ABEC88}"/>
-    <hyperlink ref="D175" r:id="rId502" xr:uid="{FE54EAA5-5BCB-4AE8-B0F0-DF219D75D2FA}"/>
-    <hyperlink ref="E175" r:id="rId503" xr:uid="{5F404BDE-7004-4B15-8063-6FFDD0232C10}"/>
-    <hyperlink ref="D176" r:id="rId504" xr:uid="{04847EC6-CA8E-40B5-A255-4AA69821E9CD}"/>
-    <hyperlink ref="E176" r:id="rId505" xr:uid="{C5321455-60AF-4B1F-B2EB-9C48ABE6CF88}"/>
-    <hyperlink ref="C176" r:id="rId506" xr:uid="{F487FA1F-6345-4747-9B2D-E8B2F3CA8F64}"/>
-    <hyperlink ref="C177" r:id="rId507" xr:uid="{0BB76D84-05E9-403F-B67C-C3BFFCCC1DE9}"/>
-    <hyperlink ref="D177" r:id="rId508" xr:uid="{E68DE772-C262-43D4-BAB1-57B7508710F5}"/>
-    <hyperlink ref="E177" r:id="rId509" xr:uid="{E2FD5107-217F-4912-8F1C-CBCA0456D0B1}"/>
-    <hyperlink ref="C178" r:id="rId510" xr:uid="{0709A472-9980-4F85-A449-8A5D6EABD5F4}"/>
-    <hyperlink ref="D178" r:id="rId511" xr:uid="{31C86E75-E56D-4C5A-965A-002F4B567CEA}"/>
-    <hyperlink ref="E178" r:id="rId512" xr:uid="{A44C8FE0-0122-4430-BB7B-95FC5AC20FD1}"/>
-    <hyperlink ref="C179" r:id="rId513" xr:uid="{6CA3E827-405F-40BE-9BA0-7F75BE64C3EF}"/>
-    <hyperlink ref="D179" r:id="rId514" xr:uid="{1AB16091-69AE-4105-9BA6-B775B46361F8}"/>
-    <hyperlink ref="E179" r:id="rId515" xr:uid="{2B7A126E-8D1B-4E8F-93A6-C98453F4B0CD}"/>
-    <hyperlink ref="C180" r:id="rId516" xr:uid="{FF9DC8D1-E300-4D00-8478-B4C4465463B0}"/>
-    <hyperlink ref="D180" r:id="rId517" xr:uid="{C7FB4928-100E-4F31-AA8B-9BB5386BD6E2}"/>
-    <hyperlink ref="E180" r:id="rId518" xr:uid="{33E88EF2-069C-4A8A-A4B9-407D561D9FA7}"/>
-    <hyperlink ref="C181" r:id="rId519" xr:uid="{AD27F6F9-722F-4772-BAD3-292259E599AE}"/>
-    <hyperlink ref="D181" r:id="rId520" xr:uid="{9855AD87-CCE8-4B4A-9D90-654E9CB9A884}"/>
-    <hyperlink ref="E181" r:id="rId521" xr:uid="{DABA9FDA-64E2-49EB-A86C-6A285B8ED457}"/>
-    <hyperlink ref="C182" r:id="rId522" xr:uid="{08DC194C-ADC7-4BD9-B1FA-D02B1EB30413}"/>
-    <hyperlink ref="D182" r:id="rId523" xr:uid="{BDCC0E77-3EA0-4F00-B40F-EB3744C4B10A}"/>
-    <hyperlink ref="E182" r:id="rId524" xr:uid="{0C11EA0B-B2D0-438E-81C0-C400F6D0799A}"/>
-    <hyperlink ref="C183" r:id="rId525" xr:uid="{13991465-B6B8-432B-B460-78ABB1DED868}"/>
-    <hyperlink ref="D183" r:id="rId526" xr:uid="{A036A9F5-033D-4A23-B1E3-B321FB1A1D5C}"/>
-    <hyperlink ref="E183" r:id="rId527" xr:uid="{D1FD862C-B5D6-4B13-931B-57B7FFF1059A}"/>
-    <hyperlink ref="C184" r:id="rId528" xr:uid="{5217B7E5-50F7-4581-9109-F6A8BC875186}"/>
-    <hyperlink ref="D184" r:id="rId529" xr:uid="{C3F790CF-A478-40B7-99F6-7D2667CBC146}"/>
-    <hyperlink ref="E184" r:id="rId530" xr:uid="{A5F80E79-506C-4A15-AACD-68F53D61E373}"/>
-    <hyperlink ref="C185" r:id="rId531" xr:uid="{62E029C0-61D3-4187-A49A-6F8E847B07E9}"/>
-    <hyperlink ref="D185" r:id="rId532" xr:uid="{682FAA6B-7ADD-4D0B-9D48-124102D3B8C4}"/>
-    <hyperlink ref="E185" r:id="rId533" xr:uid="{CB64775F-93CB-4F3C-A7B2-61AA1EEC9FF4}"/>
-    <hyperlink ref="D186" r:id="rId534" xr:uid="{33DB2910-4B9B-4EBD-94DB-9D1D8BA1A60A}"/>
-    <hyperlink ref="E186" r:id="rId535" xr:uid="{D816F0E8-5CA4-4FBA-A574-65EB5C502159}"/>
-    <hyperlink ref="C186" r:id="rId536" xr:uid="{7BED455F-4DC7-4B45-AD26-E1286840DEBE}"/>
-    <hyperlink ref="C187" r:id="rId537" xr:uid="{B17E7A06-B7A3-43DE-959C-80217F4C7404}"/>
-    <hyperlink ref="D187" r:id="rId538" xr:uid="{108A2D11-51B8-4F46-B0AE-357FA3F6BDB6}"/>
-    <hyperlink ref="E187" r:id="rId539" xr:uid="{16666982-1A83-4A62-BFC7-C4F40E6C916E}"/>
-    <hyperlink ref="C188" r:id="rId540" xr:uid="{053DBA08-46A7-4A97-9457-F0E304824F8E}"/>
-    <hyperlink ref="D188" r:id="rId541" xr:uid="{DB4ECA15-195B-4A54-858F-239BA708B125}"/>
-    <hyperlink ref="E188" r:id="rId542" xr:uid="{17CC691E-0C7E-443C-B3E1-54C8BFC12D95}"/>
-    <hyperlink ref="C189" r:id="rId543" xr:uid="{488BAF16-AD49-4FAE-8E4C-CE7962082CBA}"/>
-    <hyperlink ref="D189" r:id="rId544" xr:uid="{0B038405-DDEA-461D-994B-7F271E9120F4}"/>
-    <hyperlink ref="E189" r:id="rId545" xr:uid="{7BACCCB4-5CF4-4224-9201-E647233DE274}"/>
-    <hyperlink ref="C190" r:id="rId546" xr:uid="{E9108E47-563C-4F4D-8B1F-CB863619C501}"/>
-    <hyperlink ref="D190" r:id="rId547" xr:uid="{ECB18330-35A1-421E-8B98-A38AB1F12F4B}"/>
-    <hyperlink ref="E190" r:id="rId548" xr:uid="{594B3616-5B4C-4902-90E8-B56CF4ADD901}"/>
-    <hyperlink ref="C191" r:id="rId549" xr:uid="{BEC6DA00-205E-4FA8-BF78-644278A12620}"/>
-    <hyperlink ref="D191" r:id="rId550" xr:uid="{66E4959D-D2E5-40E0-9A50-3E9722C83879}"/>
-    <hyperlink ref="E191" r:id="rId551" xr:uid="{165E3072-0F8C-4D07-A8EE-AFB2E92D10D0}"/>
-    <hyperlink ref="C192" r:id="rId552" xr:uid="{8BDFFA66-526B-49E6-A9EF-74BACEF2FC3A}"/>
-    <hyperlink ref="D192" r:id="rId553" xr:uid="{23452AE3-198E-4555-8556-92D1EB9C8F2F}"/>
-    <hyperlink ref="E192" r:id="rId554" xr:uid="{1C8BB96E-E2D2-41A2-B51E-CA1C94882C45}"/>
-    <hyperlink ref="C193" r:id="rId555" xr:uid="{78499224-1133-4CA4-8141-97A18D48B873}"/>
-    <hyperlink ref="D193" r:id="rId556" xr:uid="{B9B02DD2-D017-4DBC-9327-5DF3E8B353CB}"/>
-    <hyperlink ref="E193" r:id="rId557" xr:uid="{4CDCE363-4F15-4C8E-88A0-16B4ACE31706}"/>
-    <hyperlink ref="D194" r:id="rId558" xr:uid="{9672DF3D-1B42-4B06-BE7E-8C371290DDD8}"/>
-    <hyperlink ref="E194" r:id="rId559" xr:uid="{A6A6609E-1ACE-4AE1-8630-67EC2A09BB1B}"/>
-    <hyperlink ref="C194" r:id="rId560" xr:uid="{2945D925-89ED-4A50-9C8A-33FAE3D9B663}"/>
-    <hyperlink ref="C195" r:id="rId561" xr:uid="{B2232121-8FC5-4AFB-B4A5-EAFCA6F8BF55}"/>
-    <hyperlink ref="D195" r:id="rId562" xr:uid="{BDB9895C-3A01-437E-B535-262F78163F79}"/>
-    <hyperlink ref="E195" r:id="rId563" xr:uid="{7E8CB580-3C77-4108-A7BB-241E5DD2F8F8}"/>
-    <hyperlink ref="C196" r:id="rId564" xr:uid="{0E762398-C5ED-49DE-9BD7-D01671B4E18A}"/>
-    <hyperlink ref="D196" r:id="rId565" xr:uid="{7FC49659-FA8F-434A-B4B6-95508B1B4D35}"/>
-    <hyperlink ref="E196" r:id="rId566" xr:uid="{5FD4642D-66C0-4BCC-9C59-E55B95CFBFBB}"/>
-    <hyperlink ref="C197" r:id="rId567" xr:uid="{63BBE702-55C8-4458-8A67-C5591C5F9247}"/>
-    <hyperlink ref="D197" r:id="rId568" xr:uid="{A666B7EF-0CBD-4183-BF04-FD5B6DDCF6FD}"/>
-    <hyperlink ref="D99" r:id="rId569" xr:uid="{BB5402C0-11CF-4FB7-9D11-E4E06DA8E09D}"/>
-    <hyperlink ref="C99" r:id="rId570" xr:uid="{5098A259-C902-4545-A7E1-E636AB33D5F8}"/>
-    <hyperlink ref="D86" r:id="rId571" display="https://www.camara.leg.br/internet/sitaqweb/TextoHTML.asp?etapa=11&amp;tpReuniaoEvento=AP%20c/%20Convidado&amp;dtReuniao=15/08/2017&amp;hrInicio=14:50:00&amp;hrFim=17:12:00&amp;origemDiscurso=&amp;nmLocal=Plen%C3%A1rio%20Principal%20-%20CD&amp;nuSessao=1047/17&amp;nuQuarto=0&amp;nuOrador=0&amp;nuInsercao=0&amp;dtHorarioQuarto=14:50&amp;sgFaseSessao=&amp;Data=15/08/2017&amp;txApelido=&amp;txFaseSessao=&amp;txTipoSessao=Permanente&amp;dtHoraQuarto=14:50&amp;txEtapa=" xr:uid="{885EDDC5-59F7-4E1C-AF16-381A4A38D774}"/>
-    <hyperlink ref="C86" r:id="rId572" xr:uid="{4A17DC70-EC44-4004-B071-6F5D899C8CA5}"/>
-    <hyperlink ref="D71" r:id="rId573" xr:uid="{D677B959-EB3C-4DDB-8AEF-E8EAE6D6D45E}"/>
-    <hyperlink ref="C71" r:id="rId574" xr:uid="{0AD8437A-2704-40CD-866A-26901C1B53CE}"/>
-    <hyperlink ref="D63" r:id="rId575" xr:uid="{5F59921F-E727-4A1F-AE6F-37476A2F81C2}"/>
-    <hyperlink ref="C63" r:id="rId576" xr:uid="{4B817215-AB66-422A-B2EE-745DCCE2715E}"/>
-    <hyperlink ref="C62" r:id="rId577" xr:uid="{2DA64800-7A72-4482-919D-DFF1D13D4B55}"/>
-    <hyperlink ref="D62" r:id="rId578" xr:uid="{E8EC2437-F030-4E8C-B6AC-917AA71D6D2D}"/>
-    <hyperlink ref="D40" r:id="rId579" xr:uid="{6C41F5BF-C09E-47D4-A816-D0E540BD6149}"/>
-    <hyperlink ref="C40" r:id="rId580" xr:uid="{CBA2CB5F-E42B-4632-83EE-22826ADE1E04}"/>
-    <hyperlink ref="E197" r:id="rId581" xr:uid="{136FF705-8DCE-4116-BE70-5F1542A088B0}"/>
-    <hyperlink ref="C198" r:id="rId582" xr:uid="{3FB904D1-0936-422F-96AB-F3B96921D779}"/>
-    <hyperlink ref="D198" r:id="rId583" xr:uid="{7A54B018-01DB-4819-9FD1-68863145C0A1}"/>
-    <hyperlink ref="E198" r:id="rId584" xr:uid="{E3C9E074-5A18-4A4E-8CA3-EEB4F330DFC6}"/>
-    <hyperlink ref="C199" r:id="rId585" xr:uid="{E2D42ECE-DCF2-4092-B7EF-C717EECA06D7}"/>
-    <hyperlink ref="D199" r:id="rId586" xr:uid="{D3B0D91F-A5F5-489B-B4BF-5B6ADA49D078}"/>
-    <hyperlink ref="E199" r:id="rId587" xr:uid="{9E3CF267-2270-4A5E-BF99-A49458146C5C}"/>
-    <hyperlink ref="C200" r:id="rId588" xr:uid="{39D382AA-57C1-42F8-ABF7-11A7F0B35567}"/>
-    <hyperlink ref="D200" r:id="rId589" xr:uid="{8CE8A2BD-98A2-45D9-B373-7C90E69ADB93}"/>
-    <hyperlink ref="E200" r:id="rId590" xr:uid="{DE229DE6-DE64-42DD-97A1-D38A12923FD3}"/>
-    <hyperlink ref="C201" r:id="rId591" xr:uid="{189D0765-1C92-4FC1-A376-28B52EA2BFAF}"/>
-    <hyperlink ref="D201" r:id="rId592" xr:uid="{2532C84C-8DB5-4D9F-8FFB-F09727EC3D64}"/>
-    <hyperlink ref="E201" r:id="rId593" xr:uid="{A9C00FED-2E5B-4151-A8D6-2CBF429036A5}"/>
-    <hyperlink ref="C202" r:id="rId594" xr:uid="{0FB758F3-8CEC-44F8-AB0B-FB5749251F72}"/>
-    <hyperlink ref="D202" r:id="rId595" xr:uid="{14790960-D653-4274-8C1A-87D26826D0D0}"/>
-    <hyperlink ref="E202" r:id="rId596" xr:uid="{669AE71B-0710-4E47-9B20-28C6E0D2A24C}"/>
-    <hyperlink ref="C203" r:id="rId597" xr:uid="{6C1C977A-8104-4C5D-BED7-C833FD88FC10}"/>
-    <hyperlink ref="D203" r:id="rId598" xr:uid="{FA52D527-723E-449E-AE77-53A711E8B5F4}"/>
-    <hyperlink ref="E203" r:id="rId599" xr:uid="{7D40609C-37B6-4DA5-86FD-A779CCE9CF33}"/>
-    <hyperlink ref="D204" r:id="rId600" xr:uid="{E1F2A5BF-32A9-48D5-81EE-19ABF3643DD2}"/>
-    <hyperlink ref="E204" r:id="rId601" xr:uid="{E561AB7E-F883-4B46-9BD4-A1A7658BB442}"/>
-    <hyperlink ref="C204" r:id="rId602" xr:uid="{0B823933-67DE-41F8-B9F5-D78FB031387C}"/>
-    <hyperlink ref="C205" r:id="rId603" xr:uid="{26F9A583-2496-4B17-A929-300CBDA2E24D}"/>
-    <hyperlink ref="D205" r:id="rId604" xr:uid="{6719EDC2-583C-49D3-9ECA-9AAEAB5A1AF8}"/>
-    <hyperlink ref="E205" r:id="rId605" xr:uid="{3243DF7A-EE24-42C4-9051-EF34793BE812}"/>
-    <hyperlink ref="C206" r:id="rId606" xr:uid="{4C45050E-CAB2-4E91-876A-26ACF94DB8B2}"/>
-    <hyperlink ref="D206" r:id="rId607" xr:uid="{4FE2A5B0-C928-4394-8042-D3AA021DA4D8}"/>
-    <hyperlink ref="E206" r:id="rId608" xr:uid="{CAB1117F-895B-408D-BFB0-CC8642447B67}"/>
-    <hyperlink ref="C207" r:id="rId609" xr:uid="{3497FE2B-F080-4F0F-9454-A2F8E2BCEA79}"/>
-    <hyperlink ref="D207" r:id="rId610" xr:uid="{C1B80CC4-8153-4B20-A3F2-B283168811C5}"/>
-    <hyperlink ref="E207" r:id="rId611" xr:uid="{BF0434BE-354E-4789-9E21-F298661908C9}"/>
-    <hyperlink ref="C208" r:id="rId612" xr:uid="{E432FEE7-0CE3-4671-A6DE-A89067FE71F8}"/>
-    <hyperlink ref="D208" r:id="rId613" xr:uid="{9B118C1B-E5E7-4F47-BFA5-206491EA6ED8}"/>
-    <hyperlink ref="E208" r:id="rId614" xr:uid="{9EA9596A-CB3D-4B30-8E07-CA8A3FF7C508}"/>
-    <hyperlink ref="C209" r:id="rId615" xr:uid="{46C6222B-B670-40C3-A605-FABE1731989A}"/>
-    <hyperlink ref="D209" r:id="rId616" xr:uid="{C653707F-D543-43CC-A01D-24A54A6A319B}"/>
-    <hyperlink ref="E209" r:id="rId617" xr:uid="{60116EA4-2834-4C7A-B4DB-1CE223CB90BB}"/>
-    <hyperlink ref="C210" r:id="rId618" xr:uid="{20EC698E-A69F-497B-8D14-1C5CA444BC21}"/>
-    <hyperlink ref="D210" r:id="rId619" xr:uid="{AFAB7C9A-C544-47BD-8645-5C31CE7C5CF3}"/>
-    <hyperlink ref="E210" r:id="rId620" xr:uid="{F53AF2AB-0CE9-45A6-B905-24C7FEEA3E52}"/>
-    <hyperlink ref="C211" r:id="rId621" xr:uid="{30CD9287-A385-456E-9D5E-59944E3156E1}"/>
-    <hyperlink ref="D211" r:id="rId622" xr:uid="{C9FDF5BB-9B0E-442F-AE18-EBCAF9FA12BA}"/>
-    <hyperlink ref="E211" r:id="rId623" xr:uid="{E3661C98-D989-4879-A8FC-B6166662C8D7}"/>
-    <hyperlink ref="C212" r:id="rId624" xr:uid="{2102EDB4-6981-4633-9FD3-E647448181FC}"/>
-    <hyperlink ref="D212" r:id="rId625" xr:uid="{0DB9D726-23FB-4B78-94AC-DFD7B21AB5AE}"/>
-    <hyperlink ref="E212" r:id="rId626" xr:uid="{BF7B36EC-2642-4F9B-A942-FC7DA39117FB}"/>
+    <hyperlink ref="C56" r:id="rId156" xr:uid="{93A3A603-A9B2-4D19-812A-74A36F16D1BC}"/>
+    <hyperlink ref="D56" r:id="rId157" xr:uid="{F3F43F43-E791-4A68-9487-58DD42F5F7B7}"/>
+    <hyperlink ref="E56" r:id="rId158" xr:uid="{E53FDCD2-A870-487C-83BB-B2F9355F084C}"/>
+    <hyperlink ref="E57" r:id="rId159" xr:uid="{95776386-802C-4E31-AB88-27B8CDF0F98E}"/>
+    <hyperlink ref="D57" r:id="rId160" xr:uid="{273B5CFE-28E9-4D37-8E20-9EEEFD512062}"/>
+    <hyperlink ref="C57" r:id="rId161" xr:uid="{CB726674-3850-4498-868B-9706F994615D}"/>
+    <hyperlink ref="C58" r:id="rId162" xr:uid="{B663A24C-0B6C-401D-AC91-CEDD5CC4C7B7}"/>
+    <hyperlink ref="D58" r:id="rId163" xr:uid="{2E990E0F-4E98-4C50-9D71-1E1591F61C5C}"/>
+    <hyperlink ref="E58" r:id="rId164" xr:uid="{A890A3C2-DD7A-4D54-AAD4-DE19A02AB080}"/>
+    <hyperlink ref="D59" r:id="rId165" xr:uid="{6B6FDF6B-3060-4EA4-A538-A32130409E58}"/>
+    <hyperlink ref="E59" r:id="rId166" xr:uid="{0B4BA579-1251-419C-83B7-16A2DE374221}"/>
+    <hyperlink ref="C59" r:id="rId167" xr:uid="{9FE2E172-5C41-4230-84CF-F6E914414453}"/>
+    <hyperlink ref="C60" r:id="rId168" xr:uid="{A3A1E70E-3606-43AB-959D-42D475EC026C}"/>
+    <hyperlink ref="D60" r:id="rId169" xr:uid="{05D726A8-B397-4927-9858-8A6F1E8C2C34}"/>
+    <hyperlink ref="E60" r:id="rId170" xr:uid="{E3E92A65-878C-4396-A979-259192CFE3FB}"/>
+    <hyperlink ref="C61" r:id="rId171" xr:uid="{9CDDC3F7-461B-41F6-A604-8C9AAF323690}"/>
+    <hyperlink ref="D61" r:id="rId172" xr:uid="{F9BD9FD8-27F4-433F-85B6-5B88A8B0B2EA}"/>
+    <hyperlink ref="E61" r:id="rId173" xr:uid="{036D4EDF-20C3-46C1-B910-16EFF6E50BBF}"/>
+    <hyperlink ref="C64" r:id="rId174" xr:uid="{2E1566B2-0D33-4DAB-8479-3FEEB5CD0159}"/>
+    <hyperlink ref="D64" r:id="rId175" xr:uid="{117EEFAC-1BA9-40E7-BF81-427F4E2C074D}"/>
+    <hyperlink ref="E64" r:id="rId176" xr:uid="{352858DF-5707-44F4-A4DD-C9D46E1C9188}"/>
+    <hyperlink ref="C65" r:id="rId177" xr:uid="{F83364B1-EDCD-40AE-B3E5-ADB81A08EB7C}"/>
+    <hyperlink ref="D65" r:id="rId178" xr:uid="{C78C668C-C893-42CE-89BA-9C9DC1B04B03}"/>
+    <hyperlink ref="E65" r:id="rId179" xr:uid="{E8577748-C8CE-4E73-BB98-1BB03AD9686A}"/>
+    <hyperlink ref="C66" r:id="rId180" xr:uid="{A58DB200-4FFE-4BF3-B93F-D7D768D15010}"/>
+    <hyperlink ref="D66" r:id="rId181" xr:uid="{63426EA7-EE17-4830-AD2C-B92AB219EFC9}"/>
+    <hyperlink ref="E66" r:id="rId182" xr:uid="{A528D6F6-6F96-4FDE-969E-517AEE4FDE49}"/>
+    <hyperlink ref="C67" r:id="rId183" xr:uid="{80D9D7A9-DD44-4211-9955-F61D7176460D}"/>
+    <hyperlink ref="D67" r:id="rId184" xr:uid="{D4A9E17D-57B2-46AE-8198-9B6AE21635E2}"/>
+    <hyperlink ref="E67" r:id="rId185" xr:uid="{714D4749-2A7B-491D-9FB8-1BF21E9A93A1}"/>
+    <hyperlink ref="C68" r:id="rId186" xr:uid="{B4C331B2-82CE-4B4E-94B3-88D151FEA07C}"/>
+    <hyperlink ref="D68" r:id="rId187" xr:uid="{C1C28575-633C-4333-AE20-6E34F0D2C138}"/>
+    <hyperlink ref="E68" r:id="rId188" xr:uid="{FE501029-2FFD-40EF-A6D2-E4F0980CB07B}"/>
+    <hyperlink ref="D69" r:id="rId189" xr:uid="{4E5BE45A-EE70-4A55-8813-6234D4AC22C3}"/>
+    <hyperlink ref="E69" r:id="rId190" xr:uid="{B6845F8F-30C8-434A-9566-8828D3FACB44}"/>
+    <hyperlink ref="C69" r:id="rId191" xr:uid="{42EC5C33-69F0-46DF-855B-9082D27FA37E}"/>
+    <hyperlink ref="C70" r:id="rId192" xr:uid="{B9C25BBF-2F1C-43AB-81D9-BA7D962E4B80}"/>
+    <hyperlink ref="D70" r:id="rId193" xr:uid="{7FAC267F-3E9F-431E-A5F7-E593B7A351C3}"/>
+    <hyperlink ref="E70" r:id="rId194" xr:uid="{931EEA1E-08EA-45E0-9646-E9D6D48A4F19}"/>
+    <hyperlink ref="C72" r:id="rId195" xr:uid="{2B570C9B-5283-429F-A6C6-071211DDB4CD}"/>
+    <hyperlink ref="D72" r:id="rId196" xr:uid="{DE416E21-0088-4A69-BD6D-D1C470435319}"/>
+    <hyperlink ref="E72" r:id="rId197" xr:uid="{D8837C3B-A0F9-4ED9-AA44-C440FB07A20C}"/>
+    <hyperlink ref="C73" r:id="rId198" xr:uid="{D6BD5389-04F2-4B58-9F33-AAA93C71092F}"/>
+    <hyperlink ref="D73" r:id="rId199" xr:uid="{7C93FBAB-8242-4810-A221-B083FC1513C1}"/>
+    <hyperlink ref="E73" r:id="rId200" xr:uid="{F0338AD3-0E74-4F5E-8444-AB3C55B8A664}"/>
+    <hyperlink ref="D74" r:id="rId201" xr:uid="{594C1034-31CE-4449-83AE-862B6480A46D}"/>
+    <hyperlink ref="E74" r:id="rId202" xr:uid="{30DAC341-1E00-4295-9B09-88B418393100}"/>
+    <hyperlink ref="C74" r:id="rId203" xr:uid="{4E97E308-91E7-4668-9B7F-2338C5857A08}"/>
+    <hyperlink ref="C75" r:id="rId204" xr:uid="{066BA063-0C85-4162-B074-0AAED730B020}"/>
+    <hyperlink ref="D75" r:id="rId205" xr:uid="{22128F9A-D8EF-4482-873E-5AB7553BCF20}"/>
+    <hyperlink ref="E75" r:id="rId206" xr:uid="{730102A0-62A5-4CA6-9C35-CB7BE66653A7}"/>
+    <hyperlink ref="D76" r:id="rId207" xr:uid="{92DE723E-DC1E-4E35-9F8A-DFC81658094A}"/>
+    <hyperlink ref="E76" r:id="rId208" xr:uid="{88C9AD40-1118-49F6-A915-7EAC16F870A2}"/>
+    <hyperlink ref="C76" r:id="rId209" xr:uid="{0DBA37A8-7096-4807-AC1B-4BEEFD66EA84}"/>
+    <hyperlink ref="C77" r:id="rId210" xr:uid="{83838767-AE02-4E24-9364-758023852C1B}"/>
+    <hyperlink ref="D77" r:id="rId211" xr:uid="{3C1F43CF-1207-4D08-A29C-EF841A48722C}"/>
+    <hyperlink ref="E77" r:id="rId212" xr:uid="{9D1B210A-0896-4875-B2FE-48517A0CA7F8}"/>
+    <hyperlink ref="D78" r:id="rId213" xr:uid="{A272A680-03CE-4750-A5EA-13B9BAD1DDA3}"/>
+    <hyperlink ref="E78" r:id="rId214" xr:uid="{F984F963-EDFC-4A31-BC8C-DE2561D61832}"/>
+    <hyperlink ref="C78" r:id="rId215" xr:uid="{68F9921C-BE67-40B9-8D57-068F721C5F32}"/>
+    <hyperlink ref="D79" r:id="rId216" xr:uid="{48B07033-F32B-4E27-9F43-BBA692FC8D29}"/>
+    <hyperlink ref="E79" r:id="rId217" xr:uid="{69916E72-32B0-4D28-9637-0EEFFADF74E8}"/>
+    <hyperlink ref="C79" r:id="rId218" xr:uid="{C8B9A133-0888-4E11-A670-EFF7CAC4ABFE}"/>
+    <hyperlink ref="D80" r:id="rId219" xr:uid="{0E15DC38-6EC8-4D48-8A86-F4AEB986ECDF}"/>
+    <hyperlink ref="E80" r:id="rId220" xr:uid="{36C1DDB0-E1FC-4E5D-949E-8F56A1E2E8FF}"/>
+    <hyperlink ref="C80" r:id="rId221" xr:uid="{B925BBDF-760B-4CD2-A22B-DB576A318F97}"/>
+    <hyperlink ref="D81" r:id="rId222" xr:uid="{5E1CFEEC-121E-4A0C-8D6E-1BE66A180602}"/>
+    <hyperlink ref="E81" r:id="rId223" xr:uid="{766EF454-F43A-4F23-8B1F-175DFBFA66C4}"/>
+    <hyperlink ref="C81" r:id="rId224" xr:uid="{F85622CB-5CD0-48DC-A9C2-D3B6BED83625}"/>
+    <hyperlink ref="D82" r:id="rId225" xr:uid="{022B4862-9904-438C-888E-088EFA87DF90}"/>
+    <hyperlink ref="E82" r:id="rId226" xr:uid="{DB096912-4591-4CA7-89B5-81A0A35646CE}"/>
+    <hyperlink ref="C82" r:id="rId227" xr:uid="{1DDD2058-A4A9-44F5-BA2A-2FC1A103A9F9}"/>
+    <hyperlink ref="C83" r:id="rId228" xr:uid="{3B08A944-BE8A-4F11-A43D-772558AE96DD}"/>
+    <hyperlink ref="D83" r:id="rId229" xr:uid="{27AB88EB-9DAF-4FA2-AA3A-E724287C8F93}"/>
+    <hyperlink ref="E83" r:id="rId230" xr:uid="{5BE5BE86-194D-42C1-86C0-0EB255719069}"/>
+    <hyperlink ref="D84" r:id="rId231" xr:uid="{70156D30-FCC6-4159-9748-163AA7650BFF}"/>
+    <hyperlink ref="E84" r:id="rId232" xr:uid="{AB61F21B-2647-4188-86EB-7A9EF52EAD4E}"/>
+    <hyperlink ref="C84" r:id="rId233" xr:uid="{AB845C66-110A-4E17-BA35-49424C8D9DB8}"/>
+    <hyperlink ref="C85" r:id="rId234" xr:uid="{4BEB7309-0983-4E2A-8044-81A5248547AD}"/>
+    <hyperlink ref="D85" r:id="rId235" xr:uid="{B47FB409-ABDE-45DB-91C0-653606E6F1FE}"/>
+    <hyperlink ref="E85" r:id="rId236" xr:uid="{9C948BFA-EE5F-4B1A-89B4-BF6DD4933F34}"/>
+    <hyperlink ref="D87" r:id="rId237" xr:uid="{A671B004-D342-45B8-BAA5-3E49FE2DE8BD}"/>
+    <hyperlink ref="E87" r:id="rId238" xr:uid="{C4019578-43D7-4898-AFB3-EAF1FF26E40C}"/>
+    <hyperlink ref="C87" r:id="rId239" xr:uid="{44B49121-69C0-4CB8-99B4-1D3604703C20}"/>
+    <hyperlink ref="D88" r:id="rId240" xr:uid="{9FB0C34A-F587-4BAE-9F2E-6FB5C63D9D1F}"/>
+    <hyperlink ref="E88" r:id="rId241" xr:uid="{F4E6ACF3-DFAA-477B-BE00-0211EEF43CD5}"/>
+    <hyperlink ref="C88" r:id="rId242" xr:uid="{77539DF1-1D8C-420E-8D0F-988850275481}"/>
+    <hyperlink ref="D89" r:id="rId243" xr:uid="{CB844098-58B7-4F8E-9B26-9BF7BCA817A0}"/>
+    <hyperlink ref="E89" r:id="rId244" xr:uid="{27CA033B-C8BD-4632-8C3B-BF86115051BF}"/>
+    <hyperlink ref="C89" r:id="rId245" xr:uid="{90338A87-20AE-4C6E-98E9-85613D1C7589}"/>
+    <hyperlink ref="D90" r:id="rId246" xr:uid="{A2814B89-6B87-4365-9C51-229D20F3F148}"/>
+    <hyperlink ref="E90" r:id="rId247" xr:uid="{880F7943-3A52-496B-A7C1-7EF72DDC2689}"/>
+    <hyperlink ref="C90" r:id="rId248" xr:uid="{0D7A2F28-4643-47C9-B897-7323740734E4}"/>
+    <hyperlink ref="C91" r:id="rId249" xr:uid="{6FAD943F-0A69-4BAF-AB56-35651FB59547}"/>
+    <hyperlink ref="D91" r:id="rId250" xr:uid="{1DE20C76-625A-4F4C-8C81-8D9C072645AF}"/>
+    <hyperlink ref="E91" r:id="rId251" xr:uid="{DB534690-3B61-4958-B81D-B687C80AA2E6}"/>
+    <hyperlink ref="C92" r:id="rId252" xr:uid="{F8F36C90-CCC9-4055-8BFD-CA71908A98D0}"/>
+    <hyperlink ref="D92" r:id="rId253" xr:uid="{7257BD60-D08C-4CBB-B7E5-8086A9C62A70}"/>
+    <hyperlink ref="E92" r:id="rId254" xr:uid="{57CB7722-444C-4E22-B23F-13AC9D1792A5}"/>
+    <hyperlink ref="C93" r:id="rId255" xr:uid="{7D8FD390-7977-4F5A-A4AE-D8AFF1779260}"/>
+    <hyperlink ref="D93" r:id="rId256" xr:uid="{C1952C13-045C-461F-8BC0-C9C86F08CAAE}"/>
+    <hyperlink ref="E93" r:id="rId257" xr:uid="{6593CB6B-985B-4C06-8E0B-4DD2A95CFB8C}"/>
+    <hyperlink ref="E94" r:id="rId258" xr:uid="{2033DE9C-AB68-4337-9666-E036632B48E9}"/>
+    <hyperlink ref="D94" r:id="rId259" xr:uid="{BC335142-CEB5-45DC-A6D5-CB1E1226051F}"/>
+    <hyperlink ref="C94" r:id="rId260" xr:uid="{373F113B-04B2-431D-8E11-05B90B52D390}"/>
+    <hyperlink ref="C95" r:id="rId261" xr:uid="{E3539E81-DF93-4A39-9945-36CEC9E34CF4}"/>
+    <hyperlink ref="D95" r:id="rId262" xr:uid="{D669F179-1AC6-4E08-96C5-C7BE89D41875}"/>
+    <hyperlink ref="E95" r:id="rId263" xr:uid="{CBC521FB-9833-4D60-918B-F3038613EC49}"/>
+    <hyperlink ref="D96" r:id="rId264" xr:uid="{1487A3FD-94F4-4C63-B36B-1C6236ACCCAA}"/>
+    <hyperlink ref="E96" r:id="rId265" xr:uid="{5F631273-96B3-48BB-A5C6-A8077E8EC752}"/>
+    <hyperlink ref="C96" r:id="rId266" xr:uid="{ADE8BEEA-ABC6-474A-A950-FF38898D34D2}"/>
+    <hyperlink ref="D97" r:id="rId267" xr:uid="{4DD3F6B0-4B1E-451C-9857-7B840584705D}"/>
+    <hyperlink ref="E97" r:id="rId268" xr:uid="{6DA9CE9D-442F-4DC5-BE8C-7745B1745575}"/>
+    <hyperlink ref="C97" r:id="rId269" xr:uid="{E59BA18D-2DA1-4FDF-9C1E-CD6D1A2620C7}"/>
+    <hyperlink ref="D98" r:id="rId270" xr:uid="{5C95BE55-05A0-4BE2-A224-2C4A40579DEE}"/>
+    <hyperlink ref="E98" r:id="rId271" xr:uid="{E2F28665-F304-48EB-AEE8-E289F7A4FC5A}"/>
+    <hyperlink ref="C98" r:id="rId272" xr:uid="{55201C98-C656-4EE7-A35F-CE17F44473C3}"/>
+    <hyperlink ref="C100" r:id="rId273" xr:uid="{79EA69E5-FEAB-4C20-B0DE-70A81655B6D4}"/>
+    <hyperlink ref="D100" r:id="rId274" xr:uid="{ED375E0D-1308-4908-9149-A0315A582320}"/>
+    <hyperlink ref="E100" r:id="rId275" xr:uid="{D46B35C8-21A4-4B52-ABFA-8A94A326F9D7}"/>
+    <hyperlink ref="C101" r:id="rId276" xr:uid="{E7ACECEC-3A28-4599-84B8-59BC02BF4FED}"/>
+    <hyperlink ref="D101" r:id="rId277" xr:uid="{465047FF-1256-4E45-AE8D-E5CEDB95F73F}"/>
+    <hyperlink ref="E101" r:id="rId278" xr:uid="{F30A2FC8-5BF5-487F-A934-EC4AC77FE211}"/>
+    <hyperlink ref="C102" r:id="rId279" xr:uid="{178FA5E3-E6A3-4365-9928-DC4296B031B7}"/>
+    <hyperlink ref="D102" r:id="rId280" xr:uid="{2487C55D-36B0-497C-8E7F-76864E5D2337}"/>
+    <hyperlink ref="E102" r:id="rId281" xr:uid="{9ABF0A5D-385F-4E38-95DF-7739D7794FCD}"/>
+    <hyperlink ref="C103" r:id="rId282" xr:uid="{5D123A8D-D901-4600-9E13-23B4081222A0}"/>
+    <hyperlink ref="D103" r:id="rId283" xr:uid="{B41BE957-8100-409E-8F6C-9FFF07208823}"/>
+    <hyperlink ref="E103" r:id="rId284" xr:uid="{7417B276-5872-4090-A0D9-C56E6230AB29}"/>
+    <hyperlink ref="C104" r:id="rId285" xr:uid="{2AC02C2A-F7B1-4CDE-8106-C0D377FFD10A}"/>
+    <hyperlink ref="D104" r:id="rId286" xr:uid="{CF5FB671-CD80-457E-9A5C-55AC19128002}"/>
+    <hyperlink ref="E104" r:id="rId287" xr:uid="{7EB7712F-F3D4-4CD0-928D-AA08612DA711}"/>
+    <hyperlink ref="C105" r:id="rId288" xr:uid="{3A98A613-5247-4EDD-9ED8-FFB31D28F72C}"/>
+    <hyperlink ref="D105" r:id="rId289" xr:uid="{B0F0B342-1498-46A9-BD50-0660E9657C90}"/>
+    <hyperlink ref="E105" r:id="rId290" xr:uid="{0B67D960-696C-427C-A875-D3B85CFF0762}"/>
+    <hyperlink ref="C106" r:id="rId291" xr:uid="{1DA3041A-7728-4026-B61E-A1AB5F15F5A8}"/>
+    <hyperlink ref="D106" r:id="rId292" xr:uid="{451E6F75-0E8E-49A5-8A5B-87255F93DD33}"/>
+    <hyperlink ref="E106" r:id="rId293" xr:uid="{D49DC68C-742B-425B-881B-A83AF4714EE4}"/>
+    <hyperlink ref="C107" r:id="rId294" xr:uid="{D226CEDC-443D-41F7-AD26-0AAF1BD9DB3F}"/>
+    <hyperlink ref="D107" r:id="rId295" xr:uid="{EF0F660D-62B8-4AA4-A272-57AB44F0E9CF}"/>
+    <hyperlink ref="E107" r:id="rId296" xr:uid="{3F4019C0-9C15-4B90-B9D3-90908DBCF849}"/>
+    <hyperlink ref="C108" r:id="rId297" xr:uid="{8B746AED-6ACC-4850-8828-FB6F0374D303}"/>
+    <hyperlink ref="D108" r:id="rId298" xr:uid="{F9014A66-3EE9-40DC-B87E-5D9054B50E5D}"/>
+    <hyperlink ref="E108" r:id="rId299" xr:uid="{4EE6DB51-0C8B-400C-A838-15E4BD633EE2}"/>
+    <hyperlink ref="C109" r:id="rId300" xr:uid="{FA69422B-0C15-4C8B-B074-46A3869AC7C9}"/>
+    <hyperlink ref="D109" r:id="rId301" xr:uid="{621EC68A-7ACE-45FB-88A3-06F720875DD7}"/>
+    <hyperlink ref="E109" r:id="rId302" xr:uid="{554DED57-0D82-433F-987B-1B34E1214C78}"/>
+    <hyperlink ref="C110" r:id="rId303" xr:uid="{4117E483-CA3B-487C-94D0-D68E8DB43993}"/>
+    <hyperlink ref="D110" r:id="rId304" xr:uid="{8AAA2CF2-8CC2-4067-AAC9-FA2A4EFE32DD}"/>
+    <hyperlink ref="E110" r:id="rId305" xr:uid="{66B74877-14BB-4AD3-8761-E581180779E3}"/>
+    <hyperlink ref="C111" r:id="rId306" xr:uid="{C527C048-13AF-4166-AAC3-24C05E9E601E}"/>
+    <hyperlink ref="D111" r:id="rId307" xr:uid="{2965799F-E19D-4831-A7B4-10AC9AAC4229}"/>
+    <hyperlink ref="E111" r:id="rId308" xr:uid="{44E6383F-DB4B-4F5D-BA87-405239E1E5E0}"/>
+    <hyperlink ref="C112" r:id="rId309" xr:uid="{714BC743-EB75-42ED-AF6E-B8B31923740F}"/>
+    <hyperlink ref="D112" r:id="rId310" xr:uid="{C53CEA57-5AB8-4F8D-BE5E-9B4CB9BD9BF5}"/>
+    <hyperlink ref="E112" r:id="rId311" xr:uid="{B6767105-A075-4865-AAC5-BF568E26C3DC}"/>
+    <hyperlink ref="C113" r:id="rId312" xr:uid="{DA3469AE-90EC-41E3-9216-B1C0BDA33A67}"/>
+    <hyperlink ref="D113" r:id="rId313" xr:uid="{557307AD-C5A9-4652-888D-A94FDF80009E}"/>
+    <hyperlink ref="E113" r:id="rId314" xr:uid="{C3DCCA91-9FBC-47D2-A94E-C1B437125A9A}"/>
+    <hyperlink ref="C114" r:id="rId315" xr:uid="{2906FCEE-6A7F-45B3-8BF5-7B231A0D23DB}"/>
+    <hyperlink ref="D114" r:id="rId316" xr:uid="{CBE1D2EA-6123-4939-A2F6-07C30E28EEE0}"/>
+    <hyperlink ref="E114" r:id="rId317" xr:uid="{31DAEDC2-35C0-48F5-A25B-93D7BF3A7450}"/>
+    <hyperlink ref="C115" r:id="rId318" xr:uid="{9E70ABF8-EABB-4B06-80D0-153AB8E19A7B}"/>
+    <hyperlink ref="D115" r:id="rId319" xr:uid="{327C9817-CBEE-4C9A-AAC6-464A863BEF9D}"/>
+    <hyperlink ref="E115" r:id="rId320" xr:uid="{A96FDAEB-0252-432D-A050-64EE5BE04F6D}"/>
+    <hyperlink ref="C116" r:id="rId321" xr:uid="{A4745FA3-0838-4B0A-8AF1-C0E8A9318E7A}"/>
+    <hyperlink ref="D116" r:id="rId322" xr:uid="{D592EA88-2676-4594-A3F8-755BA2197B17}"/>
+    <hyperlink ref="E116" r:id="rId323" xr:uid="{43298315-6704-4543-B6A3-1D12ED3BD89B}"/>
+    <hyperlink ref="C117" r:id="rId324" xr:uid="{4F507A97-E64C-4FA2-827D-A97B68F6502C}"/>
+    <hyperlink ref="D117" r:id="rId325" xr:uid="{89E85572-0309-4ECD-9E6F-6A8BFBDD0475}"/>
+    <hyperlink ref="E117" r:id="rId326" xr:uid="{6C735EE1-5379-4E04-87DC-61981092F13A}"/>
+    <hyperlink ref="C118" r:id="rId327" xr:uid="{DCB2DDD8-CEA1-4A83-927E-AA880D5F2465}"/>
+    <hyperlink ref="D118" r:id="rId328" xr:uid="{87B4582B-3A51-46CB-A7AA-14A53BEF2877}"/>
+    <hyperlink ref="E118" r:id="rId329" xr:uid="{95F3F337-662F-4DEB-899F-8B106C6AD582}"/>
+    <hyperlink ref="D119" r:id="rId330" xr:uid="{C6E03219-8688-46D5-858A-2C3BB7AC04D7}"/>
+    <hyperlink ref="E119" r:id="rId331" xr:uid="{222C944B-0CA2-4AA1-BFF7-664ED828CA3B}"/>
+    <hyperlink ref="C119" r:id="rId332" xr:uid="{50F33598-73F6-4B9D-8478-4AC6890A025A}"/>
+    <hyperlink ref="D120" r:id="rId333" xr:uid="{4AED68E4-2779-4CB0-B7AE-44AFAECA4499}"/>
+    <hyperlink ref="E120" r:id="rId334" xr:uid="{20510976-5BE1-4F80-89F3-DC95303A5BBF}"/>
+    <hyperlink ref="C120" r:id="rId335" xr:uid="{3842BBC2-0FE4-402C-A871-BFB50EE32BA0}"/>
+    <hyperlink ref="C121" r:id="rId336" xr:uid="{89D31CD8-B8E5-49D6-8FA5-D7A42F6CB540}"/>
+    <hyperlink ref="D121" r:id="rId337" xr:uid="{AC74A6C1-41F5-4315-92E2-A3C7ED59EBBD}"/>
+    <hyperlink ref="E121" r:id="rId338" xr:uid="{B1F093AF-7F7F-460F-A4F0-ADB6490D731B}"/>
+    <hyperlink ref="C122" r:id="rId339" xr:uid="{D4F65573-20F5-43D1-80BF-2795F41D9F57}"/>
+    <hyperlink ref="D122" r:id="rId340" xr:uid="{B88C2559-C22D-41ED-8F15-469DB6777B84}"/>
+    <hyperlink ref="E122" r:id="rId341" xr:uid="{EEA137CE-31F7-415B-94AB-CA2A55462E5C}"/>
+    <hyperlink ref="C123" r:id="rId342" xr:uid="{D997E317-1F11-4A83-B7F1-CF5217F8F4ED}"/>
+    <hyperlink ref="D123" r:id="rId343" xr:uid="{C9088CDA-1F58-4681-9DAD-82F7D0583EE5}"/>
+    <hyperlink ref="E123" r:id="rId344" xr:uid="{830325FC-B5CA-4053-8D5D-6DA5A0E9CEB3}"/>
+    <hyperlink ref="C124" r:id="rId345" xr:uid="{5AC4D217-D8FE-4409-862F-FAA5A86520AC}"/>
+    <hyperlink ref="D124" r:id="rId346" xr:uid="{CE468356-AB38-423F-ACE7-04587D99102E}"/>
+    <hyperlink ref="E124" r:id="rId347" xr:uid="{611001F6-2221-481D-AFA1-35DB4D386424}"/>
+    <hyperlink ref="C125" r:id="rId348" xr:uid="{FCC30E1C-7F83-4581-822A-7F2ACF21B208}"/>
+    <hyperlink ref="D125" r:id="rId349" xr:uid="{3A097561-C99B-452A-B5F9-14E12478CA8E}"/>
+    <hyperlink ref="E125" r:id="rId350" xr:uid="{5847BD3E-972F-4164-8556-AAACBBA355DB}"/>
+    <hyperlink ref="C126" r:id="rId351" xr:uid="{3BCC14C6-3272-4FB5-B30F-233B0FFAA229}"/>
+    <hyperlink ref="D126" r:id="rId352" xr:uid="{D87B0C63-927A-423F-9DEE-FB163765706A}"/>
+    <hyperlink ref="E126" r:id="rId353" xr:uid="{8D18C038-05BE-41FB-9589-349C2DB35EB6}"/>
+    <hyperlink ref="C127" r:id="rId354" xr:uid="{212AE7B7-8417-4613-9B01-457D5FAD32E2}"/>
+    <hyperlink ref="D127" r:id="rId355" xr:uid="{16169750-2789-41D4-92EE-8370C62CF1BA}"/>
+    <hyperlink ref="E127" r:id="rId356" xr:uid="{EF236839-B3F1-4D2A-8793-A6E0A9D52328}"/>
+    <hyperlink ref="C128" r:id="rId357" xr:uid="{13F5A019-E7BD-473A-8BFB-051E885B1146}"/>
+    <hyperlink ref="D128" r:id="rId358" xr:uid="{C06C249C-A9D7-4BAE-AD6C-0ECED61AA088}"/>
+    <hyperlink ref="E128" r:id="rId359" xr:uid="{C2493638-1F36-426C-A65E-9BA0E883C835}"/>
+    <hyperlink ref="C129" r:id="rId360" xr:uid="{7F246417-F2E2-4CEF-ACB8-0C0E87FFBD79}"/>
+    <hyperlink ref="D129" r:id="rId361" xr:uid="{77141049-FDE6-4B29-8926-A7256E4C0505}"/>
+    <hyperlink ref="E129" r:id="rId362" xr:uid="{F98DCA20-9796-418E-B8CA-A3E005647A01}"/>
+    <hyperlink ref="C130" r:id="rId363" xr:uid="{0BA229B0-06A2-4C48-9914-A5374B32A34F}"/>
+    <hyperlink ref="D130" r:id="rId364" xr:uid="{3F506EBE-0BD0-4794-87C1-953206B16CD4}"/>
+    <hyperlink ref="E130" r:id="rId365" xr:uid="{A615BCEB-72DE-43C7-8A07-693C54D3A0C4}"/>
+    <hyperlink ref="C131" r:id="rId366" xr:uid="{07FCC78B-BF39-43FB-A89D-700B9FB2D824}"/>
+    <hyperlink ref="D131" r:id="rId367" xr:uid="{12B43D3A-B1AA-41D0-8A47-1DDC5FBC02CC}"/>
+    <hyperlink ref="E131" r:id="rId368" xr:uid="{E1EB98C2-E2CA-4E94-8439-8B789E3754E7}"/>
+    <hyperlink ref="D132" r:id="rId369" xr:uid="{63468E1D-F523-48BF-8225-D649FBE847EC}"/>
+    <hyperlink ref="E132" r:id="rId370" xr:uid="{4D681694-A038-4227-BC2E-F2651367ACF3}"/>
+    <hyperlink ref="C132" r:id="rId371" xr:uid="{D7ECE862-4574-486D-A9A4-78F8E4FC1681}"/>
+    <hyperlink ref="C133" r:id="rId372" xr:uid="{B156B9CD-29C4-4D78-8EBA-515A4C1B6B5A}"/>
+    <hyperlink ref="D133" r:id="rId373" xr:uid="{DA45D1F5-4AD3-4F4C-8A29-855166DF6940}"/>
+    <hyperlink ref="E133" r:id="rId374" xr:uid="{596A4EF2-4527-401B-A2CE-FA6A6AE241FF}"/>
+    <hyperlink ref="C134" r:id="rId375" xr:uid="{DC92B3C9-52B9-4D63-AC4A-1FE80AD38A7B}"/>
+    <hyperlink ref="D134" r:id="rId376" xr:uid="{6653B8D2-7773-4FD1-8AB6-76B074FA4AAA}"/>
+    <hyperlink ref="E134" r:id="rId377" xr:uid="{58D58C73-9A50-44A9-A0EA-5592206BB72F}"/>
+    <hyperlink ref="C135" r:id="rId378" xr:uid="{CF269375-1231-4422-9D05-86CA9413B1AD}"/>
+    <hyperlink ref="D135" r:id="rId379" xr:uid="{7AF85C45-2D0F-4BF2-8039-612435A7F999}"/>
+    <hyperlink ref="E135" r:id="rId380" xr:uid="{B39AC57D-61C7-4384-92C0-FA4D3C141F31}"/>
+    <hyperlink ref="C136" r:id="rId381" xr:uid="{F5D55CD9-3B76-4FD8-AC67-16192C305D26}"/>
+    <hyperlink ref="D136" r:id="rId382" xr:uid="{48D8B605-74CE-472F-AFDD-08EC6689007C}"/>
+    <hyperlink ref="E136" r:id="rId383" xr:uid="{44FF3624-E323-438F-8CAB-68D1CB08688C}"/>
+    <hyperlink ref="C137" r:id="rId384" xr:uid="{CE592AC5-E5D6-495B-BB1B-85E6B7EE95DA}"/>
+    <hyperlink ref="D137" r:id="rId385" xr:uid="{D0AD0ECF-67E1-4B11-91F5-AA23D31475D4}"/>
+    <hyperlink ref="E137" r:id="rId386" xr:uid="{CA7CD45E-3E5B-4C2E-93A9-84848C1A52F2}"/>
+    <hyperlink ref="C138" r:id="rId387" xr:uid="{971AEABA-C26E-4CD2-B617-7E7AEFA79225}"/>
+    <hyperlink ref="D138" r:id="rId388" xr:uid="{E838D43A-FA34-4E17-A12D-60A467F149C2}"/>
+    <hyperlink ref="E138" r:id="rId389" xr:uid="{31F37E78-12DF-444E-A3FB-EF00403D39D4}"/>
+    <hyperlink ref="C139" r:id="rId390" xr:uid="{7DC70FA2-2641-4F66-B9F8-01F68ED70F02}"/>
+    <hyperlink ref="D139" r:id="rId391" xr:uid="{B963012C-FACA-4A11-B1C4-313CF3F6387F}"/>
+    <hyperlink ref="E139" r:id="rId392" xr:uid="{E1DCAB4B-878B-4C50-97B6-B5A5D2A2FADD}"/>
+    <hyperlink ref="C140" r:id="rId393" xr:uid="{60F58296-9148-4312-9D0C-BF4DE0690B91}"/>
+    <hyperlink ref="D140" r:id="rId394" xr:uid="{8DBCCAC8-BC9E-442F-A475-9F8639697DB9}"/>
+    <hyperlink ref="E140" r:id="rId395" xr:uid="{0B4BC81F-7CB5-41BC-88B0-3B2BBBE80A3F}"/>
+    <hyperlink ref="D141" r:id="rId396" xr:uid="{9A0BB159-B669-435C-9CB1-A2BA4C4091A9}"/>
+    <hyperlink ref="E141" r:id="rId397" xr:uid="{0055782C-E077-4204-8FF9-57BE6F8FED26}"/>
+    <hyperlink ref="C141" r:id="rId398" xr:uid="{FE323C66-30FE-40E0-8F0E-4108D9EC2713}"/>
+    <hyperlink ref="C142" r:id="rId399" xr:uid="{666B5CC7-4AFE-4EE4-93A2-099371C034E3}"/>
+    <hyperlink ref="D142" r:id="rId400" xr:uid="{A9DFF398-3782-4606-A5AD-16EB49874249}"/>
+    <hyperlink ref="E142" r:id="rId401" xr:uid="{CB3B62B3-3706-4AEA-B831-85D12973AAFB}"/>
+    <hyperlink ref="C143" r:id="rId402" xr:uid="{5B3C3EC4-7E86-40AB-980C-956D883C0DE8}"/>
+    <hyperlink ref="D143" r:id="rId403" xr:uid="{E58660DA-18E4-456D-AE6E-157A8C791640}"/>
+    <hyperlink ref="E143" r:id="rId404" xr:uid="{30D38FD6-524A-4260-A893-C02ABC8FD7D8}"/>
+    <hyperlink ref="C144" r:id="rId405" xr:uid="{EAA73046-9047-4BE9-A054-E3310DE63E1A}"/>
+    <hyperlink ref="D144" r:id="rId406" xr:uid="{54E7A160-9887-4A15-A5E4-7E98C3B546B1}"/>
+    <hyperlink ref="E144" r:id="rId407" xr:uid="{5BA4E4AA-D08F-40BB-B211-CD81B18FF87A}"/>
+    <hyperlink ref="C145" r:id="rId408" xr:uid="{E57FE190-B789-4567-B86E-2D8DD5BB470A}"/>
+    <hyperlink ref="D145" r:id="rId409" xr:uid="{303EC3AA-5A58-4C68-97E5-480D5E8B49ED}"/>
+    <hyperlink ref="E145" r:id="rId410" xr:uid="{111A682B-10E9-494F-BA71-FEC4F7FB0BD6}"/>
+    <hyperlink ref="C146" r:id="rId411" xr:uid="{E353A765-41EF-43C2-AB89-89DFAEA7EAB7}"/>
+    <hyperlink ref="D146" r:id="rId412" xr:uid="{6DB31883-29E3-4B37-A5BC-B8A2B95FBC29}"/>
+    <hyperlink ref="E146" r:id="rId413" xr:uid="{FCF11283-83AE-42A7-BB7D-85631FD6E8B9}"/>
+    <hyperlink ref="C147" r:id="rId414" xr:uid="{2CA57331-C3C7-4E12-82CB-C628ECE4CCAB}"/>
+    <hyperlink ref="D147" r:id="rId415" xr:uid="{B5E1FE84-C98A-420D-837D-C3DCBB95E91F}"/>
+    <hyperlink ref="E147" r:id="rId416" xr:uid="{20932CE8-F8AE-4689-9CD7-3D080869A55D}"/>
+    <hyperlink ref="C148" r:id="rId417" xr:uid="{7618A490-B688-42C9-94E0-4F8540FF40DB}"/>
+    <hyperlink ref="D148" r:id="rId418" xr:uid="{668BB9C5-109F-4A7E-868C-D2732EFA34A2}"/>
+    <hyperlink ref="E148" r:id="rId419" xr:uid="{0F731946-786D-4814-BAE4-8D0C99005D78}"/>
+    <hyperlink ref="C149" r:id="rId420" xr:uid="{51F53306-B34E-472A-B470-69B8029C9ED4}"/>
+    <hyperlink ref="D149" r:id="rId421" xr:uid="{F2FEECB1-F3BC-4C78-B544-613C7FF5E436}"/>
+    <hyperlink ref="E149" r:id="rId422" xr:uid="{343909DC-77D4-4FBB-BE02-DCD4EC0C20EB}"/>
+    <hyperlink ref="C150" r:id="rId423" xr:uid="{F187FD4D-E765-4937-9701-2C58603180AE}"/>
+    <hyperlink ref="D150" r:id="rId424" xr:uid="{31FB4D76-B008-46DB-9637-691B1894CE21}"/>
+    <hyperlink ref="E150" r:id="rId425" xr:uid="{03572D9E-807D-4918-B128-29411ACBB625}"/>
+    <hyperlink ref="C151" r:id="rId426" xr:uid="{5130DE5E-46EF-4B05-8FE0-179C2E7E6948}"/>
+    <hyperlink ref="D151" r:id="rId427" xr:uid="{97742F59-5F59-4D68-996E-0A272575FADC}"/>
+    <hyperlink ref="E151" r:id="rId428" xr:uid="{2355B201-6EF9-4A6A-A9B9-BF166EC28606}"/>
+    <hyperlink ref="C152" r:id="rId429" xr:uid="{407F15B9-9D77-4AFB-B5E8-1B163C7E370E}"/>
+    <hyperlink ref="D152" r:id="rId430" xr:uid="{7A5EB5DE-BDC8-4E93-9761-A6603D00EFAD}"/>
+    <hyperlink ref="E152" r:id="rId431" xr:uid="{097CE107-4BA7-4CF3-996A-093477F670F6}"/>
+    <hyperlink ref="D153" r:id="rId432" xr:uid="{51B6FCED-FA56-433D-BA3D-445C0F2FE651}"/>
+    <hyperlink ref="E153" r:id="rId433" xr:uid="{26C3E259-1ACD-4F3A-B70D-194C131947DB}"/>
+    <hyperlink ref="C153" r:id="rId434" xr:uid="{3A114C26-8E8C-45B9-94BD-FCD3CAA9597E}"/>
+    <hyperlink ref="C154" r:id="rId435" xr:uid="{9AA9391F-DE63-4135-A127-DF0F47F7D8C7}"/>
+    <hyperlink ref="D154" r:id="rId436" xr:uid="{2BF42871-0750-440A-A243-619A1C20CC7F}"/>
+    <hyperlink ref="E154" r:id="rId437" xr:uid="{D39D1674-E469-410B-9639-99835CA9A908}"/>
+    <hyperlink ref="C155" r:id="rId438" xr:uid="{5F3DC677-1855-4283-B201-795E598B8917}"/>
+    <hyperlink ref="D155" r:id="rId439" xr:uid="{97F71AB0-0556-481D-B3A2-984C5AB5ED3A}"/>
+    <hyperlink ref="E155" r:id="rId440" xr:uid="{F4091531-5EEE-42BF-9549-D3422C21479A}"/>
+    <hyperlink ref="C156" r:id="rId441" xr:uid="{09680C2A-D8C5-41B4-9F07-96FF1792918C}"/>
+    <hyperlink ref="D156" r:id="rId442" xr:uid="{B9850E60-1546-4D20-8BF8-E8A5C91504C9}"/>
+    <hyperlink ref="E156" r:id="rId443" xr:uid="{CB7D6C00-6A72-4633-A0C4-CA7AD5F7CA43}"/>
+    <hyperlink ref="C157" r:id="rId444" xr:uid="{80024236-A643-48BC-A603-88E4C61F39E9}"/>
+    <hyperlink ref="D157" r:id="rId445" xr:uid="{120C8743-AA48-4C9A-AE55-5610BE126DC3}"/>
+    <hyperlink ref="E157" r:id="rId446" xr:uid="{2D5BB430-5FE3-453B-A9D2-87D25EF175BD}"/>
+    <hyperlink ref="C158" r:id="rId447" xr:uid="{4DFB4F67-145A-44E0-BE4E-70236393A673}"/>
+    <hyperlink ref="D158" r:id="rId448" xr:uid="{63643BC2-FC62-42D6-82C6-75379B5F7031}"/>
+    <hyperlink ref="E158" r:id="rId449" xr:uid="{6CF4B868-96BA-46BA-B87F-853852F4531D}"/>
+    <hyperlink ref="C159" r:id="rId450" xr:uid="{352410C9-FE4B-4A2C-BC1F-750169232690}"/>
+    <hyperlink ref="D159" r:id="rId451" xr:uid="{AFE88A43-637E-4B75-B37A-1F57451F4619}"/>
+    <hyperlink ref="E159" r:id="rId452" xr:uid="{7535847A-C949-43A9-93A4-F0EC6DDF68DA}"/>
+    <hyperlink ref="C160" r:id="rId453" xr:uid="{4C1038DE-1D54-48E4-8E66-F691E40DCC63}"/>
+    <hyperlink ref="D160" r:id="rId454" xr:uid="{41172669-0845-43AD-9650-8B8A62925666}"/>
+    <hyperlink ref="E160" r:id="rId455" xr:uid="{B16881C8-92C0-4AA1-B859-DBDCB15AD570}"/>
+    <hyperlink ref="C161" r:id="rId456" xr:uid="{39A2F065-2C25-448A-8687-9F2149D01184}"/>
+    <hyperlink ref="D161" r:id="rId457" xr:uid="{F2ED0C3A-0135-4147-AEFF-DC4B8ED0D685}"/>
+    <hyperlink ref="E161" r:id="rId458" xr:uid="{8DF3594C-0BF9-448B-A503-24794FCECEA3}"/>
+    <hyperlink ref="D162" r:id="rId459" xr:uid="{2D27BDFB-D4B5-44B9-965C-A93682BCB150}"/>
+    <hyperlink ref="E162" r:id="rId460" xr:uid="{744A7EC5-AEB8-42E3-A556-E4E16C245E49}"/>
+    <hyperlink ref="C162" r:id="rId461" xr:uid="{1A5BE688-8DAF-46EE-BE55-B56FA387D60A}"/>
+    <hyperlink ref="C163" r:id="rId462" xr:uid="{A2A8969B-E67C-4C42-9F40-97418205870F}"/>
+    <hyperlink ref="D163" r:id="rId463" xr:uid="{8C15BC14-EB1D-4AFA-82A9-D7F5FEB92B34}"/>
+    <hyperlink ref="E163" r:id="rId464" xr:uid="{C1AF09A0-75AC-415B-AEAA-FFE6CDF5282B}"/>
+    <hyperlink ref="C164" r:id="rId465" xr:uid="{97A7FD74-2B85-4FD7-96FD-C28091A20A4D}"/>
+    <hyperlink ref="D164" r:id="rId466" xr:uid="{8C7ACE0C-84B0-4967-A6EA-73EBBBCA6E3A}"/>
+    <hyperlink ref="E164" r:id="rId467" xr:uid="{63C7876B-76A9-4A33-B78B-52C0CA2D8D5E}"/>
+    <hyperlink ref="C165" r:id="rId468" xr:uid="{06B4DEBF-7C8E-4884-91BE-A793EE0F62CC}"/>
+    <hyperlink ref="D165" r:id="rId469" xr:uid="{A9147945-5306-4AE5-BE85-C90C7FC7EC3C}"/>
+    <hyperlink ref="E165" r:id="rId470" xr:uid="{77243768-5B39-4BB1-BA96-960A09265D09}"/>
+    <hyperlink ref="D166" r:id="rId471" xr:uid="{0D2C4551-5A3A-4398-A3D2-99FB0401A7D1}"/>
+    <hyperlink ref="E166" r:id="rId472" xr:uid="{38A6A660-830B-4694-A398-A9DE1011AC6B}"/>
+    <hyperlink ref="C166" r:id="rId473" xr:uid="{5228C198-AF2C-40F8-B2F5-057085C54F0D}"/>
+    <hyperlink ref="C167" r:id="rId474" xr:uid="{A08507FD-CA4F-44FD-80EA-F0484A51F904}"/>
+    <hyperlink ref="D167" r:id="rId475" xr:uid="{F9694B45-4A2C-4F66-8EE4-DA8EE40951ED}"/>
+    <hyperlink ref="E167" r:id="rId476" xr:uid="{C3119FB8-069B-4D3F-B5C3-5883D3A505F1}"/>
+    <hyperlink ref="C168" r:id="rId477" xr:uid="{AA2D388E-48CF-41C9-B888-4F64BFF2ACC5}"/>
+    <hyperlink ref="D168" r:id="rId478" xr:uid="{136A9ACA-B873-408C-877B-B88BEDEE02DE}"/>
+    <hyperlink ref="E168" r:id="rId479" xr:uid="{45143C2B-0CE5-460D-8C8C-7BDD7391EC20}"/>
+    <hyperlink ref="C169" r:id="rId480" xr:uid="{412AABCD-D11B-4C1F-BAE3-8E9B5314FEFE}"/>
+    <hyperlink ref="D169" r:id="rId481" xr:uid="{52143DB4-9220-420E-9325-C79A91D3E77F}"/>
+    <hyperlink ref="E169" r:id="rId482" xr:uid="{EBD5079E-6759-45C1-A040-15A1D7EFA833}"/>
+    <hyperlink ref="C170" r:id="rId483" xr:uid="{D9EDA746-00FA-479B-BBF8-E6EA24906B94}"/>
+    <hyperlink ref="D170" r:id="rId484" xr:uid="{F2F02B4C-A61F-48DB-B4B9-B590F1EAE1A5}"/>
+    <hyperlink ref="E170" r:id="rId485" xr:uid="{4EF3DEB5-F631-42E5-BF23-8FD5BD7C5726}"/>
+    <hyperlink ref="C171" r:id="rId486" xr:uid="{C7AC3295-F2D7-4B73-81FE-CE9DD8908E72}"/>
+    <hyperlink ref="D171" r:id="rId487" xr:uid="{13A8A69F-88CE-42AE-A904-E26015719290}"/>
+    <hyperlink ref="E171" r:id="rId488" xr:uid="{69E9CB21-248F-4A60-986D-523E9D222CCD}"/>
+    <hyperlink ref="C172" r:id="rId489" xr:uid="{7627DCB7-8878-43A8-B6E9-AA0B9A8AA69D}"/>
+    <hyperlink ref="D172" r:id="rId490" xr:uid="{FCCBB0CF-B9DD-4759-BBA3-76BD72CDE47E}"/>
+    <hyperlink ref="E172" r:id="rId491" xr:uid="{3E811DA2-3C40-4364-9266-6773CDEE5611}"/>
+    <hyperlink ref="C173" r:id="rId492" xr:uid="{FC27C7F6-56D3-4353-B218-AEDBD69411BE}"/>
+    <hyperlink ref="D173" r:id="rId493" xr:uid="{1FAEEA19-C0F2-4B64-AB53-5CE1FCFD3EED}"/>
+    <hyperlink ref="E173" r:id="rId494" xr:uid="{9AFEB9F6-C42C-4F69-BAB9-0F96228BAB75}"/>
+    <hyperlink ref="C174" r:id="rId495" xr:uid="{782E6140-94C3-407F-BEAF-9C0D976620EB}"/>
+    <hyperlink ref="D174" r:id="rId496" xr:uid="{B6A4BB4A-CEE1-4126-85FD-8A0A92A86F6C}"/>
+    <hyperlink ref="E174" r:id="rId497" xr:uid="{4DE847BB-899E-400F-B0A1-5368BD326435}"/>
+    <hyperlink ref="C175" r:id="rId498" xr:uid="{550B60D7-37BE-42DF-A0A6-234EE2ABEC88}"/>
+    <hyperlink ref="D175" r:id="rId499" xr:uid="{FE54EAA5-5BCB-4AE8-B0F0-DF219D75D2FA}"/>
+    <hyperlink ref="E175" r:id="rId500" xr:uid="{5F404BDE-7004-4B15-8063-6FFDD0232C10}"/>
+    <hyperlink ref="D176" r:id="rId501" xr:uid="{04847EC6-CA8E-40B5-A255-4AA69821E9CD}"/>
+    <hyperlink ref="E176" r:id="rId502" xr:uid="{C5321455-60AF-4B1F-B2EB-9C48ABE6CF88}"/>
+    <hyperlink ref="C176" r:id="rId503" xr:uid="{F487FA1F-6345-4747-9B2D-E8B2F3CA8F64}"/>
+    <hyperlink ref="C177" r:id="rId504" xr:uid="{0BB76D84-05E9-403F-B67C-C3BFFCCC1DE9}"/>
+    <hyperlink ref="D177" r:id="rId505" xr:uid="{E68DE772-C262-43D4-BAB1-57B7508710F5}"/>
+    <hyperlink ref="E177" r:id="rId506" xr:uid="{E2FD5107-217F-4912-8F1C-CBCA0456D0B1}"/>
+    <hyperlink ref="C178" r:id="rId507" xr:uid="{0709A472-9980-4F85-A449-8A5D6EABD5F4}"/>
+    <hyperlink ref="D178" r:id="rId508" xr:uid="{31C86E75-E56D-4C5A-965A-002F4B567CEA}"/>
+    <hyperlink ref="E178" r:id="rId509" xr:uid="{A44C8FE0-0122-4430-BB7B-95FC5AC20FD1}"/>
+    <hyperlink ref="C179" r:id="rId510" xr:uid="{6CA3E827-405F-40BE-9BA0-7F75BE64C3EF}"/>
+    <hyperlink ref="D179" r:id="rId511" xr:uid="{1AB16091-69AE-4105-9BA6-B775B46361F8}"/>
+    <hyperlink ref="E179" r:id="rId512" xr:uid="{2B7A126E-8D1B-4E8F-93A6-C98453F4B0CD}"/>
+    <hyperlink ref="C180" r:id="rId513" xr:uid="{FF9DC8D1-E300-4D00-8478-B4C4465463B0}"/>
+    <hyperlink ref="D180" r:id="rId514" xr:uid="{C7FB4928-100E-4F31-AA8B-9BB5386BD6E2}"/>
+    <hyperlink ref="E180" r:id="rId515" xr:uid="{33E88EF2-069C-4A8A-A4B9-407D561D9FA7}"/>
+    <hyperlink ref="C181" r:id="rId516" xr:uid="{AD27F6F9-722F-4772-BAD3-292259E599AE}"/>
+    <hyperlink ref="D181" r:id="rId517" xr:uid="{9855AD87-CCE8-4B4A-9D90-654E9CB9A884}"/>
+    <hyperlink ref="E181" r:id="rId518" xr:uid="{DABA9FDA-64E2-49EB-A86C-6A285B8ED457}"/>
+    <hyperlink ref="C182" r:id="rId519" xr:uid="{08DC194C-ADC7-4BD9-B1FA-D02B1EB30413}"/>
+    <hyperlink ref="D182" r:id="rId520" xr:uid="{BDCC0E77-3EA0-4F00-B40F-EB3744C4B10A}"/>
+    <hyperlink ref="E182" r:id="rId521" xr:uid="{0C11EA0B-B2D0-438E-81C0-C400F6D0799A}"/>
+    <hyperlink ref="C183" r:id="rId522" xr:uid="{13991465-B6B8-432B-B460-78ABB1DED868}"/>
+    <hyperlink ref="D183" r:id="rId523" xr:uid="{A036A9F5-033D-4A23-B1E3-B321FB1A1D5C}"/>
+    <hyperlink ref="E183" r:id="rId524" xr:uid="{D1FD862C-B5D6-4B13-931B-57B7FFF1059A}"/>
+    <hyperlink ref="C184" r:id="rId525" xr:uid="{5217B7E5-50F7-4581-9109-F6A8BC875186}"/>
+    <hyperlink ref="D184" r:id="rId526" xr:uid="{C3F790CF-A478-40B7-99F6-7D2667CBC146}"/>
+    <hyperlink ref="E184" r:id="rId527" xr:uid="{A5F80E79-506C-4A15-AACD-68F53D61E373}"/>
+    <hyperlink ref="C185" r:id="rId528" xr:uid="{62E029C0-61D3-4187-A49A-6F8E847B07E9}"/>
+    <hyperlink ref="D185" r:id="rId529" xr:uid="{682FAA6B-7ADD-4D0B-9D48-124102D3B8C4}"/>
+    <hyperlink ref="E185" r:id="rId530" xr:uid="{CB64775F-93CB-4F3C-A7B2-61AA1EEC9FF4}"/>
+    <hyperlink ref="D186" r:id="rId531" xr:uid="{33DB2910-4B9B-4EBD-94DB-9D1D8BA1A60A}"/>
+    <hyperlink ref="E186" r:id="rId532" xr:uid="{D816F0E8-5CA4-4FBA-A574-65EB5C502159}"/>
+    <hyperlink ref="C186" r:id="rId533" xr:uid="{7BED455F-4DC7-4B45-AD26-E1286840DEBE}"/>
+    <hyperlink ref="C187" r:id="rId534" xr:uid="{B17E7A06-B7A3-43DE-959C-80217F4C7404}"/>
+    <hyperlink ref="D187" r:id="rId535" xr:uid="{108A2D11-51B8-4F46-B0AE-357FA3F6BDB6}"/>
+    <hyperlink ref="E187" r:id="rId536" xr:uid="{16666982-1A83-4A62-BFC7-C4F40E6C916E}"/>
+    <hyperlink ref="C188" r:id="rId537" xr:uid="{053DBA08-46A7-4A97-9457-F0E304824F8E}"/>
+    <hyperlink ref="D188" r:id="rId538" xr:uid="{DB4ECA15-195B-4A54-858F-239BA708B125}"/>
+    <hyperlink ref="E188" r:id="rId539" xr:uid="{17CC691E-0C7E-443C-B3E1-54C8BFC12D95}"/>
+    <hyperlink ref="C189" r:id="rId540" xr:uid="{488BAF16-AD49-4FAE-8E4C-CE7962082CBA}"/>
+    <hyperlink ref="D189" r:id="rId541" xr:uid="{0B038405-DDEA-461D-994B-7F271E9120F4}"/>
+    <hyperlink ref="E189" r:id="rId542" xr:uid="{7BACCCB4-5CF4-4224-9201-E647233DE274}"/>
+    <hyperlink ref="C190" r:id="rId543" xr:uid="{E9108E47-563C-4F4D-8B1F-CB863619C501}"/>
+    <hyperlink ref="D190" r:id="rId544" xr:uid="{ECB18330-35A1-421E-8B98-A38AB1F12F4B}"/>
+    <hyperlink ref="E190" r:id="rId545" xr:uid="{594B3616-5B4C-4902-90E8-B56CF4ADD901}"/>
+    <hyperlink ref="C191" r:id="rId546" xr:uid="{BEC6DA00-205E-4FA8-BF78-644278A12620}"/>
+    <hyperlink ref="D191" r:id="rId547" xr:uid="{66E4959D-D2E5-40E0-9A50-3E9722C83879}"/>
+    <hyperlink ref="E191" r:id="rId548" xr:uid="{165E3072-0F8C-4D07-A8EE-AFB2E92D10D0}"/>
+    <hyperlink ref="C192" r:id="rId549" xr:uid="{8BDFFA66-526B-49E6-A9EF-74BACEF2FC3A}"/>
+    <hyperlink ref="D192" r:id="rId550" xr:uid="{23452AE3-198E-4555-8556-92D1EB9C8F2F}"/>
+    <hyperlink ref="E192" r:id="rId551" xr:uid="{1C8BB96E-E2D2-41A2-B51E-CA1C94882C45}"/>
+    <hyperlink ref="C193" r:id="rId552" xr:uid="{78499224-1133-4CA4-8141-97A18D48B873}"/>
+    <hyperlink ref="D193" r:id="rId553" xr:uid="{B9B02DD2-D017-4DBC-9327-5DF3E8B353CB}"/>
+    <hyperlink ref="E193" r:id="rId554" xr:uid="{4CDCE363-4F15-4C8E-88A0-16B4ACE31706}"/>
+    <hyperlink ref="D194" r:id="rId555" xr:uid="{9672DF3D-1B42-4B06-BE7E-8C371290DDD8}"/>
+    <hyperlink ref="E194" r:id="rId556" xr:uid="{A6A6609E-1ACE-4AE1-8630-67EC2A09BB1B}"/>
+    <hyperlink ref="C194" r:id="rId557" xr:uid="{2945D925-89ED-4A50-9C8A-33FAE3D9B663}"/>
+    <hyperlink ref="C195" r:id="rId558" xr:uid="{B2232121-8FC5-4AFB-B4A5-EAFCA6F8BF55}"/>
+    <hyperlink ref="D195" r:id="rId559" xr:uid="{BDB9895C-3A01-437E-B535-262F78163F79}"/>
+    <hyperlink ref="E195" r:id="rId560" xr:uid="{7E8CB580-3C77-4108-A7BB-241E5DD2F8F8}"/>
+    <hyperlink ref="C196" r:id="rId561" xr:uid="{0E762398-C5ED-49DE-9BD7-D01671B4E18A}"/>
+    <hyperlink ref="D196" r:id="rId562" xr:uid="{7FC49659-FA8F-434A-B4B6-95508B1B4D35}"/>
+    <hyperlink ref="E196" r:id="rId563" xr:uid="{5FD4642D-66C0-4BCC-9C59-E55B95CFBFBB}"/>
+    <hyperlink ref="C197" r:id="rId564" xr:uid="{63BBE702-55C8-4458-8A67-C5591C5F9247}"/>
+    <hyperlink ref="D197" r:id="rId565" xr:uid="{A666B7EF-0CBD-4183-BF04-FD5B6DDCF6FD}"/>
+    <hyperlink ref="D99" r:id="rId566" xr:uid="{BB5402C0-11CF-4FB7-9D11-E4E06DA8E09D}"/>
+    <hyperlink ref="C99" r:id="rId567" xr:uid="{5098A259-C902-4545-A7E1-E636AB33D5F8}"/>
+    <hyperlink ref="D86" r:id="rId568" display="https://www.camara.leg.br/internet/sitaqweb/TextoHTML.asp?etapa=11&amp;tpReuniaoEvento=AP%20c/%20Convidado&amp;dtReuniao=15/08/2017&amp;hrInicio=14:50:00&amp;hrFim=17:12:00&amp;origemDiscurso=&amp;nmLocal=Plen%C3%A1rio%20Principal%20-%20CD&amp;nuSessao=1047/17&amp;nuQuarto=0&amp;nuOrador=0&amp;nuInsercao=0&amp;dtHorarioQuarto=14:50&amp;sgFaseSessao=&amp;Data=15/08/2017&amp;txApelido=&amp;txFaseSessao=&amp;txTipoSessao=Permanente&amp;dtHoraQuarto=14:50&amp;txEtapa=" xr:uid="{885EDDC5-59F7-4E1C-AF16-381A4A38D774}"/>
+    <hyperlink ref="C86" r:id="rId569" xr:uid="{4A17DC70-EC44-4004-B071-6F5D899C8CA5}"/>
+    <hyperlink ref="D71" r:id="rId570" xr:uid="{D677B959-EB3C-4DDB-8AEF-E8EAE6D6D45E}"/>
+    <hyperlink ref="C71" r:id="rId571" xr:uid="{0AD8437A-2704-40CD-866A-26901C1B53CE}"/>
+    <hyperlink ref="D63" r:id="rId572" xr:uid="{5F59921F-E727-4A1F-AE6F-37476A2F81C2}"/>
+    <hyperlink ref="C63" r:id="rId573" xr:uid="{4B817215-AB66-422A-B2EE-745DCCE2715E}"/>
+    <hyperlink ref="C62" r:id="rId574" xr:uid="{2DA64800-7A72-4482-919D-DFF1D13D4B55}"/>
+    <hyperlink ref="D62" r:id="rId575" xr:uid="{E8EC2437-F030-4E8C-B6AC-917AA71D6D2D}"/>
+    <hyperlink ref="D40" r:id="rId576" xr:uid="{6C41F5BF-C09E-47D4-A816-D0E540BD6149}"/>
+    <hyperlink ref="C40" r:id="rId577" xr:uid="{CBA2CB5F-E42B-4632-83EE-22826ADE1E04}"/>
+    <hyperlink ref="E197" r:id="rId578" xr:uid="{136FF705-8DCE-4116-BE70-5F1542A088B0}"/>
+    <hyperlink ref="C198" r:id="rId579" xr:uid="{3FB904D1-0936-422F-96AB-F3B96921D779}"/>
+    <hyperlink ref="D198" r:id="rId580" xr:uid="{7A54B018-01DB-4819-9FD1-68863145C0A1}"/>
+    <hyperlink ref="E198" r:id="rId581" xr:uid="{E3C9E074-5A18-4A4E-8CA3-EEB4F330DFC6}"/>
+    <hyperlink ref="C199" r:id="rId582" xr:uid="{E2D42ECE-DCF2-4092-B7EF-C717EECA06D7}"/>
+    <hyperlink ref="D199" r:id="rId583" xr:uid="{D3B0D91F-A5F5-489B-B4BF-5B6ADA49D078}"/>
+    <hyperlink ref="E199" r:id="rId584" xr:uid="{9E3CF267-2270-4A5E-BF99-A49458146C5C}"/>
+    <hyperlink ref="C200" r:id="rId585" xr:uid="{39D382AA-57C1-42F8-ABF7-11A7F0B35567}"/>
+    <hyperlink ref="D200" r:id="rId586" xr:uid="{8CE8A2BD-98A2-45D9-B373-7C90E69ADB93}"/>
+    <hyperlink ref="E200" r:id="rId587" xr:uid="{DE229DE6-DE64-42DD-97A1-D38A12923FD3}"/>
+    <hyperlink ref="C201" r:id="rId588" xr:uid="{189D0765-1C92-4FC1-A376-28B52EA2BFAF}"/>
+    <hyperlink ref="D201" r:id="rId589" xr:uid="{2532C84C-8DB5-4D9F-8FFB-F09727EC3D64}"/>
+    <hyperlink ref="E201" r:id="rId590" xr:uid="{A9C00FED-2E5B-4151-A8D6-2CBF429036A5}"/>
+    <hyperlink ref="C202" r:id="rId591" xr:uid="{0FB758F3-8CEC-44F8-AB0B-FB5749251F72}"/>
+    <hyperlink ref="D202" r:id="rId592" xr:uid="{14790960-D653-4274-8C1A-87D26826D0D0}"/>
+    <hyperlink ref="E202" r:id="rId593" xr:uid="{669AE71B-0710-4E47-9B20-28C6E0D2A24C}"/>
+    <hyperlink ref="C203" r:id="rId594" xr:uid="{6C1C977A-8104-4C5D-BED7-C833FD88FC10}"/>
+    <hyperlink ref="D203" r:id="rId595" xr:uid="{FA52D527-723E-449E-AE77-53A711E8B5F4}"/>
+    <hyperlink ref="E203" r:id="rId596" xr:uid="{7D40609C-37B6-4DA5-86FD-A779CCE9CF33}"/>
+    <hyperlink ref="D204" r:id="rId597" xr:uid="{E1F2A5BF-32A9-48D5-81EE-19ABF3643DD2}"/>
+    <hyperlink ref="E204" r:id="rId598" xr:uid="{E561AB7E-F883-4B46-9BD4-A1A7658BB442}"/>
+    <hyperlink ref="C204" r:id="rId599" xr:uid="{0B823933-67DE-41F8-B9F5-D78FB031387C}"/>
+    <hyperlink ref="C205" r:id="rId600" xr:uid="{26F9A583-2496-4B17-A929-300CBDA2E24D}"/>
+    <hyperlink ref="D205" r:id="rId601" xr:uid="{6719EDC2-583C-49D3-9ECA-9AAEAB5A1AF8}"/>
+    <hyperlink ref="E205" r:id="rId602" xr:uid="{3243DF7A-EE24-42C4-9051-EF34793BE812}"/>
+    <hyperlink ref="C206" r:id="rId603" xr:uid="{4C45050E-CAB2-4E91-876A-26ACF94DB8B2}"/>
+    <hyperlink ref="D206" r:id="rId604" xr:uid="{4FE2A5B0-C928-4394-8042-D3AA021DA4D8}"/>
+    <hyperlink ref="E206" r:id="rId605" xr:uid="{CAB1117F-895B-408D-BFB0-CC8642447B67}"/>
+    <hyperlink ref="C207" r:id="rId606" xr:uid="{3497FE2B-F080-4F0F-9454-A2F8E2BCEA79}"/>
+    <hyperlink ref="D207" r:id="rId607" xr:uid="{C1B80CC4-8153-4B20-A3F2-B283168811C5}"/>
+    <hyperlink ref="E207" r:id="rId608" xr:uid="{BF0434BE-354E-4789-9E21-F298661908C9}"/>
+    <hyperlink ref="C208" r:id="rId609" xr:uid="{E432FEE7-0CE3-4671-A6DE-A89067FE71F8}"/>
+    <hyperlink ref="D208" r:id="rId610" xr:uid="{9B118C1B-E5E7-4F47-BFA5-206491EA6ED8}"/>
+    <hyperlink ref="E208" r:id="rId611" xr:uid="{9EA9596A-CB3D-4B30-8E07-CA8A3FF7C508}"/>
+    <hyperlink ref="C209" r:id="rId612" xr:uid="{46C6222B-B670-40C3-A605-FABE1731989A}"/>
+    <hyperlink ref="D209" r:id="rId613" xr:uid="{C653707F-D543-43CC-A01D-24A54A6A319B}"/>
+    <hyperlink ref="E209" r:id="rId614" xr:uid="{60116EA4-2834-4C7A-B4DB-1CE223CB90BB}"/>
+    <hyperlink ref="C210" r:id="rId615" xr:uid="{20EC698E-A69F-497B-8D14-1C5CA444BC21}"/>
+    <hyperlink ref="D210" r:id="rId616" xr:uid="{AFAB7C9A-C544-47BD-8645-5C31CE7C5CF3}"/>
+    <hyperlink ref="E210" r:id="rId617" xr:uid="{F53AF2AB-0CE9-45A6-B905-24C7FEEA3E52}"/>
+    <hyperlink ref="C211" r:id="rId618" xr:uid="{30CD9287-A385-456E-9D5E-59944E3156E1}"/>
+    <hyperlink ref="D211" r:id="rId619" xr:uid="{C9FDF5BB-9B0E-442F-AE18-EBCAF9FA12BA}"/>
+    <hyperlink ref="E211" r:id="rId620" xr:uid="{E3661C98-D989-4879-A8FC-B6166662C8D7}"/>
+    <hyperlink ref="C55" r:id="rId621" xr:uid="{2102EDB4-6981-4633-9FD3-E647448181FC}"/>
+    <hyperlink ref="D55" r:id="rId622" xr:uid="{0DB9D726-23FB-4B78-94AC-DFD7B21AB5AE}"/>
+    <hyperlink ref="E55" r:id="rId623" xr:uid="{BF7B36EC-2642-4F9B-A942-FC7DA39117FB}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId627"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId624"/>
 </worksheet>
 </file>
 
@@ -6105,7 +6139,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -6113,13 +6147,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrige metadados das matérias 81-100. Apaga as matérias 94 e 95 (não há dados suficientes) e as substituem pelas 209 e 210. A base agora passa a ter 208 matérias.
</commit_message>
<xml_diff>
--- a/projeto final/1 - levantamento/Matérias CD.xlsx
+++ b/projeto final/1 - levantamento/Matérias CD.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caris\Desktop\IA024_deep_learning_nlp\projeto final\1 - levantamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B98F8F-E94C-4F8B-93F8-BBE884BDD345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27D6A41-1C35-44D4-AC9F-FD538BE37207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A25B0F39-AFD6-49AD-BAE6-0169C11C595E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A25B0F39-AFD6-49AD-BAE6-0169C11C595E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tem transcrição" sheetId="1" r:id="rId1"/>
     <sheet name="Aguardando" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tem transcrição'!$C$1:$E$211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tem transcrição'!$C$1:$E$209</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="629">
   <si>
     <t>Matéria</t>
   </si>
@@ -865,24 +865,6 @@
   </si>
   <si>
     <t>https://www.camara.leg.br/noticias/857397-ESPECIALISTAS-SUGEREM-MUDANCAS-EM-PROJETO-SOBRE-ENSINO-SUPERIOR-E-FORMACAO-TECNICA-PROFISSIONAL</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/noticias/840546-DEBATEDORES-CRITICAM-COBRANCAS-DE-VALORES-DIFERENCIADOS-DE-PLANOS-DE-SAUDE-PARA-IDOSOS</t>
-  </si>
-  <si>
-    <t>https://escriba.camara.leg.br/escriba-servicosweb/html/64528</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/internet/ordemdodia/integras/2126783.htm</t>
-  </si>
-  <si>
-    <t>https://escriba.camara.leg.br/escriba-servicosweb/html/64054</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/internet/ordemdodia/integras/2115753.htm</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/noticias/833999-DEBATEDORES-DESTACAM-COMPLEXIDADE-NO-LICENCIAMENTO-DE-HIDRELETRICAS-NA-REGIAO-NORTE</t>
   </si>
   <si>
     <t>https://escriba.camara.leg.br/escriba-servicosweb/html/64204</t>
@@ -1989,9 +1971,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2327,10 +2310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7617A561-B2B5-4674-8694-EA4F3B3BAE78}">
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,19 +2326,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B1" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="C1" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="D1" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="E1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2363,7 +2346,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -2380,7 +2363,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -2397,7 +2380,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -2414,7 +2397,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -2431,7 +2414,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -2448,7 +2431,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -2465,7 +2448,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -2482,7 +2465,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
@@ -2499,7 +2482,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -2516,7 +2499,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>31</v>
@@ -2533,7 +2516,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2550,7 +2533,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
@@ -2567,7 +2550,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
@@ -2584,7 +2567,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>41</v>
@@ -2601,7 +2584,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>44</v>
@@ -2618,7 +2601,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
@@ -2635,7 +2618,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>51</v>
@@ -2649,7 +2632,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>52</v>
@@ -2666,7 +2649,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>55</v>
@@ -2683,7 +2666,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>58</v>
@@ -2700,7 +2683,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>61</v>
@@ -2717,7 +2700,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>64</v>
@@ -2734,7 +2717,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>67</v>
@@ -2751,7 +2734,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>70</v>
@@ -2768,7 +2751,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>73</v>
@@ -2785,7 +2768,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>76</v>
@@ -2802,7 +2785,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>79</v>
@@ -2819,7 +2802,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>82</v>
@@ -2836,7 +2819,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>85</v>
@@ -2853,7 +2836,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>88</v>
@@ -2870,7 +2853,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>91</v>
@@ -2887,7 +2870,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>94</v>
@@ -2904,7 +2887,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>97</v>
@@ -2921,7 +2904,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>100</v>
@@ -2938,7 +2921,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>103</v>
@@ -2955,7 +2938,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>106</v>
@@ -2972,7 +2955,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>109</v>
@@ -2989,7 +2972,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>112</v>
@@ -3006,7 +2989,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>115</v>
@@ -3020,7 +3003,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>117</v>
@@ -3037,7 +3020,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>120</v>
@@ -3054,7 +3037,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>123</v>
@@ -3071,7 +3054,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>126</v>
@@ -3088,7 +3071,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>129</v>
@@ -3105,7 +3088,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>132</v>
@@ -3122,7 +3105,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>135</v>
@@ -3139,7 +3122,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>138</v>
@@ -3156,7 +3139,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>141</v>
@@ -3173,7 +3156,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>144</v>
@@ -3190,7 +3173,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>147</v>
@@ -3207,7 +3190,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>150</v>
@@ -3224,7 +3207,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>155</v>
@@ -3241,7 +3224,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>156</v>
@@ -3258,16 +3241,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3275,7 +3258,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>159</v>
@@ -3292,7 +3275,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>164</v>
@@ -3309,7 +3292,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>165</v>
@@ -3326,7 +3309,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>170</v>
@@ -3343,7 +3326,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>171</v>
@@ -3360,7 +3343,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>174</v>
@@ -3377,7 +3360,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>178</v>
@@ -3391,7 +3374,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>179</v>
@@ -3405,7 +3388,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>181</v>
@@ -3422,7 +3405,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>184</v>
@@ -3439,7 +3422,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>187</v>
@@ -3456,7 +3439,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>190</v>
@@ -3473,7 +3456,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>193</v>
@@ -3490,7 +3473,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>198</v>
@@ -3507,7 +3490,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>199</v>
@@ -3524,7 +3507,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>202</v>
@@ -3537,6 +3520,9 @@
       <c r="A72">
         <v>71</v>
       </c>
+      <c r="B72" t="s">
+        <v>628</v>
+      </c>
       <c r="C72" s="1" t="s">
         <v>204</v>
       </c>
@@ -3551,6 +3537,9 @@
       <c r="A73">
         <v>72</v>
       </c>
+      <c r="B73" t="s">
+        <v>628</v>
+      </c>
       <c r="C73" s="1" t="s">
         <v>207</v>
       </c>
@@ -3565,6 +3554,9 @@
       <c r="A74">
         <v>73</v>
       </c>
+      <c r="B74" t="s">
+        <v>628</v>
+      </c>
       <c r="C74" s="1" t="s">
         <v>212</v>
       </c>
@@ -3579,6 +3571,9 @@
       <c r="A75">
         <v>74</v>
       </c>
+      <c r="B75" t="s">
+        <v>628</v>
+      </c>
       <c r="C75" s="1" t="s">
         <v>213</v>
       </c>
@@ -3593,6 +3588,9 @@
       <c r="A76">
         <v>75</v>
       </c>
+      <c r="B76" t="s">
+        <v>628</v>
+      </c>
       <c r="C76" s="1" t="s">
         <v>218</v>
       </c>
@@ -3607,6 +3605,9 @@
       <c r="A77">
         <v>76</v>
       </c>
+      <c r="B77" t="s">
+        <v>628</v>
+      </c>
       <c r="C77" s="1" t="s">
         <v>219</v>
       </c>
@@ -3621,6 +3622,9 @@
       <c r="A78">
         <v>77</v>
       </c>
+      <c r="B78" t="s">
+        <v>628</v>
+      </c>
       <c r="C78" s="1" t="s">
         <v>224</v>
       </c>
@@ -3635,6 +3639,9 @@
       <c r="A79">
         <v>78</v>
       </c>
+      <c r="B79" t="s">
+        <v>628</v>
+      </c>
       <c r="C79" s="1" t="s">
         <v>227</v>
       </c>
@@ -3649,6 +3656,9 @@
       <c r="A80">
         <v>79</v>
       </c>
+      <c r="B80" t="s">
+        <v>628</v>
+      </c>
       <c r="C80" s="1" t="s">
         <v>230</v>
       </c>
@@ -3663,6 +3673,9 @@
       <c r="A81">
         <v>80</v>
       </c>
+      <c r="B81" t="s">
+        <v>628</v>
+      </c>
       <c r="C81" s="1" t="s">
         <v>233</v>
       </c>
@@ -3677,6 +3690,9 @@
       <c r="A82">
         <v>81</v>
       </c>
+      <c r="B82" t="s">
+        <v>628</v>
+      </c>
       <c r="C82" s="1" t="s">
         <v>236</v>
       </c>
@@ -3691,6 +3707,9 @@
       <c r="A83">
         <v>82</v>
       </c>
+      <c r="B83" t="s">
+        <v>628</v>
+      </c>
       <c r="C83" s="1" t="s">
         <v>237</v>
       </c>
@@ -3705,6 +3724,9 @@
       <c r="A84">
         <v>83</v>
       </c>
+      <c r="B84" t="s">
+        <v>628</v>
+      </c>
       <c r="C84" s="1" t="s">
         <v>242</v>
       </c>
@@ -3719,6 +3741,9 @@
       <c r="A85">
         <v>84</v>
       </c>
+      <c r="B85" t="s">
+        <v>628</v>
+      </c>
       <c r="C85" s="1" t="s">
         <v>243</v>
       </c>
@@ -3733,6 +3758,9 @@
       <c r="A86">
         <v>85</v>
       </c>
+      <c r="B86" t="s">
+        <v>628</v>
+      </c>
       <c r="C86" s="1" t="s">
         <v>251</v>
       </c>
@@ -3744,6 +3772,9 @@
       <c r="A87">
         <v>86</v>
       </c>
+      <c r="B87" t="s">
+        <v>628</v>
+      </c>
       <c r="C87" s="1" t="s">
         <v>254</v>
       </c>
@@ -3758,6 +3789,9 @@
       <c r="A88">
         <v>87</v>
       </c>
+      <c r="B88" t="s">
+        <v>628</v>
+      </c>
       <c r="C88" s="1" t="s">
         <v>249</v>
       </c>
@@ -3772,6 +3806,9 @@
       <c r="A89">
         <v>88</v>
       </c>
+      <c r="B89" t="s">
+        <v>628</v>
+      </c>
       <c r="C89" s="1" t="s">
         <v>259</v>
       </c>
@@ -3786,6 +3823,9 @@
       <c r="A90">
         <v>89</v>
       </c>
+      <c r="B90" t="s">
+        <v>628</v>
+      </c>
       <c r="C90" s="1" t="s">
         <v>262</v>
       </c>
@@ -3800,6 +3840,9 @@
       <c r="A91">
         <v>90</v>
       </c>
+      <c r="B91" t="s">
+        <v>628</v>
+      </c>
       <c r="C91" s="1" t="s">
         <v>263</v>
       </c>
@@ -3814,6 +3857,9 @@
       <c r="A92">
         <v>91</v>
       </c>
+      <c r="B92" t="s">
+        <v>628</v>
+      </c>
       <c r="C92" s="1" t="s">
         <v>266</v>
       </c>
@@ -3828,6 +3874,9 @@
       <c r="A93">
         <v>92</v>
       </c>
+      <c r="B93" t="s">
+        <v>628</v>
+      </c>
       <c r="C93" s="1" t="s">
         <v>269</v>
       </c>
@@ -3842,6 +3891,9 @@
       <c r="A94">
         <v>93</v>
       </c>
+      <c r="B94" t="s">
+        <v>628</v>
+      </c>
       <c r="C94" s="1" t="s">
         <v>274</v>
       </c>
@@ -3856,109 +3908,131 @@
       <c r="A95">
         <v>94</v>
       </c>
+      <c r="B95" t="s">
+        <v>628</v>
+      </c>
       <c r="C95" s="1" t="s">
-        <v>275</v>
+        <v>617</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>276</v>
+        <v>618</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>277</v>
+        <v>619</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
+      <c r="B96" t="s">
+        <v>628</v>
+      </c>
       <c r="C96" s="1" t="s">
-        <v>280</v>
+        <v>614</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>278</v>
+        <v>615</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>279</v>
+        <v>616</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
+      <c r="B97" t="s">
+        <v>628</v>
+      </c>
       <c r="C97" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
+      <c r="B98" t="s">
+        <v>628</v>
+      </c>
       <c r="C98" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
+      <c r="B99" t="s">
+        <v>628</v>
+      </c>
       <c r="C99" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
+      <c r="B100" t="s">
+        <v>628</v>
+      </c>
       <c r="C100" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
+      <c r="B101" t="s">
+        <v>628</v>
+      </c>
       <c r="C101" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
+      <c r="B102" s="2"/>
       <c r="C102" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3966,13 +4040,13 @@
         <v>102</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3980,13 +4054,13 @@
         <v>103</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3994,13 +4068,13 @@
         <v>104</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4008,13 +4082,13 @@
         <v>105</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4022,13 +4096,13 @@
         <v>106</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4036,13 +4110,13 @@
         <v>107</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -4050,13 +4124,13 @@
         <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -4064,13 +4138,13 @@
         <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4078,13 +4152,13 @@
         <v>110</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4092,13 +4166,13 @@
         <v>111</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4106,13 +4180,13 @@
         <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4120,13 +4194,13 @@
         <v>113</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4134,13 +4208,13 @@
         <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4148,13 +4222,13 @@
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4162,13 +4236,13 @@
         <v>116</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4176,13 +4250,13 @@
         <v>117</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4190,13 +4264,13 @@
         <v>118</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4204,13 +4278,13 @@
         <v>119</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4218,13 +4292,13 @@
         <v>120</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4232,13 +4306,13 @@
         <v>121</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4246,13 +4320,13 @@
         <v>122</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4260,13 +4334,13 @@
         <v>123</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4274,13 +4348,13 @@
         <v>124</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4288,13 +4362,13 @@
         <v>125</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4302,13 +4376,13 @@
         <v>126</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4316,13 +4390,13 @@
         <v>127</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4330,13 +4404,13 @@
         <v>128</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4344,13 +4418,13 @@
         <v>129</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4358,13 +4432,13 @@
         <v>130</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4372,13 +4446,13 @@
         <v>131</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4386,13 +4460,13 @@
         <v>132</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4400,13 +4474,13 @@
         <v>133</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4414,13 +4488,13 @@
         <v>134</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4428,13 +4502,13 @@
         <v>135</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4442,13 +4516,13 @@
         <v>136</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4456,13 +4530,13 @@
         <v>137</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4470,13 +4544,13 @@
         <v>138</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4484,13 +4558,13 @@
         <v>139</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4498,13 +4572,13 @@
         <v>140</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4512,13 +4586,13 @@
         <v>141</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4526,13 +4600,13 @@
         <v>142</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4540,13 +4614,13 @@
         <v>143</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4554,13 +4628,13 @@
         <v>144</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4568,13 +4642,13 @@
         <v>145</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4582,13 +4656,13 @@
         <v>146</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4596,13 +4670,13 @@
         <v>147</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4610,13 +4684,13 @@
         <v>148</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4624,13 +4698,13 @@
         <v>149</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4638,13 +4712,13 @@
         <v>150</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4652,13 +4726,13 @@
         <v>151</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4666,13 +4740,13 @@
         <v>152</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4680,13 +4754,13 @@
         <v>153</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4694,13 +4768,13 @@
         <v>154</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4708,13 +4782,13 @@
         <v>155</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4722,13 +4796,13 @@
         <v>156</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4736,13 +4810,13 @@
         <v>157</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4750,13 +4824,13 @@
         <v>158</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4764,13 +4838,13 @@
         <v>159</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4778,13 +4852,13 @@
         <v>160</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4792,13 +4866,13 @@
         <v>161</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4806,13 +4880,13 @@
         <v>162</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4820,13 +4894,13 @@
         <v>163</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4834,13 +4908,13 @@
         <v>164</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4848,13 +4922,13 @@
         <v>165</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4862,13 +4936,13 @@
         <v>166</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4876,13 +4950,13 @@
         <v>167</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4890,13 +4964,13 @@
         <v>168</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4904,13 +4978,13 @@
         <v>169</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4918,13 +4992,13 @@
         <v>170</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4932,13 +5006,13 @@
         <v>171</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4946,13 +5020,13 @@
         <v>172</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4960,13 +5034,13 @@
         <v>173</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4974,13 +5048,13 @@
         <v>174</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4988,13 +5062,13 @@
         <v>175</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5002,13 +5076,13 @@
         <v>176</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5019,7 +5093,7 @@
         <v>246</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>247</v>
@@ -5030,13 +5104,13 @@
         <v>178</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5044,13 +5118,13 @@
         <v>179</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -5058,13 +5132,13 @@
         <v>180</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -5072,13 +5146,13 @@
         <v>181</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5086,13 +5160,13 @@
         <v>182</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5100,13 +5174,13 @@
         <v>183</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5114,13 +5188,13 @@
         <v>184</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5128,13 +5202,13 @@
         <v>185</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5142,13 +5216,13 @@
         <v>186</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5156,13 +5230,13 @@
         <v>187</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5170,13 +5244,13 @@
         <v>188</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5184,13 +5258,13 @@
         <v>189</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5198,13 +5272,13 @@
         <v>190</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5212,13 +5286,13 @@
         <v>191</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5226,13 +5300,13 @@
         <v>192</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5240,13 +5314,13 @@
         <v>193</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -5254,13 +5328,13 @@
         <v>194</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5268,13 +5342,13 @@
         <v>195</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -5282,13 +5356,13 @@
         <v>196</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5296,13 +5370,13 @@
         <v>197</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5310,13 +5384,13 @@
         <v>198</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5324,13 +5398,13 @@
         <v>199</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5338,13 +5412,13 @@
         <v>200</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5352,13 +5426,13 @@
         <v>201</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5366,13 +5440,13 @@
         <v>202</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5380,13 +5454,13 @@
         <v>203</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5394,13 +5468,13 @@
         <v>204</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5408,13 +5482,13 @@
         <v>205</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5422,13 +5496,13 @@
         <v>206</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5436,13 +5510,13 @@
         <v>207</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5450,41 +5524,13 @@
         <v>208</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210">
-        <v>209</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211">
-        <v>210</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>623</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>625</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -5750,372 +5796,366 @@
     <hyperlink ref="E94" r:id="rId258" xr:uid="{2033DE9C-AB68-4337-9666-E036632B48E9}"/>
     <hyperlink ref="D94" r:id="rId259" xr:uid="{BC335142-CEB5-45DC-A6D5-CB1E1226051F}"/>
     <hyperlink ref="C94" r:id="rId260" xr:uid="{373F113B-04B2-431D-8E11-05B90B52D390}"/>
-    <hyperlink ref="C95" r:id="rId261" xr:uid="{E3539E81-DF93-4A39-9945-36CEC9E34CF4}"/>
-    <hyperlink ref="D95" r:id="rId262" xr:uid="{D669F179-1AC6-4E08-96C5-C7BE89D41875}"/>
-    <hyperlink ref="E95" r:id="rId263" xr:uid="{CBC521FB-9833-4D60-918B-F3038613EC49}"/>
-    <hyperlink ref="D96" r:id="rId264" xr:uid="{1487A3FD-94F4-4C63-B36B-1C6236ACCCAA}"/>
-    <hyperlink ref="E96" r:id="rId265" xr:uid="{5F631273-96B3-48BB-A5C6-A8077E8EC752}"/>
-    <hyperlink ref="C96" r:id="rId266" xr:uid="{ADE8BEEA-ABC6-474A-A950-FF38898D34D2}"/>
-    <hyperlink ref="D97" r:id="rId267" xr:uid="{4DD3F6B0-4B1E-451C-9857-7B840584705D}"/>
-    <hyperlink ref="E97" r:id="rId268" xr:uid="{6DA9CE9D-442F-4DC5-BE8C-7745B1745575}"/>
-    <hyperlink ref="C97" r:id="rId269" xr:uid="{E59BA18D-2DA1-4FDF-9C1E-CD6D1A2620C7}"/>
-    <hyperlink ref="D98" r:id="rId270" xr:uid="{5C95BE55-05A0-4BE2-A224-2C4A40579DEE}"/>
-    <hyperlink ref="E98" r:id="rId271" xr:uid="{E2F28665-F304-48EB-AEE8-E289F7A4FC5A}"/>
-    <hyperlink ref="C98" r:id="rId272" xr:uid="{55201C98-C656-4EE7-A35F-CE17F44473C3}"/>
-    <hyperlink ref="C100" r:id="rId273" xr:uid="{79EA69E5-FEAB-4C20-B0DE-70A81655B6D4}"/>
-    <hyperlink ref="D100" r:id="rId274" xr:uid="{ED375E0D-1308-4908-9149-A0315A582320}"/>
-    <hyperlink ref="E100" r:id="rId275" xr:uid="{D46B35C8-21A4-4B52-ABFA-8A94A326F9D7}"/>
-    <hyperlink ref="C101" r:id="rId276" xr:uid="{E7ACECEC-3A28-4599-84B8-59BC02BF4FED}"/>
-    <hyperlink ref="D101" r:id="rId277" xr:uid="{465047FF-1256-4E45-AE8D-E5CEDB95F73F}"/>
-    <hyperlink ref="E101" r:id="rId278" xr:uid="{F30A2FC8-5BF5-487F-A934-EC4AC77FE211}"/>
-    <hyperlink ref="C102" r:id="rId279" xr:uid="{178FA5E3-E6A3-4365-9928-DC4296B031B7}"/>
-    <hyperlink ref="D102" r:id="rId280" xr:uid="{2487C55D-36B0-497C-8E7F-76864E5D2337}"/>
-    <hyperlink ref="E102" r:id="rId281" xr:uid="{9ABF0A5D-385F-4E38-95DF-7739D7794FCD}"/>
-    <hyperlink ref="C103" r:id="rId282" xr:uid="{5D123A8D-D901-4600-9E13-23B4081222A0}"/>
-    <hyperlink ref="D103" r:id="rId283" xr:uid="{B41BE957-8100-409E-8F6C-9FFF07208823}"/>
-    <hyperlink ref="E103" r:id="rId284" xr:uid="{7417B276-5872-4090-A0D9-C56E6230AB29}"/>
-    <hyperlink ref="C104" r:id="rId285" xr:uid="{2AC02C2A-F7B1-4CDE-8106-C0D377FFD10A}"/>
-    <hyperlink ref="D104" r:id="rId286" xr:uid="{CF5FB671-CD80-457E-9A5C-55AC19128002}"/>
-    <hyperlink ref="E104" r:id="rId287" xr:uid="{7EB7712F-F3D4-4CD0-928D-AA08612DA711}"/>
-    <hyperlink ref="C105" r:id="rId288" xr:uid="{3A98A613-5247-4EDD-9ED8-FFB31D28F72C}"/>
-    <hyperlink ref="D105" r:id="rId289" xr:uid="{B0F0B342-1498-46A9-BD50-0660E9657C90}"/>
-    <hyperlink ref="E105" r:id="rId290" xr:uid="{0B67D960-696C-427C-A875-D3B85CFF0762}"/>
-    <hyperlink ref="C106" r:id="rId291" xr:uid="{1DA3041A-7728-4026-B61E-A1AB5F15F5A8}"/>
-    <hyperlink ref="D106" r:id="rId292" xr:uid="{451E6F75-0E8E-49A5-8A5B-87255F93DD33}"/>
-    <hyperlink ref="E106" r:id="rId293" xr:uid="{D49DC68C-742B-425B-881B-A83AF4714EE4}"/>
-    <hyperlink ref="C107" r:id="rId294" xr:uid="{D226CEDC-443D-41F7-AD26-0AAF1BD9DB3F}"/>
-    <hyperlink ref="D107" r:id="rId295" xr:uid="{EF0F660D-62B8-4AA4-A272-57AB44F0E9CF}"/>
-    <hyperlink ref="E107" r:id="rId296" xr:uid="{3F4019C0-9C15-4B90-B9D3-90908DBCF849}"/>
-    <hyperlink ref="C108" r:id="rId297" xr:uid="{8B746AED-6ACC-4850-8828-FB6F0374D303}"/>
-    <hyperlink ref="D108" r:id="rId298" xr:uid="{F9014A66-3EE9-40DC-B87E-5D9054B50E5D}"/>
-    <hyperlink ref="E108" r:id="rId299" xr:uid="{4EE6DB51-0C8B-400C-A838-15E4BD633EE2}"/>
-    <hyperlink ref="C109" r:id="rId300" xr:uid="{FA69422B-0C15-4C8B-B074-46A3869AC7C9}"/>
-    <hyperlink ref="D109" r:id="rId301" xr:uid="{621EC68A-7ACE-45FB-88A3-06F720875DD7}"/>
-    <hyperlink ref="E109" r:id="rId302" xr:uid="{554DED57-0D82-433F-987B-1B34E1214C78}"/>
-    <hyperlink ref="C110" r:id="rId303" xr:uid="{4117E483-CA3B-487C-94D0-D68E8DB43993}"/>
-    <hyperlink ref="D110" r:id="rId304" xr:uid="{8AAA2CF2-8CC2-4067-AAC9-FA2A4EFE32DD}"/>
-    <hyperlink ref="E110" r:id="rId305" xr:uid="{66B74877-14BB-4AD3-8761-E581180779E3}"/>
-    <hyperlink ref="C111" r:id="rId306" xr:uid="{C527C048-13AF-4166-AAC3-24C05E9E601E}"/>
-    <hyperlink ref="D111" r:id="rId307" xr:uid="{2965799F-E19D-4831-A7B4-10AC9AAC4229}"/>
-    <hyperlink ref="E111" r:id="rId308" xr:uid="{44E6383F-DB4B-4F5D-BA87-405239E1E5E0}"/>
-    <hyperlink ref="C112" r:id="rId309" xr:uid="{714BC743-EB75-42ED-AF6E-B8B31923740F}"/>
-    <hyperlink ref="D112" r:id="rId310" xr:uid="{C53CEA57-5AB8-4F8D-BE5E-9B4CB9BD9BF5}"/>
-    <hyperlink ref="E112" r:id="rId311" xr:uid="{B6767105-A075-4865-AAC5-BF568E26C3DC}"/>
-    <hyperlink ref="C113" r:id="rId312" xr:uid="{DA3469AE-90EC-41E3-9216-B1C0BDA33A67}"/>
-    <hyperlink ref="D113" r:id="rId313" xr:uid="{557307AD-C5A9-4652-888D-A94FDF80009E}"/>
-    <hyperlink ref="E113" r:id="rId314" xr:uid="{C3DCCA91-9FBC-47D2-A94E-C1B437125A9A}"/>
-    <hyperlink ref="C114" r:id="rId315" xr:uid="{2906FCEE-6A7F-45B3-8BF5-7B231A0D23DB}"/>
-    <hyperlink ref="D114" r:id="rId316" xr:uid="{CBE1D2EA-6123-4939-A2F6-07C30E28EEE0}"/>
-    <hyperlink ref="E114" r:id="rId317" xr:uid="{31DAEDC2-35C0-48F5-A25B-93D7BF3A7450}"/>
-    <hyperlink ref="C115" r:id="rId318" xr:uid="{9E70ABF8-EABB-4B06-80D0-153AB8E19A7B}"/>
-    <hyperlink ref="D115" r:id="rId319" xr:uid="{327C9817-CBEE-4C9A-AAC6-464A863BEF9D}"/>
-    <hyperlink ref="E115" r:id="rId320" xr:uid="{A96FDAEB-0252-432D-A050-64EE5BE04F6D}"/>
-    <hyperlink ref="C116" r:id="rId321" xr:uid="{A4745FA3-0838-4B0A-8AF1-C0E8A9318E7A}"/>
-    <hyperlink ref="D116" r:id="rId322" xr:uid="{D592EA88-2676-4594-A3F8-755BA2197B17}"/>
-    <hyperlink ref="E116" r:id="rId323" xr:uid="{43298315-6704-4543-B6A3-1D12ED3BD89B}"/>
-    <hyperlink ref="C117" r:id="rId324" xr:uid="{4F507A97-E64C-4FA2-827D-A97B68F6502C}"/>
-    <hyperlink ref="D117" r:id="rId325" xr:uid="{89E85572-0309-4ECD-9E6F-6A8BFBDD0475}"/>
-    <hyperlink ref="E117" r:id="rId326" xr:uid="{6C735EE1-5379-4E04-87DC-61981092F13A}"/>
-    <hyperlink ref="C118" r:id="rId327" xr:uid="{DCB2DDD8-CEA1-4A83-927E-AA880D5F2465}"/>
-    <hyperlink ref="D118" r:id="rId328" xr:uid="{87B4582B-3A51-46CB-A7AA-14A53BEF2877}"/>
-    <hyperlink ref="E118" r:id="rId329" xr:uid="{95F3F337-662F-4DEB-899F-8B106C6AD582}"/>
-    <hyperlink ref="D119" r:id="rId330" xr:uid="{C6E03219-8688-46D5-858A-2C3BB7AC04D7}"/>
-    <hyperlink ref="E119" r:id="rId331" xr:uid="{222C944B-0CA2-4AA1-BFF7-664ED828CA3B}"/>
-    <hyperlink ref="C119" r:id="rId332" xr:uid="{50F33598-73F6-4B9D-8478-4AC6890A025A}"/>
-    <hyperlink ref="D120" r:id="rId333" xr:uid="{4AED68E4-2779-4CB0-B7AE-44AFAECA4499}"/>
-    <hyperlink ref="E120" r:id="rId334" xr:uid="{20510976-5BE1-4F80-89F3-DC95303A5BBF}"/>
-    <hyperlink ref="C120" r:id="rId335" xr:uid="{3842BBC2-0FE4-402C-A871-BFB50EE32BA0}"/>
-    <hyperlink ref="C121" r:id="rId336" xr:uid="{89D31CD8-B8E5-49D6-8FA5-D7A42F6CB540}"/>
-    <hyperlink ref="D121" r:id="rId337" xr:uid="{AC74A6C1-41F5-4315-92E2-A3C7ED59EBBD}"/>
-    <hyperlink ref="E121" r:id="rId338" xr:uid="{B1F093AF-7F7F-460F-A4F0-ADB6490D731B}"/>
-    <hyperlink ref="C122" r:id="rId339" xr:uid="{D4F65573-20F5-43D1-80BF-2795F41D9F57}"/>
-    <hyperlink ref="D122" r:id="rId340" xr:uid="{B88C2559-C22D-41ED-8F15-469DB6777B84}"/>
-    <hyperlink ref="E122" r:id="rId341" xr:uid="{EEA137CE-31F7-415B-94AB-CA2A55462E5C}"/>
-    <hyperlink ref="C123" r:id="rId342" xr:uid="{D997E317-1F11-4A83-B7F1-CF5217F8F4ED}"/>
-    <hyperlink ref="D123" r:id="rId343" xr:uid="{C9088CDA-1F58-4681-9DAD-82F7D0583EE5}"/>
-    <hyperlink ref="E123" r:id="rId344" xr:uid="{830325FC-B5CA-4053-8D5D-6DA5A0E9CEB3}"/>
-    <hyperlink ref="C124" r:id="rId345" xr:uid="{5AC4D217-D8FE-4409-862F-FAA5A86520AC}"/>
-    <hyperlink ref="D124" r:id="rId346" xr:uid="{CE468356-AB38-423F-ACE7-04587D99102E}"/>
-    <hyperlink ref="E124" r:id="rId347" xr:uid="{611001F6-2221-481D-AFA1-35DB4D386424}"/>
-    <hyperlink ref="C125" r:id="rId348" xr:uid="{FCC30E1C-7F83-4581-822A-7F2ACF21B208}"/>
-    <hyperlink ref="D125" r:id="rId349" xr:uid="{3A097561-C99B-452A-B5F9-14E12478CA8E}"/>
-    <hyperlink ref="E125" r:id="rId350" xr:uid="{5847BD3E-972F-4164-8556-AAACBBA355DB}"/>
-    <hyperlink ref="C126" r:id="rId351" xr:uid="{3BCC14C6-3272-4FB5-B30F-233B0FFAA229}"/>
-    <hyperlink ref="D126" r:id="rId352" xr:uid="{D87B0C63-927A-423F-9DEE-FB163765706A}"/>
-    <hyperlink ref="E126" r:id="rId353" xr:uid="{8D18C038-05BE-41FB-9589-349C2DB35EB6}"/>
-    <hyperlink ref="C127" r:id="rId354" xr:uid="{212AE7B7-8417-4613-9B01-457D5FAD32E2}"/>
-    <hyperlink ref="D127" r:id="rId355" xr:uid="{16169750-2789-41D4-92EE-8370C62CF1BA}"/>
-    <hyperlink ref="E127" r:id="rId356" xr:uid="{EF236839-B3F1-4D2A-8793-A6E0A9D52328}"/>
-    <hyperlink ref="C128" r:id="rId357" xr:uid="{13F5A019-E7BD-473A-8BFB-051E885B1146}"/>
-    <hyperlink ref="D128" r:id="rId358" xr:uid="{C06C249C-A9D7-4BAE-AD6C-0ECED61AA088}"/>
-    <hyperlink ref="E128" r:id="rId359" xr:uid="{C2493638-1F36-426C-A65E-9BA0E883C835}"/>
-    <hyperlink ref="C129" r:id="rId360" xr:uid="{7F246417-F2E2-4CEF-ACB8-0C0E87FFBD79}"/>
-    <hyperlink ref="D129" r:id="rId361" xr:uid="{77141049-FDE6-4B29-8926-A7256E4C0505}"/>
-    <hyperlink ref="E129" r:id="rId362" xr:uid="{F98DCA20-9796-418E-B8CA-A3E005647A01}"/>
-    <hyperlink ref="C130" r:id="rId363" xr:uid="{0BA229B0-06A2-4C48-9914-A5374B32A34F}"/>
-    <hyperlink ref="D130" r:id="rId364" xr:uid="{3F506EBE-0BD0-4794-87C1-953206B16CD4}"/>
-    <hyperlink ref="E130" r:id="rId365" xr:uid="{A615BCEB-72DE-43C7-8A07-693C54D3A0C4}"/>
-    <hyperlink ref="C131" r:id="rId366" xr:uid="{07FCC78B-BF39-43FB-A89D-700B9FB2D824}"/>
-    <hyperlink ref="D131" r:id="rId367" xr:uid="{12B43D3A-B1AA-41D0-8A47-1DDC5FBC02CC}"/>
-    <hyperlink ref="E131" r:id="rId368" xr:uid="{E1EB98C2-E2CA-4E94-8439-8B789E3754E7}"/>
-    <hyperlink ref="D132" r:id="rId369" xr:uid="{63468E1D-F523-48BF-8225-D649FBE847EC}"/>
-    <hyperlink ref="E132" r:id="rId370" xr:uid="{4D681694-A038-4227-BC2E-F2651367ACF3}"/>
-    <hyperlink ref="C132" r:id="rId371" xr:uid="{D7ECE862-4574-486D-A9A4-78F8E4FC1681}"/>
-    <hyperlink ref="C133" r:id="rId372" xr:uid="{B156B9CD-29C4-4D78-8EBA-515A4C1B6B5A}"/>
-    <hyperlink ref="D133" r:id="rId373" xr:uid="{DA45D1F5-4AD3-4F4C-8A29-855166DF6940}"/>
-    <hyperlink ref="E133" r:id="rId374" xr:uid="{596A4EF2-4527-401B-A2CE-FA6A6AE241FF}"/>
-    <hyperlink ref="C134" r:id="rId375" xr:uid="{DC92B3C9-52B9-4D63-AC4A-1FE80AD38A7B}"/>
-    <hyperlink ref="D134" r:id="rId376" xr:uid="{6653B8D2-7773-4FD1-8AB6-76B074FA4AAA}"/>
-    <hyperlink ref="E134" r:id="rId377" xr:uid="{58D58C73-9A50-44A9-A0EA-5592206BB72F}"/>
-    <hyperlink ref="C135" r:id="rId378" xr:uid="{CF269375-1231-4422-9D05-86CA9413B1AD}"/>
-    <hyperlink ref="D135" r:id="rId379" xr:uid="{7AF85C45-2D0F-4BF2-8039-612435A7F999}"/>
-    <hyperlink ref="E135" r:id="rId380" xr:uid="{B39AC57D-61C7-4384-92C0-FA4D3C141F31}"/>
-    <hyperlink ref="C136" r:id="rId381" xr:uid="{F5D55CD9-3B76-4FD8-AC67-16192C305D26}"/>
-    <hyperlink ref="D136" r:id="rId382" xr:uid="{48D8B605-74CE-472F-AFDD-08EC6689007C}"/>
-    <hyperlink ref="E136" r:id="rId383" xr:uid="{44FF3624-E323-438F-8CAB-68D1CB08688C}"/>
-    <hyperlink ref="C137" r:id="rId384" xr:uid="{CE592AC5-E5D6-495B-BB1B-85E6B7EE95DA}"/>
-    <hyperlink ref="D137" r:id="rId385" xr:uid="{D0AD0ECF-67E1-4B11-91F5-AA23D31475D4}"/>
-    <hyperlink ref="E137" r:id="rId386" xr:uid="{CA7CD45E-3E5B-4C2E-93A9-84848C1A52F2}"/>
-    <hyperlink ref="C138" r:id="rId387" xr:uid="{971AEABA-C26E-4CD2-B617-7E7AEFA79225}"/>
-    <hyperlink ref="D138" r:id="rId388" xr:uid="{E838D43A-FA34-4E17-A12D-60A467F149C2}"/>
-    <hyperlink ref="E138" r:id="rId389" xr:uid="{31F37E78-12DF-444E-A3FB-EF00403D39D4}"/>
-    <hyperlink ref="C139" r:id="rId390" xr:uid="{7DC70FA2-2641-4F66-B9F8-01F68ED70F02}"/>
-    <hyperlink ref="D139" r:id="rId391" xr:uid="{B963012C-FACA-4A11-B1C4-313CF3F6387F}"/>
-    <hyperlink ref="E139" r:id="rId392" xr:uid="{E1DCAB4B-878B-4C50-97B6-B5A5D2A2FADD}"/>
-    <hyperlink ref="C140" r:id="rId393" xr:uid="{60F58296-9148-4312-9D0C-BF4DE0690B91}"/>
-    <hyperlink ref="D140" r:id="rId394" xr:uid="{8DBCCAC8-BC9E-442F-A475-9F8639697DB9}"/>
-    <hyperlink ref="E140" r:id="rId395" xr:uid="{0B4BC81F-7CB5-41BC-88B0-3B2BBBE80A3F}"/>
-    <hyperlink ref="D141" r:id="rId396" xr:uid="{9A0BB159-B669-435C-9CB1-A2BA4C4091A9}"/>
-    <hyperlink ref="E141" r:id="rId397" xr:uid="{0055782C-E077-4204-8FF9-57BE6F8FED26}"/>
-    <hyperlink ref="C141" r:id="rId398" xr:uid="{FE323C66-30FE-40E0-8F0E-4108D9EC2713}"/>
-    <hyperlink ref="C142" r:id="rId399" xr:uid="{666B5CC7-4AFE-4EE4-93A2-099371C034E3}"/>
-    <hyperlink ref="D142" r:id="rId400" xr:uid="{A9DFF398-3782-4606-A5AD-16EB49874249}"/>
-    <hyperlink ref="E142" r:id="rId401" xr:uid="{CB3B62B3-3706-4AEA-B831-85D12973AAFB}"/>
-    <hyperlink ref="C143" r:id="rId402" xr:uid="{5B3C3EC4-7E86-40AB-980C-956D883C0DE8}"/>
-    <hyperlink ref="D143" r:id="rId403" xr:uid="{E58660DA-18E4-456D-AE6E-157A8C791640}"/>
-    <hyperlink ref="E143" r:id="rId404" xr:uid="{30D38FD6-524A-4260-A893-C02ABC8FD7D8}"/>
-    <hyperlink ref="C144" r:id="rId405" xr:uid="{EAA73046-9047-4BE9-A054-E3310DE63E1A}"/>
-    <hyperlink ref="D144" r:id="rId406" xr:uid="{54E7A160-9887-4A15-A5E4-7E98C3B546B1}"/>
-    <hyperlink ref="E144" r:id="rId407" xr:uid="{5BA4E4AA-D08F-40BB-B211-CD81B18FF87A}"/>
-    <hyperlink ref="C145" r:id="rId408" xr:uid="{E57FE190-B789-4567-B86E-2D8DD5BB470A}"/>
-    <hyperlink ref="D145" r:id="rId409" xr:uid="{303EC3AA-5A58-4C68-97E5-480D5E8B49ED}"/>
-    <hyperlink ref="E145" r:id="rId410" xr:uid="{111A682B-10E9-494F-BA71-FEC4F7FB0BD6}"/>
-    <hyperlink ref="C146" r:id="rId411" xr:uid="{E353A765-41EF-43C2-AB89-89DFAEA7EAB7}"/>
-    <hyperlink ref="D146" r:id="rId412" xr:uid="{6DB31883-29E3-4B37-A5BC-B8A2B95FBC29}"/>
-    <hyperlink ref="E146" r:id="rId413" xr:uid="{FCF11283-83AE-42A7-BB7D-85631FD6E8B9}"/>
-    <hyperlink ref="C147" r:id="rId414" xr:uid="{2CA57331-C3C7-4E12-82CB-C628ECE4CCAB}"/>
-    <hyperlink ref="D147" r:id="rId415" xr:uid="{B5E1FE84-C98A-420D-837D-C3DCBB95E91F}"/>
-    <hyperlink ref="E147" r:id="rId416" xr:uid="{20932CE8-F8AE-4689-9CD7-3D080869A55D}"/>
-    <hyperlink ref="C148" r:id="rId417" xr:uid="{7618A490-B688-42C9-94E0-4F8540FF40DB}"/>
-    <hyperlink ref="D148" r:id="rId418" xr:uid="{668BB9C5-109F-4A7E-868C-D2732EFA34A2}"/>
-    <hyperlink ref="E148" r:id="rId419" xr:uid="{0F731946-786D-4814-BAE4-8D0C99005D78}"/>
-    <hyperlink ref="C149" r:id="rId420" xr:uid="{51F53306-B34E-472A-B470-69B8029C9ED4}"/>
-    <hyperlink ref="D149" r:id="rId421" xr:uid="{F2FEECB1-F3BC-4C78-B544-613C7FF5E436}"/>
-    <hyperlink ref="E149" r:id="rId422" xr:uid="{343909DC-77D4-4FBB-BE02-DCD4EC0C20EB}"/>
-    <hyperlink ref="C150" r:id="rId423" xr:uid="{F187FD4D-E765-4937-9701-2C58603180AE}"/>
-    <hyperlink ref="D150" r:id="rId424" xr:uid="{31FB4D76-B008-46DB-9637-691B1894CE21}"/>
-    <hyperlink ref="E150" r:id="rId425" xr:uid="{03572D9E-807D-4918-B128-29411ACBB625}"/>
-    <hyperlink ref="C151" r:id="rId426" xr:uid="{5130DE5E-46EF-4B05-8FE0-179C2E7E6948}"/>
-    <hyperlink ref="D151" r:id="rId427" xr:uid="{97742F59-5F59-4D68-996E-0A272575FADC}"/>
-    <hyperlink ref="E151" r:id="rId428" xr:uid="{2355B201-6EF9-4A6A-A9B9-BF166EC28606}"/>
-    <hyperlink ref="C152" r:id="rId429" xr:uid="{407F15B9-9D77-4AFB-B5E8-1B163C7E370E}"/>
-    <hyperlink ref="D152" r:id="rId430" xr:uid="{7A5EB5DE-BDC8-4E93-9761-A6603D00EFAD}"/>
-    <hyperlink ref="E152" r:id="rId431" xr:uid="{097CE107-4BA7-4CF3-996A-093477F670F6}"/>
-    <hyperlink ref="D153" r:id="rId432" xr:uid="{51B6FCED-FA56-433D-BA3D-445C0F2FE651}"/>
-    <hyperlink ref="E153" r:id="rId433" xr:uid="{26C3E259-1ACD-4F3A-B70D-194C131947DB}"/>
-    <hyperlink ref="C153" r:id="rId434" xr:uid="{3A114C26-8E8C-45B9-94BD-FCD3CAA9597E}"/>
-    <hyperlink ref="C154" r:id="rId435" xr:uid="{9AA9391F-DE63-4135-A127-DF0F47F7D8C7}"/>
-    <hyperlink ref="D154" r:id="rId436" xr:uid="{2BF42871-0750-440A-A243-619A1C20CC7F}"/>
-    <hyperlink ref="E154" r:id="rId437" xr:uid="{D39D1674-E469-410B-9639-99835CA9A908}"/>
-    <hyperlink ref="C155" r:id="rId438" xr:uid="{5F3DC677-1855-4283-B201-795E598B8917}"/>
-    <hyperlink ref="D155" r:id="rId439" xr:uid="{97F71AB0-0556-481D-B3A2-984C5AB5ED3A}"/>
-    <hyperlink ref="E155" r:id="rId440" xr:uid="{F4091531-5EEE-42BF-9549-D3422C21479A}"/>
-    <hyperlink ref="C156" r:id="rId441" xr:uid="{09680C2A-D8C5-41B4-9F07-96FF1792918C}"/>
-    <hyperlink ref="D156" r:id="rId442" xr:uid="{B9850E60-1546-4D20-8BF8-E8A5C91504C9}"/>
-    <hyperlink ref="E156" r:id="rId443" xr:uid="{CB7D6C00-6A72-4633-A0C4-CA7AD5F7CA43}"/>
-    <hyperlink ref="C157" r:id="rId444" xr:uid="{80024236-A643-48BC-A603-88E4C61F39E9}"/>
-    <hyperlink ref="D157" r:id="rId445" xr:uid="{120C8743-AA48-4C9A-AE55-5610BE126DC3}"/>
-    <hyperlink ref="E157" r:id="rId446" xr:uid="{2D5BB430-5FE3-453B-A9D2-87D25EF175BD}"/>
-    <hyperlink ref="C158" r:id="rId447" xr:uid="{4DFB4F67-145A-44E0-BE4E-70236393A673}"/>
-    <hyperlink ref="D158" r:id="rId448" xr:uid="{63643BC2-FC62-42D6-82C6-75379B5F7031}"/>
-    <hyperlink ref="E158" r:id="rId449" xr:uid="{6CF4B868-96BA-46BA-B87F-853852F4531D}"/>
-    <hyperlink ref="C159" r:id="rId450" xr:uid="{352410C9-FE4B-4A2C-BC1F-750169232690}"/>
-    <hyperlink ref="D159" r:id="rId451" xr:uid="{AFE88A43-637E-4B75-B37A-1F57451F4619}"/>
-    <hyperlink ref="E159" r:id="rId452" xr:uid="{7535847A-C949-43A9-93A4-F0EC6DDF68DA}"/>
-    <hyperlink ref="C160" r:id="rId453" xr:uid="{4C1038DE-1D54-48E4-8E66-F691E40DCC63}"/>
-    <hyperlink ref="D160" r:id="rId454" xr:uid="{41172669-0845-43AD-9650-8B8A62925666}"/>
-    <hyperlink ref="E160" r:id="rId455" xr:uid="{B16881C8-92C0-4AA1-B859-DBDCB15AD570}"/>
-    <hyperlink ref="C161" r:id="rId456" xr:uid="{39A2F065-2C25-448A-8687-9F2149D01184}"/>
-    <hyperlink ref="D161" r:id="rId457" xr:uid="{F2ED0C3A-0135-4147-AEFF-DC4B8ED0D685}"/>
-    <hyperlink ref="E161" r:id="rId458" xr:uid="{8DF3594C-0BF9-448B-A503-24794FCECEA3}"/>
-    <hyperlink ref="D162" r:id="rId459" xr:uid="{2D27BDFB-D4B5-44B9-965C-A93682BCB150}"/>
-    <hyperlink ref="E162" r:id="rId460" xr:uid="{744A7EC5-AEB8-42E3-A556-E4E16C245E49}"/>
-    <hyperlink ref="C162" r:id="rId461" xr:uid="{1A5BE688-8DAF-46EE-BE55-B56FA387D60A}"/>
-    <hyperlink ref="C163" r:id="rId462" xr:uid="{A2A8969B-E67C-4C42-9F40-97418205870F}"/>
-    <hyperlink ref="D163" r:id="rId463" xr:uid="{8C15BC14-EB1D-4AFA-82A9-D7F5FEB92B34}"/>
-    <hyperlink ref="E163" r:id="rId464" xr:uid="{C1AF09A0-75AC-415B-AEAA-FFE6CDF5282B}"/>
-    <hyperlink ref="C164" r:id="rId465" xr:uid="{97A7FD74-2B85-4FD7-96FD-C28091A20A4D}"/>
-    <hyperlink ref="D164" r:id="rId466" xr:uid="{8C7ACE0C-84B0-4967-A6EA-73EBBBCA6E3A}"/>
-    <hyperlink ref="E164" r:id="rId467" xr:uid="{63C7876B-76A9-4A33-B78B-52C0CA2D8D5E}"/>
-    <hyperlink ref="C165" r:id="rId468" xr:uid="{06B4DEBF-7C8E-4884-91BE-A793EE0F62CC}"/>
-    <hyperlink ref="D165" r:id="rId469" xr:uid="{A9147945-5306-4AE5-BE85-C90C7FC7EC3C}"/>
-    <hyperlink ref="E165" r:id="rId470" xr:uid="{77243768-5B39-4BB1-BA96-960A09265D09}"/>
-    <hyperlink ref="D166" r:id="rId471" xr:uid="{0D2C4551-5A3A-4398-A3D2-99FB0401A7D1}"/>
-    <hyperlink ref="E166" r:id="rId472" xr:uid="{38A6A660-830B-4694-A398-A9DE1011AC6B}"/>
-    <hyperlink ref="C166" r:id="rId473" xr:uid="{5228C198-AF2C-40F8-B2F5-057085C54F0D}"/>
-    <hyperlink ref="C167" r:id="rId474" xr:uid="{A08507FD-CA4F-44FD-80EA-F0484A51F904}"/>
-    <hyperlink ref="D167" r:id="rId475" xr:uid="{F9694B45-4A2C-4F66-8EE4-DA8EE40951ED}"/>
-    <hyperlink ref="E167" r:id="rId476" xr:uid="{C3119FB8-069B-4D3F-B5C3-5883D3A505F1}"/>
-    <hyperlink ref="C168" r:id="rId477" xr:uid="{AA2D388E-48CF-41C9-B888-4F64BFF2ACC5}"/>
-    <hyperlink ref="D168" r:id="rId478" xr:uid="{136A9ACA-B873-408C-877B-B88BEDEE02DE}"/>
-    <hyperlink ref="E168" r:id="rId479" xr:uid="{45143C2B-0CE5-460D-8C8C-7BDD7391EC20}"/>
-    <hyperlink ref="C169" r:id="rId480" xr:uid="{412AABCD-D11B-4C1F-BAE3-8E9B5314FEFE}"/>
-    <hyperlink ref="D169" r:id="rId481" xr:uid="{52143DB4-9220-420E-9325-C79A91D3E77F}"/>
-    <hyperlink ref="E169" r:id="rId482" xr:uid="{EBD5079E-6759-45C1-A040-15A1D7EFA833}"/>
-    <hyperlink ref="C170" r:id="rId483" xr:uid="{D9EDA746-00FA-479B-BBF8-E6EA24906B94}"/>
-    <hyperlink ref="D170" r:id="rId484" xr:uid="{F2F02B4C-A61F-48DB-B4B9-B590F1EAE1A5}"/>
-    <hyperlink ref="E170" r:id="rId485" xr:uid="{4EF3DEB5-F631-42E5-BF23-8FD5BD7C5726}"/>
-    <hyperlink ref="C171" r:id="rId486" xr:uid="{C7AC3295-F2D7-4B73-81FE-CE9DD8908E72}"/>
-    <hyperlink ref="D171" r:id="rId487" xr:uid="{13A8A69F-88CE-42AE-A904-E26015719290}"/>
-    <hyperlink ref="E171" r:id="rId488" xr:uid="{69E9CB21-248F-4A60-986D-523E9D222CCD}"/>
-    <hyperlink ref="C172" r:id="rId489" xr:uid="{7627DCB7-8878-43A8-B6E9-AA0B9A8AA69D}"/>
-    <hyperlink ref="D172" r:id="rId490" xr:uid="{FCCBB0CF-B9DD-4759-BBA3-76BD72CDE47E}"/>
-    <hyperlink ref="E172" r:id="rId491" xr:uid="{3E811DA2-3C40-4364-9266-6773CDEE5611}"/>
-    <hyperlink ref="C173" r:id="rId492" xr:uid="{FC27C7F6-56D3-4353-B218-AEDBD69411BE}"/>
-    <hyperlink ref="D173" r:id="rId493" xr:uid="{1FAEEA19-C0F2-4B64-AB53-5CE1FCFD3EED}"/>
-    <hyperlink ref="E173" r:id="rId494" xr:uid="{9AFEB9F6-C42C-4F69-BAB9-0F96228BAB75}"/>
-    <hyperlink ref="C174" r:id="rId495" xr:uid="{782E6140-94C3-407F-BEAF-9C0D976620EB}"/>
-    <hyperlink ref="D174" r:id="rId496" xr:uid="{B6A4BB4A-CEE1-4126-85FD-8A0A92A86F6C}"/>
-    <hyperlink ref="E174" r:id="rId497" xr:uid="{4DE847BB-899E-400F-B0A1-5368BD326435}"/>
-    <hyperlink ref="C175" r:id="rId498" xr:uid="{550B60D7-37BE-42DF-A0A6-234EE2ABEC88}"/>
-    <hyperlink ref="D175" r:id="rId499" xr:uid="{FE54EAA5-5BCB-4AE8-B0F0-DF219D75D2FA}"/>
-    <hyperlink ref="E175" r:id="rId500" xr:uid="{5F404BDE-7004-4B15-8063-6FFDD0232C10}"/>
-    <hyperlink ref="D176" r:id="rId501" xr:uid="{04847EC6-CA8E-40B5-A255-4AA69821E9CD}"/>
-    <hyperlink ref="E176" r:id="rId502" xr:uid="{C5321455-60AF-4B1F-B2EB-9C48ABE6CF88}"/>
-    <hyperlink ref="C176" r:id="rId503" xr:uid="{F487FA1F-6345-4747-9B2D-E8B2F3CA8F64}"/>
-    <hyperlink ref="C177" r:id="rId504" xr:uid="{0BB76D84-05E9-403F-B67C-C3BFFCCC1DE9}"/>
-    <hyperlink ref="D177" r:id="rId505" xr:uid="{E68DE772-C262-43D4-BAB1-57B7508710F5}"/>
-    <hyperlink ref="E177" r:id="rId506" xr:uid="{E2FD5107-217F-4912-8F1C-CBCA0456D0B1}"/>
-    <hyperlink ref="C178" r:id="rId507" xr:uid="{0709A472-9980-4F85-A449-8A5D6EABD5F4}"/>
-    <hyperlink ref="D178" r:id="rId508" xr:uid="{31C86E75-E56D-4C5A-965A-002F4B567CEA}"/>
-    <hyperlink ref="E178" r:id="rId509" xr:uid="{A44C8FE0-0122-4430-BB7B-95FC5AC20FD1}"/>
-    <hyperlink ref="C179" r:id="rId510" xr:uid="{6CA3E827-405F-40BE-9BA0-7F75BE64C3EF}"/>
-    <hyperlink ref="D179" r:id="rId511" xr:uid="{1AB16091-69AE-4105-9BA6-B775B46361F8}"/>
-    <hyperlink ref="E179" r:id="rId512" xr:uid="{2B7A126E-8D1B-4E8F-93A6-C98453F4B0CD}"/>
-    <hyperlink ref="C180" r:id="rId513" xr:uid="{FF9DC8D1-E300-4D00-8478-B4C4465463B0}"/>
-    <hyperlink ref="D180" r:id="rId514" xr:uid="{C7FB4928-100E-4F31-AA8B-9BB5386BD6E2}"/>
-    <hyperlink ref="E180" r:id="rId515" xr:uid="{33E88EF2-069C-4A8A-A4B9-407D561D9FA7}"/>
-    <hyperlink ref="C181" r:id="rId516" xr:uid="{AD27F6F9-722F-4772-BAD3-292259E599AE}"/>
-    <hyperlink ref="D181" r:id="rId517" xr:uid="{9855AD87-CCE8-4B4A-9D90-654E9CB9A884}"/>
-    <hyperlink ref="E181" r:id="rId518" xr:uid="{DABA9FDA-64E2-49EB-A86C-6A285B8ED457}"/>
-    <hyperlink ref="C182" r:id="rId519" xr:uid="{08DC194C-ADC7-4BD9-B1FA-D02B1EB30413}"/>
-    <hyperlink ref="D182" r:id="rId520" xr:uid="{BDCC0E77-3EA0-4F00-B40F-EB3744C4B10A}"/>
-    <hyperlink ref="E182" r:id="rId521" xr:uid="{0C11EA0B-B2D0-438E-81C0-C400F6D0799A}"/>
-    <hyperlink ref="C183" r:id="rId522" xr:uid="{13991465-B6B8-432B-B460-78ABB1DED868}"/>
-    <hyperlink ref="D183" r:id="rId523" xr:uid="{A036A9F5-033D-4A23-B1E3-B321FB1A1D5C}"/>
-    <hyperlink ref="E183" r:id="rId524" xr:uid="{D1FD862C-B5D6-4B13-931B-57B7FFF1059A}"/>
-    <hyperlink ref="C184" r:id="rId525" xr:uid="{5217B7E5-50F7-4581-9109-F6A8BC875186}"/>
-    <hyperlink ref="D184" r:id="rId526" xr:uid="{C3F790CF-A478-40B7-99F6-7D2667CBC146}"/>
-    <hyperlink ref="E184" r:id="rId527" xr:uid="{A5F80E79-506C-4A15-AACD-68F53D61E373}"/>
-    <hyperlink ref="C185" r:id="rId528" xr:uid="{62E029C0-61D3-4187-A49A-6F8E847B07E9}"/>
-    <hyperlink ref="D185" r:id="rId529" xr:uid="{682FAA6B-7ADD-4D0B-9D48-124102D3B8C4}"/>
-    <hyperlink ref="E185" r:id="rId530" xr:uid="{CB64775F-93CB-4F3C-A7B2-61AA1EEC9FF4}"/>
-    <hyperlink ref="D186" r:id="rId531" xr:uid="{33DB2910-4B9B-4EBD-94DB-9D1D8BA1A60A}"/>
-    <hyperlink ref="E186" r:id="rId532" xr:uid="{D816F0E8-5CA4-4FBA-A574-65EB5C502159}"/>
-    <hyperlink ref="C186" r:id="rId533" xr:uid="{7BED455F-4DC7-4B45-AD26-E1286840DEBE}"/>
-    <hyperlink ref="C187" r:id="rId534" xr:uid="{B17E7A06-B7A3-43DE-959C-80217F4C7404}"/>
-    <hyperlink ref="D187" r:id="rId535" xr:uid="{108A2D11-51B8-4F46-B0AE-357FA3F6BDB6}"/>
-    <hyperlink ref="E187" r:id="rId536" xr:uid="{16666982-1A83-4A62-BFC7-C4F40E6C916E}"/>
-    <hyperlink ref="C188" r:id="rId537" xr:uid="{053DBA08-46A7-4A97-9457-F0E304824F8E}"/>
-    <hyperlink ref="D188" r:id="rId538" xr:uid="{DB4ECA15-195B-4A54-858F-239BA708B125}"/>
-    <hyperlink ref="E188" r:id="rId539" xr:uid="{17CC691E-0C7E-443C-B3E1-54C8BFC12D95}"/>
-    <hyperlink ref="C189" r:id="rId540" xr:uid="{488BAF16-AD49-4FAE-8E4C-CE7962082CBA}"/>
-    <hyperlink ref="D189" r:id="rId541" xr:uid="{0B038405-DDEA-461D-994B-7F271E9120F4}"/>
-    <hyperlink ref="E189" r:id="rId542" xr:uid="{7BACCCB4-5CF4-4224-9201-E647233DE274}"/>
-    <hyperlink ref="C190" r:id="rId543" xr:uid="{E9108E47-563C-4F4D-8B1F-CB863619C501}"/>
-    <hyperlink ref="D190" r:id="rId544" xr:uid="{ECB18330-35A1-421E-8B98-A38AB1F12F4B}"/>
-    <hyperlink ref="E190" r:id="rId545" xr:uid="{594B3616-5B4C-4902-90E8-B56CF4ADD901}"/>
-    <hyperlink ref="C191" r:id="rId546" xr:uid="{BEC6DA00-205E-4FA8-BF78-644278A12620}"/>
-    <hyperlink ref="D191" r:id="rId547" xr:uid="{66E4959D-D2E5-40E0-9A50-3E9722C83879}"/>
-    <hyperlink ref="E191" r:id="rId548" xr:uid="{165E3072-0F8C-4D07-A8EE-AFB2E92D10D0}"/>
-    <hyperlink ref="C192" r:id="rId549" xr:uid="{8BDFFA66-526B-49E6-A9EF-74BACEF2FC3A}"/>
-    <hyperlink ref="D192" r:id="rId550" xr:uid="{23452AE3-198E-4555-8556-92D1EB9C8F2F}"/>
-    <hyperlink ref="E192" r:id="rId551" xr:uid="{1C8BB96E-E2D2-41A2-B51E-CA1C94882C45}"/>
-    <hyperlink ref="C193" r:id="rId552" xr:uid="{78499224-1133-4CA4-8141-97A18D48B873}"/>
-    <hyperlink ref="D193" r:id="rId553" xr:uid="{B9B02DD2-D017-4DBC-9327-5DF3E8B353CB}"/>
-    <hyperlink ref="E193" r:id="rId554" xr:uid="{4CDCE363-4F15-4C8E-88A0-16B4ACE31706}"/>
-    <hyperlink ref="D194" r:id="rId555" xr:uid="{9672DF3D-1B42-4B06-BE7E-8C371290DDD8}"/>
-    <hyperlink ref="E194" r:id="rId556" xr:uid="{A6A6609E-1ACE-4AE1-8630-67EC2A09BB1B}"/>
-    <hyperlink ref="C194" r:id="rId557" xr:uid="{2945D925-89ED-4A50-9C8A-33FAE3D9B663}"/>
-    <hyperlink ref="C195" r:id="rId558" xr:uid="{B2232121-8FC5-4AFB-B4A5-EAFCA6F8BF55}"/>
-    <hyperlink ref="D195" r:id="rId559" xr:uid="{BDB9895C-3A01-437E-B535-262F78163F79}"/>
-    <hyperlink ref="E195" r:id="rId560" xr:uid="{7E8CB580-3C77-4108-A7BB-241E5DD2F8F8}"/>
-    <hyperlink ref="C196" r:id="rId561" xr:uid="{0E762398-C5ED-49DE-9BD7-D01671B4E18A}"/>
-    <hyperlink ref="D196" r:id="rId562" xr:uid="{7FC49659-FA8F-434A-B4B6-95508B1B4D35}"/>
-    <hyperlink ref="E196" r:id="rId563" xr:uid="{5FD4642D-66C0-4BCC-9C59-E55B95CFBFBB}"/>
-    <hyperlink ref="C197" r:id="rId564" xr:uid="{63BBE702-55C8-4458-8A67-C5591C5F9247}"/>
-    <hyperlink ref="D197" r:id="rId565" xr:uid="{A666B7EF-0CBD-4183-BF04-FD5B6DDCF6FD}"/>
-    <hyperlink ref="D99" r:id="rId566" xr:uid="{BB5402C0-11CF-4FB7-9D11-E4E06DA8E09D}"/>
-    <hyperlink ref="C99" r:id="rId567" xr:uid="{5098A259-C902-4545-A7E1-E636AB33D5F8}"/>
-    <hyperlink ref="D86" r:id="rId568" display="https://www.camara.leg.br/internet/sitaqweb/TextoHTML.asp?etapa=11&amp;tpReuniaoEvento=AP%20c/%20Convidado&amp;dtReuniao=15/08/2017&amp;hrInicio=14:50:00&amp;hrFim=17:12:00&amp;origemDiscurso=&amp;nmLocal=Plen%C3%A1rio%20Principal%20-%20CD&amp;nuSessao=1047/17&amp;nuQuarto=0&amp;nuOrador=0&amp;nuInsercao=0&amp;dtHorarioQuarto=14:50&amp;sgFaseSessao=&amp;Data=15/08/2017&amp;txApelido=&amp;txFaseSessao=&amp;txTipoSessao=Permanente&amp;dtHoraQuarto=14:50&amp;txEtapa=" xr:uid="{885EDDC5-59F7-4E1C-AF16-381A4A38D774}"/>
-    <hyperlink ref="C86" r:id="rId569" xr:uid="{4A17DC70-EC44-4004-B071-6F5D899C8CA5}"/>
-    <hyperlink ref="D71" r:id="rId570" xr:uid="{D677B959-EB3C-4DDB-8AEF-E8EAE6D6D45E}"/>
-    <hyperlink ref="C71" r:id="rId571" xr:uid="{0AD8437A-2704-40CD-866A-26901C1B53CE}"/>
-    <hyperlink ref="D63" r:id="rId572" xr:uid="{5F59921F-E727-4A1F-AE6F-37476A2F81C2}"/>
-    <hyperlink ref="C63" r:id="rId573" xr:uid="{4B817215-AB66-422A-B2EE-745DCCE2715E}"/>
-    <hyperlink ref="C62" r:id="rId574" xr:uid="{2DA64800-7A72-4482-919D-DFF1D13D4B55}"/>
-    <hyperlink ref="D62" r:id="rId575" xr:uid="{E8EC2437-F030-4E8C-B6AC-917AA71D6D2D}"/>
-    <hyperlink ref="D40" r:id="rId576" xr:uid="{6C41F5BF-C09E-47D4-A816-D0E540BD6149}"/>
-    <hyperlink ref="C40" r:id="rId577" xr:uid="{CBA2CB5F-E42B-4632-83EE-22826ADE1E04}"/>
-    <hyperlink ref="E197" r:id="rId578" xr:uid="{136FF705-8DCE-4116-BE70-5F1542A088B0}"/>
-    <hyperlink ref="C198" r:id="rId579" xr:uid="{3FB904D1-0936-422F-96AB-F3B96921D779}"/>
-    <hyperlink ref="D198" r:id="rId580" xr:uid="{7A54B018-01DB-4819-9FD1-68863145C0A1}"/>
-    <hyperlink ref="E198" r:id="rId581" xr:uid="{E3C9E074-5A18-4A4E-8CA3-EEB4F330DFC6}"/>
-    <hyperlink ref="C199" r:id="rId582" xr:uid="{E2D42ECE-DCF2-4092-B7EF-C717EECA06D7}"/>
-    <hyperlink ref="D199" r:id="rId583" xr:uid="{D3B0D91F-A5F5-489B-B4BF-5B6ADA49D078}"/>
-    <hyperlink ref="E199" r:id="rId584" xr:uid="{9E3CF267-2270-4A5E-BF99-A49458146C5C}"/>
-    <hyperlink ref="C200" r:id="rId585" xr:uid="{39D382AA-57C1-42F8-ABF7-11A7F0B35567}"/>
-    <hyperlink ref="D200" r:id="rId586" xr:uid="{8CE8A2BD-98A2-45D9-B373-7C90E69ADB93}"/>
-    <hyperlink ref="E200" r:id="rId587" xr:uid="{DE229DE6-DE64-42DD-97A1-D38A12923FD3}"/>
-    <hyperlink ref="C201" r:id="rId588" xr:uid="{189D0765-1C92-4FC1-A376-28B52EA2BFAF}"/>
-    <hyperlink ref="D201" r:id="rId589" xr:uid="{2532C84C-8DB5-4D9F-8FFB-F09727EC3D64}"/>
-    <hyperlink ref="E201" r:id="rId590" xr:uid="{A9C00FED-2E5B-4151-A8D6-2CBF429036A5}"/>
-    <hyperlink ref="C202" r:id="rId591" xr:uid="{0FB758F3-8CEC-44F8-AB0B-FB5749251F72}"/>
-    <hyperlink ref="D202" r:id="rId592" xr:uid="{14790960-D653-4274-8C1A-87D26826D0D0}"/>
-    <hyperlink ref="E202" r:id="rId593" xr:uid="{669AE71B-0710-4E47-9B20-28C6E0D2A24C}"/>
-    <hyperlink ref="C203" r:id="rId594" xr:uid="{6C1C977A-8104-4C5D-BED7-C833FD88FC10}"/>
-    <hyperlink ref="D203" r:id="rId595" xr:uid="{FA52D527-723E-449E-AE77-53A711E8B5F4}"/>
-    <hyperlink ref="E203" r:id="rId596" xr:uid="{7D40609C-37B6-4DA5-86FD-A779CCE9CF33}"/>
-    <hyperlink ref="D204" r:id="rId597" xr:uid="{E1F2A5BF-32A9-48D5-81EE-19ABF3643DD2}"/>
-    <hyperlink ref="E204" r:id="rId598" xr:uid="{E561AB7E-F883-4B46-9BD4-A1A7658BB442}"/>
-    <hyperlink ref="C204" r:id="rId599" xr:uid="{0B823933-67DE-41F8-B9F5-D78FB031387C}"/>
-    <hyperlink ref="C205" r:id="rId600" xr:uid="{26F9A583-2496-4B17-A929-300CBDA2E24D}"/>
-    <hyperlink ref="D205" r:id="rId601" xr:uid="{6719EDC2-583C-49D3-9ECA-9AAEAB5A1AF8}"/>
-    <hyperlink ref="E205" r:id="rId602" xr:uid="{3243DF7A-EE24-42C4-9051-EF34793BE812}"/>
-    <hyperlink ref="C206" r:id="rId603" xr:uid="{4C45050E-CAB2-4E91-876A-26ACF94DB8B2}"/>
-    <hyperlink ref="D206" r:id="rId604" xr:uid="{4FE2A5B0-C928-4394-8042-D3AA021DA4D8}"/>
-    <hyperlink ref="E206" r:id="rId605" xr:uid="{CAB1117F-895B-408D-BFB0-CC8642447B67}"/>
-    <hyperlink ref="C207" r:id="rId606" xr:uid="{3497FE2B-F080-4F0F-9454-A2F8E2BCEA79}"/>
-    <hyperlink ref="D207" r:id="rId607" xr:uid="{C1B80CC4-8153-4B20-A3F2-B283168811C5}"/>
-    <hyperlink ref="E207" r:id="rId608" xr:uid="{BF0434BE-354E-4789-9E21-F298661908C9}"/>
-    <hyperlink ref="C208" r:id="rId609" xr:uid="{E432FEE7-0CE3-4671-A6DE-A89067FE71F8}"/>
-    <hyperlink ref="D208" r:id="rId610" xr:uid="{9B118C1B-E5E7-4F47-BFA5-206491EA6ED8}"/>
-    <hyperlink ref="E208" r:id="rId611" xr:uid="{9EA9596A-CB3D-4B30-8E07-CA8A3FF7C508}"/>
-    <hyperlink ref="C209" r:id="rId612" xr:uid="{46C6222B-B670-40C3-A605-FABE1731989A}"/>
-    <hyperlink ref="D209" r:id="rId613" xr:uid="{C653707F-D543-43CC-A01D-24A54A6A319B}"/>
-    <hyperlink ref="E209" r:id="rId614" xr:uid="{60116EA4-2834-4C7A-B4DB-1CE223CB90BB}"/>
-    <hyperlink ref="C210" r:id="rId615" xr:uid="{20EC698E-A69F-497B-8D14-1C5CA444BC21}"/>
-    <hyperlink ref="D210" r:id="rId616" xr:uid="{AFAB7C9A-C544-47BD-8645-5C31CE7C5CF3}"/>
-    <hyperlink ref="E210" r:id="rId617" xr:uid="{F53AF2AB-0CE9-45A6-B905-24C7FEEA3E52}"/>
-    <hyperlink ref="C211" r:id="rId618" xr:uid="{30CD9287-A385-456E-9D5E-59944E3156E1}"/>
-    <hyperlink ref="D211" r:id="rId619" xr:uid="{C9FDF5BB-9B0E-442F-AE18-EBCAF9FA12BA}"/>
-    <hyperlink ref="E211" r:id="rId620" xr:uid="{E3661C98-D989-4879-A8FC-B6166662C8D7}"/>
-    <hyperlink ref="C55" r:id="rId621" xr:uid="{2102EDB4-6981-4633-9FD3-E647448181FC}"/>
-    <hyperlink ref="D55" r:id="rId622" xr:uid="{0DB9D726-23FB-4B78-94AC-DFD7B21AB5AE}"/>
-    <hyperlink ref="E55" r:id="rId623" xr:uid="{BF7B36EC-2642-4F9B-A942-FC7DA39117FB}"/>
+    <hyperlink ref="D97" r:id="rId261" xr:uid="{4DD3F6B0-4B1E-451C-9857-7B840584705D}"/>
+    <hyperlink ref="E97" r:id="rId262" xr:uid="{6DA9CE9D-442F-4DC5-BE8C-7745B1745575}"/>
+    <hyperlink ref="C97" r:id="rId263" xr:uid="{E59BA18D-2DA1-4FDF-9C1E-CD6D1A2620C7}"/>
+    <hyperlink ref="D98" r:id="rId264" xr:uid="{5C95BE55-05A0-4BE2-A224-2C4A40579DEE}"/>
+    <hyperlink ref="E98" r:id="rId265" xr:uid="{E2F28665-F304-48EB-AEE8-E289F7A4FC5A}"/>
+    <hyperlink ref="C98" r:id="rId266" xr:uid="{55201C98-C656-4EE7-A35F-CE17F44473C3}"/>
+    <hyperlink ref="C100" r:id="rId267" xr:uid="{79EA69E5-FEAB-4C20-B0DE-70A81655B6D4}"/>
+    <hyperlink ref="D100" r:id="rId268" xr:uid="{ED375E0D-1308-4908-9149-A0315A582320}"/>
+    <hyperlink ref="E100" r:id="rId269" xr:uid="{D46B35C8-21A4-4B52-ABFA-8A94A326F9D7}"/>
+    <hyperlink ref="C101" r:id="rId270" xr:uid="{E7ACECEC-3A28-4599-84B8-59BC02BF4FED}"/>
+    <hyperlink ref="D101" r:id="rId271" xr:uid="{465047FF-1256-4E45-AE8D-E5CEDB95F73F}"/>
+    <hyperlink ref="E101" r:id="rId272" xr:uid="{F30A2FC8-5BF5-487F-A934-EC4AC77FE211}"/>
+    <hyperlink ref="C102" r:id="rId273" xr:uid="{178FA5E3-E6A3-4365-9928-DC4296B031B7}"/>
+    <hyperlink ref="D102" r:id="rId274" xr:uid="{2487C55D-36B0-497C-8E7F-76864E5D2337}"/>
+    <hyperlink ref="E102" r:id="rId275" xr:uid="{9ABF0A5D-385F-4E38-95DF-7739D7794FCD}"/>
+    <hyperlink ref="C103" r:id="rId276" xr:uid="{5D123A8D-D901-4600-9E13-23B4081222A0}"/>
+    <hyperlink ref="D103" r:id="rId277" xr:uid="{B41BE957-8100-409E-8F6C-9FFF07208823}"/>
+    <hyperlink ref="E103" r:id="rId278" xr:uid="{7417B276-5872-4090-A0D9-C56E6230AB29}"/>
+    <hyperlink ref="C104" r:id="rId279" xr:uid="{2AC02C2A-F7B1-4CDE-8106-C0D377FFD10A}"/>
+    <hyperlink ref="D104" r:id="rId280" xr:uid="{CF5FB671-CD80-457E-9A5C-55AC19128002}"/>
+    <hyperlink ref="E104" r:id="rId281" xr:uid="{7EB7712F-F3D4-4CD0-928D-AA08612DA711}"/>
+    <hyperlink ref="C105" r:id="rId282" xr:uid="{3A98A613-5247-4EDD-9ED8-FFB31D28F72C}"/>
+    <hyperlink ref="D105" r:id="rId283" xr:uid="{B0F0B342-1498-46A9-BD50-0660E9657C90}"/>
+    <hyperlink ref="E105" r:id="rId284" xr:uid="{0B67D960-696C-427C-A875-D3B85CFF0762}"/>
+    <hyperlink ref="C106" r:id="rId285" xr:uid="{1DA3041A-7728-4026-B61E-A1AB5F15F5A8}"/>
+    <hyperlink ref="D106" r:id="rId286" xr:uid="{451E6F75-0E8E-49A5-8A5B-87255F93DD33}"/>
+    <hyperlink ref="E106" r:id="rId287" xr:uid="{D49DC68C-742B-425B-881B-A83AF4714EE4}"/>
+    <hyperlink ref="C107" r:id="rId288" xr:uid="{D226CEDC-443D-41F7-AD26-0AAF1BD9DB3F}"/>
+    <hyperlink ref="D107" r:id="rId289" xr:uid="{EF0F660D-62B8-4AA4-A272-57AB44F0E9CF}"/>
+    <hyperlink ref="E107" r:id="rId290" xr:uid="{3F4019C0-9C15-4B90-B9D3-90908DBCF849}"/>
+    <hyperlink ref="C108" r:id="rId291" xr:uid="{8B746AED-6ACC-4850-8828-FB6F0374D303}"/>
+    <hyperlink ref="D108" r:id="rId292" xr:uid="{F9014A66-3EE9-40DC-B87E-5D9054B50E5D}"/>
+    <hyperlink ref="E108" r:id="rId293" xr:uid="{4EE6DB51-0C8B-400C-A838-15E4BD633EE2}"/>
+    <hyperlink ref="C109" r:id="rId294" xr:uid="{FA69422B-0C15-4C8B-B074-46A3869AC7C9}"/>
+    <hyperlink ref="D109" r:id="rId295" xr:uid="{621EC68A-7ACE-45FB-88A3-06F720875DD7}"/>
+    <hyperlink ref="E109" r:id="rId296" xr:uid="{554DED57-0D82-433F-987B-1B34E1214C78}"/>
+    <hyperlink ref="C110" r:id="rId297" xr:uid="{4117E483-CA3B-487C-94D0-D68E8DB43993}"/>
+    <hyperlink ref="D110" r:id="rId298" xr:uid="{8AAA2CF2-8CC2-4067-AAC9-FA2A4EFE32DD}"/>
+    <hyperlink ref="E110" r:id="rId299" xr:uid="{66B74877-14BB-4AD3-8761-E581180779E3}"/>
+    <hyperlink ref="C111" r:id="rId300" xr:uid="{C527C048-13AF-4166-AAC3-24C05E9E601E}"/>
+    <hyperlink ref="D111" r:id="rId301" xr:uid="{2965799F-E19D-4831-A7B4-10AC9AAC4229}"/>
+    <hyperlink ref="E111" r:id="rId302" xr:uid="{44E6383F-DB4B-4F5D-BA87-405239E1E5E0}"/>
+    <hyperlink ref="C112" r:id="rId303" xr:uid="{714BC743-EB75-42ED-AF6E-B8B31923740F}"/>
+    <hyperlink ref="D112" r:id="rId304" xr:uid="{C53CEA57-5AB8-4F8D-BE5E-9B4CB9BD9BF5}"/>
+    <hyperlink ref="E112" r:id="rId305" xr:uid="{B6767105-A075-4865-AAC5-BF568E26C3DC}"/>
+    <hyperlink ref="C113" r:id="rId306" xr:uid="{DA3469AE-90EC-41E3-9216-B1C0BDA33A67}"/>
+    <hyperlink ref="D113" r:id="rId307" xr:uid="{557307AD-C5A9-4652-888D-A94FDF80009E}"/>
+    <hyperlink ref="E113" r:id="rId308" xr:uid="{C3DCCA91-9FBC-47D2-A94E-C1B437125A9A}"/>
+    <hyperlink ref="C114" r:id="rId309" xr:uid="{2906FCEE-6A7F-45B3-8BF5-7B231A0D23DB}"/>
+    <hyperlink ref="D114" r:id="rId310" xr:uid="{CBE1D2EA-6123-4939-A2F6-07C30E28EEE0}"/>
+    <hyperlink ref="E114" r:id="rId311" xr:uid="{31DAEDC2-35C0-48F5-A25B-93D7BF3A7450}"/>
+    <hyperlink ref="C115" r:id="rId312" xr:uid="{9E70ABF8-EABB-4B06-80D0-153AB8E19A7B}"/>
+    <hyperlink ref="D115" r:id="rId313" xr:uid="{327C9817-CBEE-4C9A-AAC6-464A863BEF9D}"/>
+    <hyperlink ref="E115" r:id="rId314" xr:uid="{A96FDAEB-0252-432D-A050-64EE5BE04F6D}"/>
+    <hyperlink ref="C116" r:id="rId315" xr:uid="{A4745FA3-0838-4B0A-8AF1-C0E8A9318E7A}"/>
+    <hyperlink ref="D116" r:id="rId316" xr:uid="{D592EA88-2676-4594-A3F8-755BA2197B17}"/>
+    <hyperlink ref="E116" r:id="rId317" xr:uid="{43298315-6704-4543-B6A3-1D12ED3BD89B}"/>
+    <hyperlink ref="C117" r:id="rId318" xr:uid="{4F507A97-E64C-4FA2-827D-A97B68F6502C}"/>
+    <hyperlink ref="D117" r:id="rId319" xr:uid="{89E85572-0309-4ECD-9E6F-6A8BFBDD0475}"/>
+    <hyperlink ref="E117" r:id="rId320" xr:uid="{6C735EE1-5379-4E04-87DC-61981092F13A}"/>
+    <hyperlink ref="C118" r:id="rId321" xr:uid="{DCB2DDD8-CEA1-4A83-927E-AA880D5F2465}"/>
+    <hyperlink ref="D118" r:id="rId322" xr:uid="{87B4582B-3A51-46CB-A7AA-14A53BEF2877}"/>
+    <hyperlink ref="E118" r:id="rId323" xr:uid="{95F3F337-662F-4DEB-899F-8B106C6AD582}"/>
+    <hyperlink ref="D119" r:id="rId324" xr:uid="{C6E03219-8688-46D5-858A-2C3BB7AC04D7}"/>
+    <hyperlink ref="E119" r:id="rId325" xr:uid="{222C944B-0CA2-4AA1-BFF7-664ED828CA3B}"/>
+    <hyperlink ref="C119" r:id="rId326" xr:uid="{50F33598-73F6-4B9D-8478-4AC6890A025A}"/>
+    <hyperlink ref="D120" r:id="rId327" xr:uid="{4AED68E4-2779-4CB0-B7AE-44AFAECA4499}"/>
+    <hyperlink ref="E120" r:id="rId328" xr:uid="{20510976-5BE1-4F80-89F3-DC95303A5BBF}"/>
+    <hyperlink ref="C120" r:id="rId329" xr:uid="{3842BBC2-0FE4-402C-A871-BFB50EE32BA0}"/>
+    <hyperlink ref="C121" r:id="rId330" xr:uid="{89D31CD8-B8E5-49D6-8FA5-D7A42F6CB540}"/>
+    <hyperlink ref="D121" r:id="rId331" xr:uid="{AC74A6C1-41F5-4315-92E2-A3C7ED59EBBD}"/>
+    <hyperlink ref="E121" r:id="rId332" xr:uid="{B1F093AF-7F7F-460F-A4F0-ADB6490D731B}"/>
+    <hyperlink ref="C122" r:id="rId333" xr:uid="{D4F65573-20F5-43D1-80BF-2795F41D9F57}"/>
+    <hyperlink ref="D122" r:id="rId334" xr:uid="{B88C2559-C22D-41ED-8F15-469DB6777B84}"/>
+    <hyperlink ref="E122" r:id="rId335" xr:uid="{EEA137CE-31F7-415B-94AB-CA2A55462E5C}"/>
+    <hyperlink ref="C123" r:id="rId336" xr:uid="{D997E317-1F11-4A83-B7F1-CF5217F8F4ED}"/>
+    <hyperlink ref="D123" r:id="rId337" xr:uid="{C9088CDA-1F58-4681-9DAD-82F7D0583EE5}"/>
+    <hyperlink ref="E123" r:id="rId338" xr:uid="{830325FC-B5CA-4053-8D5D-6DA5A0E9CEB3}"/>
+    <hyperlink ref="C124" r:id="rId339" xr:uid="{5AC4D217-D8FE-4409-862F-FAA5A86520AC}"/>
+    <hyperlink ref="D124" r:id="rId340" xr:uid="{CE468356-AB38-423F-ACE7-04587D99102E}"/>
+    <hyperlink ref="E124" r:id="rId341" xr:uid="{611001F6-2221-481D-AFA1-35DB4D386424}"/>
+    <hyperlink ref="C125" r:id="rId342" xr:uid="{FCC30E1C-7F83-4581-822A-7F2ACF21B208}"/>
+    <hyperlink ref="D125" r:id="rId343" xr:uid="{3A097561-C99B-452A-B5F9-14E12478CA8E}"/>
+    <hyperlink ref="E125" r:id="rId344" xr:uid="{5847BD3E-972F-4164-8556-AAACBBA355DB}"/>
+    <hyperlink ref="C126" r:id="rId345" xr:uid="{3BCC14C6-3272-4FB5-B30F-233B0FFAA229}"/>
+    <hyperlink ref="D126" r:id="rId346" xr:uid="{D87B0C63-927A-423F-9DEE-FB163765706A}"/>
+    <hyperlink ref="E126" r:id="rId347" xr:uid="{8D18C038-05BE-41FB-9589-349C2DB35EB6}"/>
+    <hyperlink ref="C127" r:id="rId348" xr:uid="{212AE7B7-8417-4613-9B01-457D5FAD32E2}"/>
+    <hyperlink ref="D127" r:id="rId349" xr:uid="{16169750-2789-41D4-92EE-8370C62CF1BA}"/>
+    <hyperlink ref="E127" r:id="rId350" xr:uid="{EF236839-B3F1-4D2A-8793-A6E0A9D52328}"/>
+    <hyperlink ref="C128" r:id="rId351" xr:uid="{13F5A019-E7BD-473A-8BFB-051E885B1146}"/>
+    <hyperlink ref="D128" r:id="rId352" xr:uid="{C06C249C-A9D7-4BAE-AD6C-0ECED61AA088}"/>
+    <hyperlink ref="E128" r:id="rId353" xr:uid="{C2493638-1F36-426C-A65E-9BA0E883C835}"/>
+    <hyperlink ref="C129" r:id="rId354" xr:uid="{7F246417-F2E2-4CEF-ACB8-0C0E87FFBD79}"/>
+    <hyperlink ref="D129" r:id="rId355" xr:uid="{77141049-FDE6-4B29-8926-A7256E4C0505}"/>
+    <hyperlink ref="E129" r:id="rId356" xr:uid="{F98DCA20-9796-418E-B8CA-A3E005647A01}"/>
+    <hyperlink ref="C130" r:id="rId357" xr:uid="{0BA229B0-06A2-4C48-9914-A5374B32A34F}"/>
+    <hyperlink ref="D130" r:id="rId358" xr:uid="{3F506EBE-0BD0-4794-87C1-953206B16CD4}"/>
+    <hyperlink ref="E130" r:id="rId359" xr:uid="{A615BCEB-72DE-43C7-8A07-693C54D3A0C4}"/>
+    <hyperlink ref="C131" r:id="rId360" xr:uid="{07FCC78B-BF39-43FB-A89D-700B9FB2D824}"/>
+    <hyperlink ref="D131" r:id="rId361" xr:uid="{12B43D3A-B1AA-41D0-8A47-1DDC5FBC02CC}"/>
+    <hyperlink ref="E131" r:id="rId362" xr:uid="{E1EB98C2-E2CA-4E94-8439-8B789E3754E7}"/>
+    <hyperlink ref="D132" r:id="rId363" xr:uid="{63468E1D-F523-48BF-8225-D649FBE847EC}"/>
+    <hyperlink ref="E132" r:id="rId364" xr:uid="{4D681694-A038-4227-BC2E-F2651367ACF3}"/>
+    <hyperlink ref="C132" r:id="rId365" xr:uid="{D7ECE862-4574-486D-A9A4-78F8E4FC1681}"/>
+    <hyperlink ref="C133" r:id="rId366" xr:uid="{B156B9CD-29C4-4D78-8EBA-515A4C1B6B5A}"/>
+    <hyperlink ref="D133" r:id="rId367" xr:uid="{DA45D1F5-4AD3-4F4C-8A29-855166DF6940}"/>
+    <hyperlink ref="E133" r:id="rId368" xr:uid="{596A4EF2-4527-401B-A2CE-FA6A6AE241FF}"/>
+    <hyperlink ref="C134" r:id="rId369" xr:uid="{DC92B3C9-52B9-4D63-AC4A-1FE80AD38A7B}"/>
+    <hyperlink ref="D134" r:id="rId370" xr:uid="{6653B8D2-7773-4FD1-8AB6-76B074FA4AAA}"/>
+    <hyperlink ref="E134" r:id="rId371" xr:uid="{58D58C73-9A50-44A9-A0EA-5592206BB72F}"/>
+    <hyperlink ref="C135" r:id="rId372" xr:uid="{CF269375-1231-4422-9D05-86CA9413B1AD}"/>
+    <hyperlink ref="D135" r:id="rId373" xr:uid="{7AF85C45-2D0F-4BF2-8039-612435A7F999}"/>
+    <hyperlink ref="E135" r:id="rId374" xr:uid="{B39AC57D-61C7-4384-92C0-FA4D3C141F31}"/>
+    <hyperlink ref="C136" r:id="rId375" xr:uid="{F5D55CD9-3B76-4FD8-AC67-16192C305D26}"/>
+    <hyperlink ref="D136" r:id="rId376" xr:uid="{48D8B605-74CE-472F-AFDD-08EC6689007C}"/>
+    <hyperlink ref="E136" r:id="rId377" xr:uid="{44FF3624-E323-438F-8CAB-68D1CB08688C}"/>
+    <hyperlink ref="C137" r:id="rId378" xr:uid="{CE592AC5-E5D6-495B-BB1B-85E6B7EE95DA}"/>
+    <hyperlink ref="D137" r:id="rId379" xr:uid="{D0AD0ECF-67E1-4B11-91F5-AA23D31475D4}"/>
+    <hyperlink ref="E137" r:id="rId380" xr:uid="{CA7CD45E-3E5B-4C2E-93A9-84848C1A52F2}"/>
+    <hyperlink ref="C138" r:id="rId381" xr:uid="{971AEABA-C26E-4CD2-B617-7E7AEFA79225}"/>
+    <hyperlink ref="D138" r:id="rId382" xr:uid="{E838D43A-FA34-4E17-A12D-60A467F149C2}"/>
+    <hyperlink ref="E138" r:id="rId383" xr:uid="{31F37E78-12DF-444E-A3FB-EF00403D39D4}"/>
+    <hyperlink ref="C139" r:id="rId384" xr:uid="{7DC70FA2-2641-4F66-B9F8-01F68ED70F02}"/>
+    <hyperlink ref="D139" r:id="rId385" xr:uid="{B963012C-FACA-4A11-B1C4-313CF3F6387F}"/>
+    <hyperlink ref="E139" r:id="rId386" xr:uid="{E1DCAB4B-878B-4C50-97B6-B5A5D2A2FADD}"/>
+    <hyperlink ref="C140" r:id="rId387" xr:uid="{60F58296-9148-4312-9D0C-BF4DE0690B91}"/>
+    <hyperlink ref="D140" r:id="rId388" xr:uid="{8DBCCAC8-BC9E-442F-A475-9F8639697DB9}"/>
+    <hyperlink ref="E140" r:id="rId389" xr:uid="{0B4BC81F-7CB5-41BC-88B0-3B2BBBE80A3F}"/>
+    <hyperlink ref="D141" r:id="rId390" xr:uid="{9A0BB159-B669-435C-9CB1-A2BA4C4091A9}"/>
+    <hyperlink ref="E141" r:id="rId391" xr:uid="{0055782C-E077-4204-8FF9-57BE6F8FED26}"/>
+    <hyperlink ref="C141" r:id="rId392" xr:uid="{FE323C66-30FE-40E0-8F0E-4108D9EC2713}"/>
+    <hyperlink ref="C142" r:id="rId393" xr:uid="{666B5CC7-4AFE-4EE4-93A2-099371C034E3}"/>
+    <hyperlink ref="D142" r:id="rId394" xr:uid="{A9DFF398-3782-4606-A5AD-16EB49874249}"/>
+    <hyperlink ref="E142" r:id="rId395" xr:uid="{CB3B62B3-3706-4AEA-B831-85D12973AAFB}"/>
+    <hyperlink ref="C143" r:id="rId396" xr:uid="{5B3C3EC4-7E86-40AB-980C-956D883C0DE8}"/>
+    <hyperlink ref="D143" r:id="rId397" xr:uid="{E58660DA-18E4-456D-AE6E-157A8C791640}"/>
+    <hyperlink ref="E143" r:id="rId398" xr:uid="{30D38FD6-524A-4260-A893-C02ABC8FD7D8}"/>
+    <hyperlink ref="C144" r:id="rId399" xr:uid="{EAA73046-9047-4BE9-A054-E3310DE63E1A}"/>
+    <hyperlink ref="D144" r:id="rId400" xr:uid="{54E7A160-9887-4A15-A5E4-7E98C3B546B1}"/>
+    <hyperlink ref="E144" r:id="rId401" xr:uid="{5BA4E4AA-D08F-40BB-B211-CD81B18FF87A}"/>
+    <hyperlink ref="C145" r:id="rId402" xr:uid="{E57FE190-B789-4567-B86E-2D8DD5BB470A}"/>
+    <hyperlink ref="D145" r:id="rId403" xr:uid="{303EC3AA-5A58-4C68-97E5-480D5E8B49ED}"/>
+    <hyperlink ref="E145" r:id="rId404" xr:uid="{111A682B-10E9-494F-BA71-FEC4F7FB0BD6}"/>
+    <hyperlink ref="C146" r:id="rId405" xr:uid="{E353A765-41EF-43C2-AB89-89DFAEA7EAB7}"/>
+    <hyperlink ref="D146" r:id="rId406" xr:uid="{6DB31883-29E3-4B37-A5BC-B8A2B95FBC29}"/>
+    <hyperlink ref="E146" r:id="rId407" xr:uid="{FCF11283-83AE-42A7-BB7D-85631FD6E8B9}"/>
+    <hyperlink ref="C147" r:id="rId408" xr:uid="{2CA57331-C3C7-4E12-82CB-C628ECE4CCAB}"/>
+    <hyperlink ref="D147" r:id="rId409" xr:uid="{B5E1FE84-C98A-420D-837D-C3DCBB95E91F}"/>
+    <hyperlink ref="E147" r:id="rId410" xr:uid="{20932CE8-F8AE-4689-9CD7-3D080869A55D}"/>
+    <hyperlink ref="C148" r:id="rId411" xr:uid="{7618A490-B688-42C9-94E0-4F8540FF40DB}"/>
+    <hyperlink ref="D148" r:id="rId412" xr:uid="{668BB9C5-109F-4A7E-868C-D2732EFA34A2}"/>
+    <hyperlink ref="E148" r:id="rId413" xr:uid="{0F731946-786D-4814-BAE4-8D0C99005D78}"/>
+    <hyperlink ref="C149" r:id="rId414" xr:uid="{51F53306-B34E-472A-B470-69B8029C9ED4}"/>
+    <hyperlink ref="D149" r:id="rId415" xr:uid="{F2FEECB1-F3BC-4C78-B544-613C7FF5E436}"/>
+    <hyperlink ref="E149" r:id="rId416" xr:uid="{343909DC-77D4-4FBB-BE02-DCD4EC0C20EB}"/>
+    <hyperlink ref="C150" r:id="rId417" xr:uid="{F187FD4D-E765-4937-9701-2C58603180AE}"/>
+    <hyperlink ref="D150" r:id="rId418" xr:uid="{31FB4D76-B008-46DB-9637-691B1894CE21}"/>
+    <hyperlink ref="E150" r:id="rId419" xr:uid="{03572D9E-807D-4918-B128-29411ACBB625}"/>
+    <hyperlink ref="C151" r:id="rId420" xr:uid="{5130DE5E-46EF-4B05-8FE0-179C2E7E6948}"/>
+    <hyperlink ref="D151" r:id="rId421" xr:uid="{97742F59-5F59-4D68-996E-0A272575FADC}"/>
+    <hyperlink ref="E151" r:id="rId422" xr:uid="{2355B201-6EF9-4A6A-A9B9-BF166EC28606}"/>
+    <hyperlink ref="C152" r:id="rId423" xr:uid="{407F15B9-9D77-4AFB-B5E8-1B163C7E370E}"/>
+    <hyperlink ref="D152" r:id="rId424" xr:uid="{7A5EB5DE-BDC8-4E93-9761-A6603D00EFAD}"/>
+    <hyperlink ref="E152" r:id="rId425" xr:uid="{097CE107-4BA7-4CF3-996A-093477F670F6}"/>
+    <hyperlink ref="D153" r:id="rId426" xr:uid="{51B6FCED-FA56-433D-BA3D-445C0F2FE651}"/>
+    <hyperlink ref="E153" r:id="rId427" xr:uid="{26C3E259-1ACD-4F3A-B70D-194C131947DB}"/>
+    <hyperlink ref="C153" r:id="rId428" xr:uid="{3A114C26-8E8C-45B9-94BD-FCD3CAA9597E}"/>
+    <hyperlink ref="C154" r:id="rId429" xr:uid="{9AA9391F-DE63-4135-A127-DF0F47F7D8C7}"/>
+    <hyperlink ref="D154" r:id="rId430" xr:uid="{2BF42871-0750-440A-A243-619A1C20CC7F}"/>
+    <hyperlink ref="E154" r:id="rId431" xr:uid="{D39D1674-E469-410B-9639-99835CA9A908}"/>
+    <hyperlink ref="C155" r:id="rId432" xr:uid="{5F3DC677-1855-4283-B201-795E598B8917}"/>
+    <hyperlink ref="D155" r:id="rId433" xr:uid="{97F71AB0-0556-481D-B3A2-984C5AB5ED3A}"/>
+    <hyperlink ref="E155" r:id="rId434" xr:uid="{F4091531-5EEE-42BF-9549-D3422C21479A}"/>
+    <hyperlink ref="C156" r:id="rId435" xr:uid="{09680C2A-D8C5-41B4-9F07-96FF1792918C}"/>
+    <hyperlink ref="D156" r:id="rId436" xr:uid="{B9850E60-1546-4D20-8BF8-E8A5C91504C9}"/>
+    <hyperlink ref="E156" r:id="rId437" xr:uid="{CB7D6C00-6A72-4633-A0C4-CA7AD5F7CA43}"/>
+    <hyperlink ref="C157" r:id="rId438" xr:uid="{80024236-A643-48BC-A603-88E4C61F39E9}"/>
+    <hyperlink ref="D157" r:id="rId439" xr:uid="{120C8743-AA48-4C9A-AE55-5610BE126DC3}"/>
+    <hyperlink ref="E157" r:id="rId440" xr:uid="{2D5BB430-5FE3-453B-A9D2-87D25EF175BD}"/>
+    <hyperlink ref="C158" r:id="rId441" xr:uid="{4DFB4F67-145A-44E0-BE4E-70236393A673}"/>
+    <hyperlink ref="D158" r:id="rId442" xr:uid="{63643BC2-FC62-42D6-82C6-75379B5F7031}"/>
+    <hyperlink ref="E158" r:id="rId443" xr:uid="{6CF4B868-96BA-46BA-B87F-853852F4531D}"/>
+    <hyperlink ref="C159" r:id="rId444" xr:uid="{352410C9-FE4B-4A2C-BC1F-750169232690}"/>
+    <hyperlink ref="D159" r:id="rId445" xr:uid="{AFE88A43-637E-4B75-B37A-1F57451F4619}"/>
+    <hyperlink ref="E159" r:id="rId446" xr:uid="{7535847A-C949-43A9-93A4-F0EC6DDF68DA}"/>
+    <hyperlink ref="C160" r:id="rId447" xr:uid="{4C1038DE-1D54-48E4-8E66-F691E40DCC63}"/>
+    <hyperlink ref="D160" r:id="rId448" xr:uid="{41172669-0845-43AD-9650-8B8A62925666}"/>
+    <hyperlink ref="E160" r:id="rId449" xr:uid="{B16881C8-92C0-4AA1-B859-DBDCB15AD570}"/>
+    <hyperlink ref="C161" r:id="rId450" xr:uid="{39A2F065-2C25-448A-8687-9F2149D01184}"/>
+    <hyperlink ref="D161" r:id="rId451" xr:uid="{F2ED0C3A-0135-4147-AEFF-DC4B8ED0D685}"/>
+    <hyperlink ref="E161" r:id="rId452" xr:uid="{8DF3594C-0BF9-448B-A503-24794FCECEA3}"/>
+    <hyperlink ref="D162" r:id="rId453" xr:uid="{2D27BDFB-D4B5-44B9-965C-A93682BCB150}"/>
+    <hyperlink ref="E162" r:id="rId454" xr:uid="{744A7EC5-AEB8-42E3-A556-E4E16C245E49}"/>
+    <hyperlink ref="C162" r:id="rId455" xr:uid="{1A5BE688-8DAF-46EE-BE55-B56FA387D60A}"/>
+    <hyperlink ref="C163" r:id="rId456" xr:uid="{A2A8969B-E67C-4C42-9F40-97418205870F}"/>
+    <hyperlink ref="D163" r:id="rId457" xr:uid="{8C15BC14-EB1D-4AFA-82A9-D7F5FEB92B34}"/>
+    <hyperlink ref="E163" r:id="rId458" xr:uid="{C1AF09A0-75AC-415B-AEAA-FFE6CDF5282B}"/>
+    <hyperlink ref="C164" r:id="rId459" xr:uid="{97A7FD74-2B85-4FD7-96FD-C28091A20A4D}"/>
+    <hyperlink ref="D164" r:id="rId460" xr:uid="{8C7ACE0C-84B0-4967-A6EA-73EBBBCA6E3A}"/>
+    <hyperlink ref="E164" r:id="rId461" xr:uid="{63C7876B-76A9-4A33-B78B-52C0CA2D8D5E}"/>
+    <hyperlink ref="C165" r:id="rId462" xr:uid="{06B4DEBF-7C8E-4884-91BE-A793EE0F62CC}"/>
+    <hyperlink ref="D165" r:id="rId463" xr:uid="{A9147945-5306-4AE5-BE85-C90C7FC7EC3C}"/>
+    <hyperlink ref="E165" r:id="rId464" xr:uid="{77243768-5B39-4BB1-BA96-960A09265D09}"/>
+    <hyperlink ref="D166" r:id="rId465" xr:uid="{0D2C4551-5A3A-4398-A3D2-99FB0401A7D1}"/>
+    <hyperlink ref="E166" r:id="rId466" xr:uid="{38A6A660-830B-4694-A398-A9DE1011AC6B}"/>
+    <hyperlink ref="C166" r:id="rId467" xr:uid="{5228C198-AF2C-40F8-B2F5-057085C54F0D}"/>
+    <hyperlink ref="C167" r:id="rId468" xr:uid="{A08507FD-CA4F-44FD-80EA-F0484A51F904}"/>
+    <hyperlink ref="D167" r:id="rId469" xr:uid="{F9694B45-4A2C-4F66-8EE4-DA8EE40951ED}"/>
+    <hyperlink ref="E167" r:id="rId470" xr:uid="{C3119FB8-069B-4D3F-B5C3-5883D3A505F1}"/>
+    <hyperlink ref="C168" r:id="rId471" xr:uid="{AA2D388E-48CF-41C9-B888-4F64BFF2ACC5}"/>
+    <hyperlink ref="D168" r:id="rId472" xr:uid="{136A9ACA-B873-408C-877B-B88BEDEE02DE}"/>
+    <hyperlink ref="E168" r:id="rId473" xr:uid="{45143C2B-0CE5-460D-8C8C-7BDD7391EC20}"/>
+    <hyperlink ref="C169" r:id="rId474" xr:uid="{412AABCD-D11B-4C1F-BAE3-8E9B5314FEFE}"/>
+    <hyperlink ref="D169" r:id="rId475" xr:uid="{52143DB4-9220-420E-9325-C79A91D3E77F}"/>
+    <hyperlink ref="E169" r:id="rId476" xr:uid="{EBD5079E-6759-45C1-A040-15A1D7EFA833}"/>
+    <hyperlink ref="C170" r:id="rId477" xr:uid="{D9EDA746-00FA-479B-BBF8-E6EA24906B94}"/>
+    <hyperlink ref="D170" r:id="rId478" xr:uid="{F2F02B4C-A61F-48DB-B4B9-B590F1EAE1A5}"/>
+    <hyperlink ref="E170" r:id="rId479" xr:uid="{4EF3DEB5-F631-42E5-BF23-8FD5BD7C5726}"/>
+    <hyperlink ref="C171" r:id="rId480" xr:uid="{C7AC3295-F2D7-4B73-81FE-CE9DD8908E72}"/>
+    <hyperlink ref="D171" r:id="rId481" xr:uid="{13A8A69F-88CE-42AE-A904-E26015719290}"/>
+    <hyperlink ref="E171" r:id="rId482" xr:uid="{69E9CB21-248F-4A60-986D-523E9D222CCD}"/>
+    <hyperlink ref="C172" r:id="rId483" xr:uid="{7627DCB7-8878-43A8-B6E9-AA0B9A8AA69D}"/>
+    <hyperlink ref="D172" r:id="rId484" xr:uid="{FCCBB0CF-B9DD-4759-BBA3-76BD72CDE47E}"/>
+    <hyperlink ref="E172" r:id="rId485" xr:uid="{3E811DA2-3C40-4364-9266-6773CDEE5611}"/>
+    <hyperlink ref="C173" r:id="rId486" xr:uid="{FC27C7F6-56D3-4353-B218-AEDBD69411BE}"/>
+    <hyperlink ref="D173" r:id="rId487" xr:uid="{1FAEEA19-C0F2-4B64-AB53-5CE1FCFD3EED}"/>
+    <hyperlink ref="E173" r:id="rId488" xr:uid="{9AFEB9F6-C42C-4F69-BAB9-0F96228BAB75}"/>
+    <hyperlink ref="C174" r:id="rId489" xr:uid="{782E6140-94C3-407F-BEAF-9C0D976620EB}"/>
+    <hyperlink ref="D174" r:id="rId490" xr:uid="{B6A4BB4A-CEE1-4126-85FD-8A0A92A86F6C}"/>
+    <hyperlink ref="E174" r:id="rId491" xr:uid="{4DE847BB-899E-400F-B0A1-5368BD326435}"/>
+    <hyperlink ref="C175" r:id="rId492" xr:uid="{550B60D7-37BE-42DF-A0A6-234EE2ABEC88}"/>
+    <hyperlink ref="D175" r:id="rId493" xr:uid="{FE54EAA5-5BCB-4AE8-B0F0-DF219D75D2FA}"/>
+    <hyperlink ref="E175" r:id="rId494" xr:uid="{5F404BDE-7004-4B15-8063-6FFDD0232C10}"/>
+    <hyperlink ref="D176" r:id="rId495" xr:uid="{04847EC6-CA8E-40B5-A255-4AA69821E9CD}"/>
+    <hyperlink ref="E176" r:id="rId496" xr:uid="{C5321455-60AF-4B1F-B2EB-9C48ABE6CF88}"/>
+    <hyperlink ref="C176" r:id="rId497" xr:uid="{F487FA1F-6345-4747-9B2D-E8B2F3CA8F64}"/>
+    <hyperlink ref="C177" r:id="rId498" xr:uid="{0BB76D84-05E9-403F-B67C-C3BFFCCC1DE9}"/>
+    <hyperlink ref="D177" r:id="rId499" xr:uid="{E68DE772-C262-43D4-BAB1-57B7508710F5}"/>
+    <hyperlink ref="E177" r:id="rId500" xr:uid="{E2FD5107-217F-4912-8F1C-CBCA0456D0B1}"/>
+    <hyperlink ref="C178" r:id="rId501" xr:uid="{0709A472-9980-4F85-A449-8A5D6EABD5F4}"/>
+    <hyperlink ref="D178" r:id="rId502" xr:uid="{31C86E75-E56D-4C5A-965A-002F4B567CEA}"/>
+    <hyperlink ref="E178" r:id="rId503" xr:uid="{A44C8FE0-0122-4430-BB7B-95FC5AC20FD1}"/>
+    <hyperlink ref="C179" r:id="rId504" xr:uid="{6CA3E827-405F-40BE-9BA0-7F75BE64C3EF}"/>
+    <hyperlink ref="D179" r:id="rId505" xr:uid="{1AB16091-69AE-4105-9BA6-B775B46361F8}"/>
+    <hyperlink ref="E179" r:id="rId506" xr:uid="{2B7A126E-8D1B-4E8F-93A6-C98453F4B0CD}"/>
+    <hyperlink ref="C180" r:id="rId507" xr:uid="{FF9DC8D1-E300-4D00-8478-B4C4465463B0}"/>
+    <hyperlink ref="D180" r:id="rId508" xr:uid="{C7FB4928-100E-4F31-AA8B-9BB5386BD6E2}"/>
+    <hyperlink ref="E180" r:id="rId509" xr:uid="{33E88EF2-069C-4A8A-A4B9-407D561D9FA7}"/>
+    <hyperlink ref="C181" r:id="rId510" xr:uid="{AD27F6F9-722F-4772-BAD3-292259E599AE}"/>
+    <hyperlink ref="D181" r:id="rId511" xr:uid="{9855AD87-CCE8-4B4A-9D90-654E9CB9A884}"/>
+    <hyperlink ref="E181" r:id="rId512" xr:uid="{DABA9FDA-64E2-49EB-A86C-6A285B8ED457}"/>
+    <hyperlink ref="C182" r:id="rId513" xr:uid="{08DC194C-ADC7-4BD9-B1FA-D02B1EB30413}"/>
+    <hyperlink ref="D182" r:id="rId514" xr:uid="{BDCC0E77-3EA0-4F00-B40F-EB3744C4B10A}"/>
+    <hyperlink ref="E182" r:id="rId515" xr:uid="{0C11EA0B-B2D0-438E-81C0-C400F6D0799A}"/>
+    <hyperlink ref="C183" r:id="rId516" xr:uid="{13991465-B6B8-432B-B460-78ABB1DED868}"/>
+    <hyperlink ref="D183" r:id="rId517" xr:uid="{A036A9F5-033D-4A23-B1E3-B321FB1A1D5C}"/>
+    <hyperlink ref="E183" r:id="rId518" xr:uid="{D1FD862C-B5D6-4B13-931B-57B7FFF1059A}"/>
+    <hyperlink ref="C184" r:id="rId519" xr:uid="{5217B7E5-50F7-4581-9109-F6A8BC875186}"/>
+    <hyperlink ref="D184" r:id="rId520" xr:uid="{C3F790CF-A478-40B7-99F6-7D2667CBC146}"/>
+    <hyperlink ref="E184" r:id="rId521" xr:uid="{A5F80E79-506C-4A15-AACD-68F53D61E373}"/>
+    <hyperlink ref="C185" r:id="rId522" xr:uid="{62E029C0-61D3-4187-A49A-6F8E847B07E9}"/>
+    <hyperlink ref="D185" r:id="rId523" xr:uid="{682FAA6B-7ADD-4D0B-9D48-124102D3B8C4}"/>
+    <hyperlink ref="E185" r:id="rId524" xr:uid="{CB64775F-93CB-4F3C-A7B2-61AA1EEC9FF4}"/>
+    <hyperlink ref="D186" r:id="rId525" xr:uid="{33DB2910-4B9B-4EBD-94DB-9D1D8BA1A60A}"/>
+    <hyperlink ref="E186" r:id="rId526" xr:uid="{D816F0E8-5CA4-4FBA-A574-65EB5C502159}"/>
+    <hyperlink ref="C186" r:id="rId527" xr:uid="{7BED455F-4DC7-4B45-AD26-E1286840DEBE}"/>
+    <hyperlink ref="C187" r:id="rId528" xr:uid="{B17E7A06-B7A3-43DE-959C-80217F4C7404}"/>
+    <hyperlink ref="D187" r:id="rId529" xr:uid="{108A2D11-51B8-4F46-B0AE-357FA3F6BDB6}"/>
+    <hyperlink ref="E187" r:id="rId530" xr:uid="{16666982-1A83-4A62-BFC7-C4F40E6C916E}"/>
+    <hyperlink ref="C188" r:id="rId531" xr:uid="{053DBA08-46A7-4A97-9457-F0E304824F8E}"/>
+    <hyperlink ref="D188" r:id="rId532" xr:uid="{DB4ECA15-195B-4A54-858F-239BA708B125}"/>
+    <hyperlink ref="E188" r:id="rId533" xr:uid="{17CC691E-0C7E-443C-B3E1-54C8BFC12D95}"/>
+    <hyperlink ref="C189" r:id="rId534" xr:uid="{488BAF16-AD49-4FAE-8E4C-CE7962082CBA}"/>
+    <hyperlink ref="D189" r:id="rId535" xr:uid="{0B038405-DDEA-461D-994B-7F271E9120F4}"/>
+    <hyperlink ref="E189" r:id="rId536" xr:uid="{7BACCCB4-5CF4-4224-9201-E647233DE274}"/>
+    <hyperlink ref="C190" r:id="rId537" xr:uid="{E9108E47-563C-4F4D-8B1F-CB863619C501}"/>
+    <hyperlink ref="D190" r:id="rId538" xr:uid="{ECB18330-35A1-421E-8B98-A38AB1F12F4B}"/>
+    <hyperlink ref="E190" r:id="rId539" xr:uid="{594B3616-5B4C-4902-90E8-B56CF4ADD901}"/>
+    <hyperlink ref="C191" r:id="rId540" xr:uid="{BEC6DA00-205E-4FA8-BF78-644278A12620}"/>
+    <hyperlink ref="D191" r:id="rId541" xr:uid="{66E4959D-D2E5-40E0-9A50-3E9722C83879}"/>
+    <hyperlink ref="E191" r:id="rId542" xr:uid="{165E3072-0F8C-4D07-A8EE-AFB2E92D10D0}"/>
+    <hyperlink ref="C192" r:id="rId543" xr:uid="{8BDFFA66-526B-49E6-A9EF-74BACEF2FC3A}"/>
+    <hyperlink ref="D192" r:id="rId544" xr:uid="{23452AE3-198E-4555-8556-92D1EB9C8F2F}"/>
+    <hyperlink ref="E192" r:id="rId545" xr:uid="{1C8BB96E-E2D2-41A2-B51E-CA1C94882C45}"/>
+    <hyperlink ref="C193" r:id="rId546" xr:uid="{78499224-1133-4CA4-8141-97A18D48B873}"/>
+    <hyperlink ref="D193" r:id="rId547" xr:uid="{B9B02DD2-D017-4DBC-9327-5DF3E8B353CB}"/>
+    <hyperlink ref="E193" r:id="rId548" xr:uid="{4CDCE363-4F15-4C8E-88A0-16B4ACE31706}"/>
+    <hyperlink ref="D194" r:id="rId549" xr:uid="{9672DF3D-1B42-4B06-BE7E-8C371290DDD8}"/>
+    <hyperlink ref="E194" r:id="rId550" xr:uid="{A6A6609E-1ACE-4AE1-8630-67EC2A09BB1B}"/>
+    <hyperlink ref="C194" r:id="rId551" xr:uid="{2945D925-89ED-4A50-9C8A-33FAE3D9B663}"/>
+    <hyperlink ref="C195" r:id="rId552" xr:uid="{B2232121-8FC5-4AFB-B4A5-EAFCA6F8BF55}"/>
+    <hyperlink ref="D195" r:id="rId553" xr:uid="{BDB9895C-3A01-437E-B535-262F78163F79}"/>
+    <hyperlink ref="E195" r:id="rId554" xr:uid="{7E8CB580-3C77-4108-A7BB-241E5DD2F8F8}"/>
+    <hyperlink ref="C196" r:id="rId555" xr:uid="{0E762398-C5ED-49DE-9BD7-D01671B4E18A}"/>
+    <hyperlink ref="D196" r:id="rId556" xr:uid="{7FC49659-FA8F-434A-B4B6-95508B1B4D35}"/>
+    <hyperlink ref="E196" r:id="rId557" xr:uid="{5FD4642D-66C0-4BCC-9C59-E55B95CFBFBB}"/>
+    <hyperlink ref="C197" r:id="rId558" xr:uid="{63BBE702-55C8-4458-8A67-C5591C5F9247}"/>
+    <hyperlink ref="D197" r:id="rId559" xr:uid="{A666B7EF-0CBD-4183-BF04-FD5B6DDCF6FD}"/>
+    <hyperlink ref="D99" r:id="rId560" xr:uid="{BB5402C0-11CF-4FB7-9D11-E4E06DA8E09D}"/>
+    <hyperlink ref="C99" r:id="rId561" xr:uid="{5098A259-C902-4545-A7E1-E636AB33D5F8}"/>
+    <hyperlink ref="D86" r:id="rId562" display="https://www.camara.leg.br/internet/sitaqweb/TextoHTML.asp?etapa=11&amp;tpReuniaoEvento=AP%20c/%20Convidado&amp;dtReuniao=15/08/2017&amp;hrInicio=14:50:00&amp;hrFim=17:12:00&amp;origemDiscurso=&amp;nmLocal=Plen%C3%A1rio%20Principal%20-%20CD&amp;nuSessao=1047/17&amp;nuQuarto=0&amp;nuOrador=0&amp;nuInsercao=0&amp;dtHorarioQuarto=14:50&amp;sgFaseSessao=&amp;Data=15/08/2017&amp;txApelido=&amp;txFaseSessao=&amp;txTipoSessao=Permanente&amp;dtHoraQuarto=14:50&amp;txEtapa=" xr:uid="{885EDDC5-59F7-4E1C-AF16-381A4A38D774}"/>
+    <hyperlink ref="C86" r:id="rId563" xr:uid="{4A17DC70-EC44-4004-B071-6F5D899C8CA5}"/>
+    <hyperlink ref="D71" r:id="rId564" xr:uid="{D677B959-EB3C-4DDB-8AEF-E8EAE6D6D45E}"/>
+    <hyperlink ref="C71" r:id="rId565" xr:uid="{0AD8437A-2704-40CD-866A-26901C1B53CE}"/>
+    <hyperlink ref="D63" r:id="rId566" xr:uid="{5F59921F-E727-4A1F-AE6F-37476A2F81C2}"/>
+    <hyperlink ref="C63" r:id="rId567" xr:uid="{4B817215-AB66-422A-B2EE-745DCCE2715E}"/>
+    <hyperlink ref="C62" r:id="rId568" xr:uid="{2DA64800-7A72-4482-919D-DFF1D13D4B55}"/>
+    <hyperlink ref="D62" r:id="rId569" xr:uid="{E8EC2437-F030-4E8C-B6AC-917AA71D6D2D}"/>
+    <hyperlink ref="D40" r:id="rId570" xr:uid="{6C41F5BF-C09E-47D4-A816-D0E540BD6149}"/>
+    <hyperlink ref="C40" r:id="rId571" xr:uid="{CBA2CB5F-E42B-4632-83EE-22826ADE1E04}"/>
+    <hyperlink ref="E197" r:id="rId572" xr:uid="{136FF705-8DCE-4116-BE70-5F1542A088B0}"/>
+    <hyperlink ref="C198" r:id="rId573" xr:uid="{3FB904D1-0936-422F-96AB-F3B96921D779}"/>
+    <hyperlink ref="D198" r:id="rId574" xr:uid="{7A54B018-01DB-4819-9FD1-68863145C0A1}"/>
+    <hyperlink ref="E198" r:id="rId575" xr:uid="{E3C9E074-5A18-4A4E-8CA3-EEB4F330DFC6}"/>
+    <hyperlink ref="C199" r:id="rId576" xr:uid="{E2D42ECE-DCF2-4092-B7EF-C717EECA06D7}"/>
+    <hyperlink ref="D199" r:id="rId577" xr:uid="{D3B0D91F-A5F5-489B-B4BF-5B6ADA49D078}"/>
+    <hyperlink ref="E199" r:id="rId578" xr:uid="{9E3CF267-2270-4A5E-BF99-A49458146C5C}"/>
+    <hyperlink ref="C200" r:id="rId579" xr:uid="{39D382AA-57C1-42F8-ABF7-11A7F0B35567}"/>
+    <hyperlink ref="D200" r:id="rId580" xr:uid="{8CE8A2BD-98A2-45D9-B373-7C90E69ADB93}"/>
+    <hyperlink ref="E200" r:id="rId581" xr:uid="{DE229DE6-DE64-42DD-97A1-D38A12923FD3}"/>
+    <hyperlink ref="C201" r:id="rId582" xr:uid="{189D0765-1C92-4FC1-A376-28B52EA2BFAF}"/>
+    <hyperlink ref="D201" r:id="rId583" xr:uid="{2532C84C-8DB5-4D9F-8FFB-F09727EC3D64}"/>
+    <hyperlink ref="E201" r:id="rId584" xr:uid="{A9C00FED-2E5B-4151-A8D6-2CBF429036A5}"/>
+    <hyperlink ref="C202" r:id="rId585" xr:uid="{0FB758F3-8CEC-44F8-AB0B-FB5749251F72}"/>
+    <hyperlink ref="D202" r:id="rId586" xr:uid="{14790960-D653-4274-8C1A-87D26826D0D0}"/>
+    <hyperlink ref="E202" r:id="rId587" xr:uid="{669AE71B-0710-4E47-9B20-28C6E0D2A24C}"/>
+    <hyperlink ref="C203" r:id="rId588" xr:uid="{6C1C977A-8104-4C5D-BED7-C833FD88FC10}"/>
+    <hyperlink ref="D203" r:id="rId589" xr:uid="{FA52D527-723E-449E-AE77-53A711E8B5F4}"/>
+    <hyperlink ref="E203" r:id="rId590" xr:uid="{7D40609C-37B6-4DA5-86FD-A779CCE9CF33}"/>
+    <hyperlink ref="D204" r:id="rId591" xr:uid="{E1F2A5BF-32A9-48D5-81EE-19ABF3643DD2}"/>
+    <hyperlink ref="E204" r:id="rId592" xr:uid="{E561AB7E-F883-4B46-9BD4-A1A7658BB442}"/>
+    <hyperlink ref="C204" r:id="rId593" xr:uid="{0B823933-67DE-41F8-B9F5-D78FB031387C}"/>
+    <hyperlink ref="C205" r:id="rId594" xr:uid="{26F9A583-2496-4B17-A929-300CBDA2E24D}"/>
+    <hyperlink ref="D205" r:id="rId595" xr:uid="{6719EDC2-583C-49D3-9ECA-9AAEAB5A1AF8}"/>
+    <hyperlink ref="E205" r:id="rId596" xr:uid="{3243DF7A-EE24-42C4-9051-EF34793BE812}"/>
+    <hyperlink ref="C206" r:id="rId597" xr:uid="{4C45050E-CAB2-4E91-876A-26ACF94DB8B2}"/>
+    <hyperlink ref="D206" r:id="rId598" xr:uid="{4FE2A5B0-C928-4394-8042-D3AA021DA4D8}"/>
+    <hyperlink ref="E206" r:id="rId599" xr:uid="{CAB1117F-895B-408D-BFB0-CC8642447B67}"/>
+    <hyperlink ref="C207" r:id="rId600" xr:uid="{3497FE2B-F080-4F0F-9454-A2F8E2BCEA79}"/>
+    <hyperlink ref="D207" r:id="rId601" xr:uid="{C1B80CC4-8153-4B20-A3F2-B283168811C5}"/>
+    <hyperlink ref="E207" r:id="rId602" xr:uid="{BF0434BE-354E-4789-9E21-F298661908C9}"/>
+    <hyperlink ref="C208" r:id="rId603" xr:uid="{E432FEE7-0CE3-4671-A6DE-A89067FE71F8}"/>
+    <hyperlink ref="D208" r:id="rId604" xr:uid="{9B118C1B-E5E7-4F47-BFA5-206491EA6ED8}"/>
+    <hyperlink ref="E208" r:id="rId605" xr:uid="{9EA9596A-CB3D-4B30-8E07-CA8A3FF7C508}"/>
+    <hyperlink ref="C209" r:id="rId606" xr:uid="{46C6222B-B670-40C3-A605-FABE1731989A}"/>
+    <hyperlink ref="D209" r:id="rId607" xr:uid="{C653707F-D543-43CC-A01D-24A54A6A319B}"/>
+    <hyperlink ref="E209" r:id="rId608" xr:uid="{60116EA4-2834-4C7A-B4DB-1CE223CB90BB}"/>
+    <hyperlink ref="C96" r:id="rId609" xr:uid="{20EC698E-A69F-497B-8D14-1C5CA444BC21}"/>
+    <hyperlink ref="D96" r:id="rId610" xr:uid="{AFAB7C9A-C544-47BD-8645-5C31CE7C5CF3}"/>
+    <hyperlink ref="E96" r:id="rId611" xr:uid="{F53AF2AB-0CE9-45A6-B905-24C7FEEA3E52}"/>
+    <hyperlink ref="C95" r:id="rId612" xr:uid="{30CD9287-A385-456E-9D5E-59944E3156E1}"/>
+    <hyperlink ref="D95" r:id="rId613" xr:uid="{C9FDF5BB-9B0E-442F-AE18-EBCAF9FA12BA}"/>
+    <hyperlink ref="E95" r:id="rId614" xr:uid="{E3661C98-D989-4879-A8FC-B6166662C8D7}"/>
+    <hyperlink ref="C55" r:id="rId615" xr:uid="{2102EDB4-6981-4633-9FD3-E647448181FC}"/>
+    <hyperlink ref="D55" r:id="rId616" xr:uid="{0DB9D726-23FB-4B78-94AC-DFD7B21AB5AE}"/>
+    <hyperlink ref="E55" r:id="rId617" xr:uid="{BF7B36EC-2642-4F9B-A942-FC7DA39117FB}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId624"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId618"/>
 </worksheet>
 </file>
 
@@ -6147,13 +6187,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrige metadados das matérias 185-206
</commit_message>
<xml_diff>
--- a/projeto final/1 - levantamento/Matérias CD.xlsx
+++ b/projeto final/1 - levantamento/Matérias CD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caris\Desktop\IA024_deep_learning_nlp\projeto final\1 - levantamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27D6A41-1C35-44D4-AC9F-FD538BE37207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14046AFC-4A8B-4FF2-8FF6-5F98FE5FA63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A25B0F39-AFD6-49AD-BAE6-0169C11C595E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Aguardando" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tem transcrição'!$C$1:$E$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tem transcrição'!$C$1:$E$207</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="624">
   <si>
     <t>Matéria</t>
   </si>
@@ -795,12 +795,6 @@
     <t>Tem que pegar a transcrição</t>
   </si>
   <si>
-    <t>https://www.camara.leg.br/noticias/520599-DIFICULDADES-PARA-FINANCIAR-EDUCACAO-PODEM-GERAR-DISTORCOES-SOCIAIS-AINDA-MAIORES,-AFIRMAM-DEBATEDORES</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/internet/sitaqweb/TextoHTML.asp?etapa=11&amp;tpReuniaoEvento=AP%20c/%20Convidado&amp;dtReuniao=15/08/2017&amp;hrInicio=14:50:00&amp;hrFim=17:12:00&amp;origemDiscurso=&amp;nmLocal=Plen%C3%A1rio%20Principal%20-%20CD&amp;nuSessao=1047/17&amp;nuQuarto=0&amp;nuOrador=0&amp;nuInsercao=0&amp;dtHorarioQuarto=14:50&amp;sgFaseSessao=&amp;Data=15/08/2017&amp;txApelido=&amp;txFaseSessao=&amp;txTipoSessao=Permanente&amp;dtHoraQuarto=14:50&amp;txEtapa=</t>
-  </si>
-  <si>
     <t>https://www.camara.leg.br/internet/ordemdodia/integras/2410397.htm</t>
   </si>
   <si>
@@ -1537,15 +1531,6 @@
   </si>
   <si>
     <t>https://www.camara.leg.br/internet/ordemdodia/integras/2368779.htm</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/noticias/997410-DEBATEDORES-INDICAM-NECESSIDADE-DE-INVESTIMENTOS-PARA-MELHOR-ATENDIMENTO-DE-URGENCIAS</t>
-  </si>
-  <si>
-    <t>https://escriba.camara.leg.br/escriba-servicosweb/html/69352</t>
-  </si>
-  <si>
-    <t>https://www.camara.leg.br/internet/ordemdodia/integras/2327010.htm</t>
   </si>
   <si>
     <t>https://www.camara.leg.br/noticias/997189-NISIA-TRINDADE-REBATE-POLEMICAS-E-DETALHA-INVESTIMENTOS-DO-NOVO-PAC-NA-SAUDE</t>
@@ -1971,10 +1956,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2310,10 +2294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7617A561-B2B5-4674-8694-EA4F3B3BAE78}">
-  <dimension ref="A1:E209"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,19 +2310,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="B1" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="C1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="D1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E1" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2346,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -2363,7 +2347,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -2380,7 +2364,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -2397,7 +2381,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -2414,7 +2398,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -2431,7 +2415,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -2448,7 +2432,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -2465,7 +2449,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
@@ -2482,7 +2466,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -2499,7 +2483,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>31</v>
@@ -2516,7 +2500,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -2533,7 +2517,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
@@ -2550,7 +2534,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
@@ -2567,7 +2551,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>41</v>
@@ -2584,7 +2568,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>44</v>
@@ -2601,7 +2585,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
@@ -2618,7 +2602,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>51</v>
@@ -2632,7 +2616,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>52</v>
@@ -2649,7 +2633,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>55</v>
@@ -2666,7 +2650,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>58</v>
@@ -2683,7 +2667,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>61</v>
@@ -2700,7 +2684,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>64</v>
@@ -2717,7 +2701,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>67</v>
@@ -2734,7 +2718,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>70</v>
@@ -2751,7 +2735,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>73</v>
@@ -2768,7 +2752,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>76</v>
@@ -2785,7 +2769,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>79</v>
@@ -2802,7 +2786,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>82</v>
@@ -2819,7 +2803,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>85</v>
@@ -2836,7 +2820,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>88</v>
@@ -2853,7 +2837,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>91</v>
@@ -2870,7 +2854,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>94</v>
@@ -2887,7 +2871,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>97</v>
@@ -2904,7 +2888,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>100</v>
@@ -2921,7 +2905,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>103</v>
@@ -2938,7 +2922,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>106</v>
@@ -2955,7 +2939,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>109</v>
@@ -2972,7 +2956,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>112</v>
@@ -2989,7 +2973,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>115</v>
@@ -3003,7 +2987,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>117</v>
@@ -3020,7 +3004,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>120</v>
@@ -3037,7 +3021,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>123</v>
@@ -3054,7 +3038,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>126</v>
@@ -3071,7 +3055,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>129</v>
@@ -3088,7 +3072,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>132</v>
@@ -3105,7 +3089,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>135</v>
@@ -3122,7 +3106,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>138</v>
@@ -3139,7 +3123,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>141</v>
@@ -3156,7 +3140,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>144</v>
@@ -3173,7 +3157,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>147</v>
@@ -3190,7 +3174,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>150</v>
@@ -3207,7 +3191,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>155</v>
@@ -3224,7 +3208,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>156</v>
@@ -3241,16 +3225,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,7 +3242,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>159</v>
@@ -3275,7 +3259,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>164</v>
@@ -3292,7 +3276,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>165</v>
@@ -3309,7 +3293,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>170</v>
@@ -3326,7 +3310,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>171</v>
@@ -3343,7 +3327,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>174</v>
@@ -3360,7 +3344,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>178</v>
@@ -3374,7 +3358,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>179</v>
@@ -3388,7 +3372,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>181</v>
@@ -3405,7 +3389,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>184</v>
@@ -3422,7 +3406,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>187</v>
@@ -3439,7 +3423,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>190</v>
@@ -3456,7 +3440,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>193</v>
@@ -3473,7 +3457,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>198</v>
@@ -3490,7 +3474,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>199</v>
@@ -3507,7 +3491,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>202</v>
@@ -3521,7 +3505,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>204</v>
@@ -3538,7 +3522,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>207</v>
@@ -3555,7 +3539,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>212</v>
@@ -3572,7 +3556,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>213</v>
@@ -3589,7 +3573,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>218</v>
@@ -3606,7 +3590,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>219</v>
@@ -3623,7 +3607,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>224</v>
@@ -3640,7 +3624,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>227</v>
@@ -3657,7 +3641,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>230</v>
@@ -3674,7 +3658,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>233</v>
@@ -3691,7 +3675,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>236</v>
@@ -3708,7 +3692,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>237</v>
@@ -3725,7 +3709,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>242</v>
@@ -3742,7 +3726,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>243</v>
@@ -3759,13 +3743,16 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>251</v>
+        <v>606</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>252</v>
+        <v>607</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3773,16 +3760,16 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3790,13 +3777,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>249</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>248</v>
@@ -3807,16 +3794,16 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3824,16 +3811,16 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3841,16 +3828,16 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3858,16 +3845,16 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3875,16 +3862,16 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3892,16 +3879,16 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3909,16 +3896,16 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3926,16 +3913,16 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3943,16 +3930,16 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3960,16 +3947,16 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3977,13 +3964,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3991,16 +3978,16 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E100" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4008,1092 +3995,1322 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E101" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
-      <c r="B102" s="2"/>
+      <c r="B102" t="s">
+        <v>623</v>
+      </c>
       <c r="C102" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
+      <c r="B103" t="s">
+        <v>623</v>
+      </c>
       <c r="C103" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
+      <c r="B104" t="s">
+        <v>623</v>
+      </c>
       <c r="C104" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E104" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
+      <c r="B105" t="s">
+        <v>623</v>
+      </c>
       <c r="C105" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
+      <c r="B106" t="s">
+        <v>623</v>
+      </c>
       <c r="C106" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E106" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
+      <c r="B107" t="s">
+        <v>623</v>
+      </c>
       <c r="C107" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E107" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
+      <c r="B108" t="s">
+        <v>623</v>
+      </c>
       <c r="C108" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E108" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
+      <c r="B109" t="s">
+        <v>623</v>
+      </c>
       <c r="C109" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
+      <c r="B110" t="s">
+        <v>623</v>
+      </c>
       <c r="C110" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
+      <c r="B111" t="s">
+        <v>623</v>
+      </c>
       <c r="C111" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E111" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
+      <c r="B112" t="s">
+        <v>623</v>
+      </c>
       <c r="C112" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E112" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
+      <c r="B113" t="s">
+        <v>623</v>
+      </c>
       <c r="C113" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E113" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
+      <c r="B114" t="s">
+        <v>623</v>
+      </c>
       <c r="C114" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E114" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
+      <c r="B115" t="s">
+        <v>623</v>
+      </c>
       <c r="C115" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E115" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
+      <c r="B116" t="s">
+        <v>623</v>
+      </c>
       <c r="C116" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
+      <c r="B117" t="s">
+        <v>623</v>
+      </c>
       <c r="C117" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E117" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
+      <c r="B118" t="s">
+        <v>623</v>
+      </c>
       <c r="C118" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
+      <c r="B119" t="s">
+        <v>623</v>
+      </c>
       <c r="C119" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
+      <c r="B120" t="s">
+        <v>623</v>
+      </c>
       <c r="C120" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
+      <c r="B121" t="s">
+        <v>623</v>
+      </c>
       <c r="C121" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
+      <c r="B122" t="s">
+        <v>623</v>
+      </c>
       <c r="C122" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
+      <c r="B123" t="s">
+        <v>623</v>
+      </c>
       <c r="C123" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E123" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
+      <c r="B124" t="s">
+        <v>623</v>
+      </c>
       <c r="C124" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E124" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
+      <c r="B125" t="s">
+        <v>623</v>
+      </c>
       <c r="C125" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E125" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
+      <c r="B126" t="s">
+        <v>623</v>
+      </c>
       <c r="C126" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E126" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
+      <c r="B127" t="s">
+        <v>623</v>
+      </c>
       <c r="C127" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
+      <c r="B128" t="s">
+        <v>623</v>
+      </c>
       <c r="C128" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
+      <c r="B129" t="s">
+        <v>623</v>
+      </c>
       <c r="C129" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E129" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
+      <c r="B130" t="s">
+        <v>623</v>
+      </c>
       <c r="C130" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E130" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
+      <c r="B131" t="s">
+        <v>623</v>
+      </c>
       <c r="C131" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
+      <c r="B132" t="s">
+        <v>623</v>
+      </c>
       <c r="C132" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
+      <c r="B133" t="s">
+        <v>623</v>
+      </c>
       <c r="C133" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E133" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
+      <c r="B134" t="s">
+        <v>623</v>
+      </c>
       <c r="C134" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E134" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
+      <c r="B135" t="s">
+        <v>623</v>
+      </c>
       <c r="C135" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E135" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
+      <c r="B136" t="s">
+        <v>623</v>
+      </c>
       <c r="C136" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E136" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
+      <c r="B137" t="s">
+        <v>623</v>
+      </c>
       <c r="C137" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
+      <c r="B138" t="s">
+        <v>623</v>
+      </c>
       <c r="C138" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E138" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
+      <c r="B139" t="s">
+        <v>623</v>
+      </c>
       <c r="C139" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E139" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
+      <c r="B140" t="s">
+        <v>623</v>
+      </c>
       <c r="C140" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E140" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
+      <c r="B141" t="s">
+        <v>623</v>
+      </c>
       <c r="C141" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
+      <c r="B142" t="s">
+        <v>623</v>
+      </c>
       <c r="C142" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E142" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
+      <c r="B143" t="s">
+        <v>623</v>
+      </c>
       <c r="C143" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E143" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
+      <c r="B144" t="s">
+        <v>623</v>
+      </c>
       <c r="C144" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E144" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
+      <c r="B145" t="s">
+        <v>623</v>
+      </c>
       <c r="C145" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E145" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
+      <c r="B146" t="s">
+        <v>623</v>
+      </c>
       <c r="C146" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="E146" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
+      <c r="B147" t="s">
+        <v>623</v>
+      </c>
       <c r="C147" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E147" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
+      <c r="B148" t="s">
+        <v>623</v>
+      </c>
       <c r="C148" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E148" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
+      <c r="B149" t="s">
+        <v>623</v>
+      </c>
       <c r="C149" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E149" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
+      <c r="B150" t="s">
+        <v>623</v>
+      </c>
       <c r="C150" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E150" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
+      <c r="B151" t="s">
+        <v>623</v>
+      </c>
       <c r="C151" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E151" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
+      <c r="B152" t="s">
+        <v>623</v>
+      </c>
       <c r="C152" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E152" s="1" t="s">
         <v>442</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
+      <c r="B153" t="s">
+        <v>623</v>
+      </c>
       <c r="C153" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
+      <c r="B154" t="s">
+        <v>623</v>
+      </c>
       <c r="C154" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E154" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
+      <c r="B155" t="s">
+        <v>623</v>
+      </c>
       <c r="C155" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="E155" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
+      <c r="B156" t="s">
+        <v>623</v>
+      </c>
       <c r="C156" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E156" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
+      <c r="B157" t="s">
+        <v>623</v>
+      </c>
       <c r="C157" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E157" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
+      <c r="B158" t="s">
+        <v>623</v>
+      </c>
       <c r="C158" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E158" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
+      <c r="B159" t="s">
+        <v>623</v>
+      </c>
       <c r="C159" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E159" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
+      <c r="B160" t="s">
+        <v>623</v>
+      </c>
       <c r="C160" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="E160" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
+      <c r="B161" t="s">
+        <v>623</v>
+      </c>
       <c r="C161" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E161" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
+      <c r="B162" t="s">
+        <v>623</v>
+      </c>
       <c r="C162" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
+      <c r="B163" t="s">
+        <v>623</v>
+      </c>
       <c r="C163" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E163" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
+      <c r="B164" t="s">
+        <v>623</v>
+      </c>
       <c r="C164" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E164" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
+      <c r="B165" t="s">
+        <v>623</v>
+      </c>
       <c r="C165" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E165" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
+      <c r="B166" t="s">
+        <v>623</v>
+      </c>
       <c r="C166" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
+      <c r="B167" t="s">
+        <v>623</v>
+      </c>
       <c r="C167" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E167" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
+      <c r="B168" t="s">
+        <v>623</v>
+      </c>
       <c r="C168" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E168" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
+      <c r="B169" t="s">
+        <v>623</v>
+      </c>
       <c r="C169" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E169" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
+      <c r="B170" t="s">
+        <v>623</v>
+      </c>
       <c r="C170" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E170" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
+      <c r="B171" t="s">
+        <v>623</v>
+      </c>
       <c r="C171" s="1" t="s">
-        <v>499</v>
+        <v>603</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>500</v>
+        <v>604</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>501</v>
+        <v>605</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
+      <c r="B172" t="s">
+        <v>623</v>
+      </c>
       <c r="C172" s="1" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
+      <c r="B173" t="s">
+        <v>623</v>
+      </c>
       <c r="C173" s="1" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
+      <c r="B174" t="s">
+        <v>623</v>
+      </c>
       <c r="C174" s="1" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
+      <c r="B175" t="s">
+        <v>623</v>
+      </c>
       <c r="C175" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
+      <c r="B176" t="s">
+        <v>623</v>
+      </c>
       <c r="C176" s="1" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
+      <c r="B177" t="s">
+        <v>623</v>
+      </c>
       <c r="C177" s="1" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
+      <c r="B178" t="s">
+        <v>623</v>
+      </c>
       <c r="C178" s="1" t="s">
         <v>246</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>247</v>
@@ -5103,434 +5320,493 @@
       <c r="A179">
         <v>178</v>
       </c>
+      <c r="B179" t="s">
+        <v>623</v>
+      </c>
       <c r="C179" s="1" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
+      <c r="B180" t="s">
+        <v>623</v>
+      </c>
       <c r="C180" s="1" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
+      <c r="B181" t="s">
+        <v>623</v>
+      </c>
       <c r="C181" s="1" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
+      <c r="B182" t="s">
+        <v>623</v>
+      </c>
       <c r="C182" s="1" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
+      <c r="B183" t="s">
+        <v>623</v>
+      </c>
       <c r="C183" s="1" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
+      <c r="B184" t="s">
+        <v>623</v>
+      </c>
       <c r="C184" s="1" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
+      <c r="B185" t="s">
+        <v>623</v>
+      </c>
       <c r="C185" s="1" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
+      <c r="B186" t="s">
+        <v>623</v>
+      </c>
       <c r="C186" s="1" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
+      <c r="B187" t="s">
+        <v>623</v>
+      </c>
       <c r="C187" s="1" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
+      <c r="B188" t="s">
+        <v>623</v>
+      </c>
       <c r="C188" s="1" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
+      <c r="B189" t="s">
+        <v>623</v>
+      </c>
       <c r="C189" s="1" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
+      <c r="B190" t="s">
+        <v>623</v>
+      </c>
       <c r="C190" s="1" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
+      <c r="B191" t="s">
+        <v>623</v>
+      </c>
       <c r="C191" s="1" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
+      <c r="B192" t="s">
+        <v>623</v>
+      </c>
       <c r="C192" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
+      <c r="B193" t="s">
+        <v>623</v>
+      </c>
       <c r="C193" s="1" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
+      <c r="B194" t="s">
+        <v>623</v>
+      </c>
       <c r="C194" s="1" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
+      <c r="B195" t="s">
+        <v>623</v>
+      </c>
       <c r="C195" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
+      <c r="B196" t="s">
+        <v>623</v>
+      </c>
       <c r="C196" s="1" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
+      <c r="B197" t="s">
+        <v>623</v>
+      </c>
       <c r="C197" s="1" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
+      <c r="B198" t="s">
+        <v>623</v>
+      </c>
       <c r="C198" s="1" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
+      <c r="B199" t="s">
+        <v>623</v>
+      </c>
       <c r="C199" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
+      <c r="B200" t="s">
+        <v>623</v>
+      </c>
       <c r="C200" s="1" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
+      <c r="B201" t="s">
+        <v>623</v>
+      </c>
       <c r="C201" s="1" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
+      <c r="B202" t="s">
+        <v>623</v>
+      </c>
       <c r="C202" s="1" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
+      <c r="B203" t="s">
+        <v>623</v>
+      </c>
       <c r="C203" s="1" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
+      <c r="B204" t="s">
+        <v>623</v>
+      </c>
       <c r="C204" s="1" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
+      <c r="B205" t="s">
+        <v>623</v>
+      </c>
       <c r="C205" s="1" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
+      <c r="B206" t="s">
+        <v>623</v>
+      </c>
       <c r="C206" s="1" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
+      <c r="B207" t="s">
+        <v>623</v>
+      </c>
       <c r="C207" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208">
-        <v>207</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>609</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209">
-        <v>208</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
     </row>
   </sheetData>
@@ -6015,147 +6291,142 @@
     <hyperlink ref="C170" r:id="rId477" xr:uid="{D9EDA746-00FA-479B-BBF8-E6EA24906B94}"/>
     <hyperlink ref="D170" r:id="rId478" xr:uid="{F2F02B4C-A61F-48DB-B4B9-B590F1EAE1A5}"/>
     <hyperlink ref="E170" r:id="rId479" xr:uid="{4EF3DEB5-F631-42E5-BF23-8FD5BD7C5726}"/>
-    <hyperlink ref="C171" r:id="rId480" xr:uid="{C7AC3295-F2D7-4B73-81FE-CE9DD8908E72}"/>
-    <hyperlink ref="D171" r:id="rId481" xr:uid="{13A8A69F-88CE-42AE-A904-E26015719290}"/>
-    <hyperlink ref="E171" r:id="rId482" xr:uid="{69E9CB21-248F-4A60-986D-523E9D222CCD}"/>
-    <hyperlink ref="C172" r:id="rId483" xr:uid="{7627DCB7-8878-43A8-B6E9-AA0B9A8AA69D}"/>
-    <hyperlink ref="D172" r:id="rId484" xr:uid="{FCCBB0CF-B9DD-4759-BBA3-76BD72CDE47E}"/>
-    <hyperlink ref="E172" r:id="rId485" xr:uid="{3E811DA2-3C40-4364-9266-6773CDEE5611}"/>
-    <hyperlink ref="C173" r:id="rId486" xr:uid="{FC27C7F6-56D3-4353-B218-AEDBD69411BE}"/>
-    <hyperlink ref="D173" r:id="rId487" xr:uid="{1FAEEA19-C0F2-4B64-AB53-5CE1FCFD3EED}"/>
-    <hyperlink ref="E173" r:id="rId488" xr:uid="{9AFEB9F6-C42C-4F69-BAB9-0F96228BAB75}"/>
-    <hyperlink ref="C174" r:id="rId489" xr:uid="{782E6140-94C3-407F-BEAF-9C0D976620EB}"/>
-    <hyperlink ref="D174" r:id="rId490" xr:uid="{B6A4BB4A-CEE1-4126-85FD-8A0A92A86F6C}"/>
-    <hyperlink ref="E174" r:id="rId491" xr:uid="{4DE847BB-899E-400F-B0A1-5368BD326435}"/>
-    <hyperlink ref="C175" r:id="rId492" xr:uid="{550B60D7-37BE-42DF-A0A6-234EE2ABEC88}"/>
-    <hyperlink ref="D175" r:id="rId493" xr:uid="{FE54EAA5-5BCB-4AE8-B0F0-DF219D75D2FA}"/>
-    <hyperlink ref="E175" r:id="rId494" xr:uid="{5F404BDE-7004-4B15-8063-6FFDD0232C10}"/>
-    <hyperlink ref="D176" r:id="rId495" xr:uid="{04847EC6-CA8E-40B5-A255-4AA69821E9CD}"/>
-    <hyperlink ref="E176" r:id="rId496" xr:uid="{C5321455-60AF-4B1F-B2EB-9C48ABE6CF88}"/>
-    <hyperlink ref="C176" r:id="rId497" xr:uid="{F487FA1F-6345-4747-9B2D-E8B2F3CA8F64}"/>
-    <hyperlink ref="C177" r:id="rId498" xr:uid="{0BB76D84-05E9-403F-B67C-C3BFFCCC1DE9}"/>
-    <hyperlink ref="D177" r:id="rId499" xr:uid="{E68DE772-C262-43D4-BAB1-57B7508710F5}"/>
-    <hyperlink ref="E177" r:id="rId500" xr:uid="{E2FD5107-217F-4912-8F1C-CBCA0456D0B1}"/>
-    <hyperlink ref="C178" r:id="rId501" xr:uid="{0709A472-9980-4F85-A449-8A5D6EABD5F4}"/>
-    <hyperlink ref="D178" r:id="rId502" xr:uid="{31C86E75-E56D-4C5A-965A-002F4B567CEA}"/>
-    <hyperlink ref="E178" r:id="rId503" xr:uid="{A44C8FE0-0122-4430-BB7B-95FC5AC20FD1}"/>
-    <hyperlink ref="C179" r:id="rId504" xr:uid="{6CA3E827-405F-40BE-9BA0-7F75BE64C3EF}"/>
-    <hyperlink ref="D179" r:id="rId505" xr:uid="{1AB16091-69AE-4105-9BA6-B775B46361F8}"/>
-    <hyperlink ref="E179" r:id="rId506" xr:uid="{2B7A126E-8D1B-4E8F-93A6-C98453F4B0CD}"/>
-    <hyperlink ref="C180" r:id="rId507" xr:uid="{FF9DC8D1-E300-4D00-8478-B4C4465463B0}"/>
-    <hyperlink ref="D180" r:id="rId508" xr:uid="{C7FB4928-100E-4F31-AA8B-9BB5386BD6E2}"/>
-    <hyperlink ref="E180" r:id="rId509" xr:uid="{33E88EF2-069C-4A8A-A4B9-407D561D9FA7}"/>
-    <hyperlink ref="C181" r:id="rId510" xr:uid="{AD27F6F9-722F-4772-BAD3-292259E599AE}"/>
-    <hyperlink ref="D181" r:id="rId511" xr:uid="{9855AD87-CCE8-4B4A-9D90-654E9CB9A884}"/>
-    <hyperlink ref="E181" r:id="rId512" xr:uid="{DABA9FDA-64E2-49EB-A86C-6A285B8ED457}"/>
-    <hyperlink ref="C182" r:id="rId513" xr:uid="{08DC194C-ADC7-4BD9-B1FA-D02B1EB30413}"/>
-    <hyperlink ref="D182" r:id="rId514" xr:uid="{BDCC0E77-3EA0-4F00-B40F-EB3744C4B10A}"/>
-    <hyperlink ref="E182" r:id="rId515" xr:uid="{0C11EA0B-B2D0-438E-81C0-C400F6D0799A}"/>
-    <hyperlink ref="C183" r:id="rId516" xr:uid="{13991465-B6B8-432B-B460-78ABB1DED868}"/>
-    <hyperlink ref="D183" r:id="rId517" xr:uid="{A036A9F5-033D-4A23-B1E3-B321FB1A1D5C}"/>
-    <hyperlink ref="E183" r:id="rId518" xr:uid="{D1FD862C-B5D6-4B13-931B-57B7FFF1059A}"/>
-    <hyperlink ref="C184" r:id="rId519" xr:uid="{5217B7E5-50F7-4581-9109-F6A8BC875186}"/>
-    <hyperlink ref="D184" r:id="rId520" xr:uid="{C3F790CF-A478-40B7-99F6-7D2667CBC146}"/>
-    <hyperlink ref="E184" r:id="rId521" xr:uid="{A5F80E79-506C-4A15-AACD-68F53D61E373}"/>
-    <hyperlink ref="C185" r:id="rId522" xr:uid="{62E029C0-61D3-4187-A49A-6F8E847B07E9}"/>
-    <hyperlink ref="D185" r:id="rId523" xr:uid="{682FAA6B-7ADD-4D0B-9D48-124102D3B8C4}"/>
-    <hyperlink ref="E185" r:id="rId524" xr:uid="{CB64775F-93CB-4F3C-A7B2-61AA1EEC9FF4}"/>
-    <hyperlink ref="D186" r:id="rId525" xr:uid="{33DB2910-4B9B-4EBD-94DB-9D1D8BA1A60A}"/>
-    <hyperlink ref="E186" r:id="rId526" xr:uid="{D816F0E8-5CA4-4FBA-A574-65EB5C502159}"/>
-    <hyperlink ref="C186" r:id="rId527" xr:uid="{7BED455F-4DC7-4B45-AD26-E1286840DEBE}"/>
-    <hyperlink ref="C187" r:id="rId528" xr:uid="{B17E7A06-B7A3-43DE-959C-80217F4C7404}"/>
-    <hyperlink ref="D187" r:id="rId529" xr:uid="{108A2D11-51B8-4F46-B0AE-357FA3F6BDB6}"/>
-    <hyperlink ref="E187" r:id="rId530" xr:uid="{16666982-1A83-4A62-BFC7-C4F40E6C916E}"/>
-    <hyperlink ref="C188" r:id="rId531" xr:uid="{053DBA08-46A7-4A97-9457-F0E304824F8E}"/>
-    <hyperlink ref="D188" r:id="rId532" xr:uid="{DB4ECA15-195B-4A54-858F-239BA708B125}"/>
-    <hyperlink ref="E188" r:id="rId533" xr:uid="{17CC691E-0C7E-443C-B3E1-54C8BFC12D95}"/>
-    <hyperlink ref="C189" r:id="rId534" xr:uid="{488BAF16-AD49-4FAE-8E4C-CE7962082CBA}"/>
-    <hyperlink ref="D189" r:id="rId535" xr:uid="{0B038405-DDEA-461D-994B-7F271E9120F4}"/>
-    <hyperlink ref="E189" r:id="rId536" xr:uid="{7BACCCB4-5CF4-4224-9201-E647233DE274}"/>
-    <hyperlink ref="C190" r:id="rId537" xr:uid="{E9108E47-563C-4F4D-8B1F-CB863619C501}"/>
-    <hyperlink ref="D190" r:id="rId538" xr:uid="{ECB18330-35A1-421E-8B98-A38AB1F12F4B}"/>
-    <hyperlink ref="E190" r:id="rId539" xr:uid="{594B3616-5B4C-4902-90E8-B56CF4ADD901}"/>
-    <hyperlink ref="C191" r:id="rId540" xr:uid="{BEC6DA00-205E-4FA8-BF78-644278A12620}"/>
-    <hyperlink ref="D191" r:id="rId541" xr:uid="{66E4959D-D2E5-40E0-9A50-3E9722C83879}"/>
-    <hyperlink ref="E191" r:id="rId542" xr:uid="{165E3072-0F8C-4D07-A8EE-AFB2E92D10D0}"/>
-    <hyperlink ref="C192" r:id="rId543" xr:uid="{8BDFFA66-526B-49E6-A9EF-74BACEF2FC3A}"/>
-    <hyperlink ref="D192" r:id="rId544" xr:uid="{23452AE3-198E-4555-8556-92D1EB9C8F2F}"/>
-    <hyperlink ref="E192" r:id="rId545" xr:uid="{1C8BB96E-E2D2-41A2-B51E-CA1C94882C45}"/>
-    <hyperlink ref="C193" r:id="rId546" xr:uid="{78499224-1133-4CA4-8141-97A18D48B873}"/>
-    <hyperlink ref="D193" r:id="rId547" xr:uid="{B9B02DD2-D017-4DBC-9327-5DF3E8B353CB}"/>
-    <hyperlink ref="E193" r:id="rId548" xr:uid="{4CDCE363-4F15-4C8E-88A0-16B4ACE31706}"/>
-    <hyperlink ref="D194" r:id="rId549" xr:uid="{9672DF3D-1B42-4B06-BE7E-8C371290DDD8}"/>
-    <hyperlink ref="E194" r:id="rId550" xr:uid="{A6A6609E-1ACE-4AE1-8630-67EC2A09BB1B}"/>
-    <hyperlink ref="C194" r:id="rId551" xr:uid="{2945D925-89ED-4A50-9C8A-33FAE3D9B663}"/>
-    <hyperlink ref="C195" r:id="rId552" xr:uid="{B2232121-8FC5-4AFB-B4A5-EAFCA6F8BF55}"/>
-    <hyperlink ref="D195" r:id="rId553" xr:uid="{BDB9895C-3A01-437E-B535-262F78163F79}"/>
-    <hyperlink ref="E195" r:id="rId554" xr:uid="{7E8CB580-3C77-4108-A7BB-241E5DD2F8F8}"/>
-    <hyperlink ref="C196" r:id="rId555" xr:uid="{0E762398-C5ED-49DE-9BD7-D01671B4E18A}"/>
-    <hyperlink ref="D196" r:id="rId556" xr:uid="{7FC49659-FA8F-434A-B4B6-95508B1B4D35}"/>
-    <hyperlink ref="E196" r:id="rId557" xr:uid="{5FD4642D-66C0-4BCC-9C59-E55B95CFBFBB}"/>
-    <hyperlink ref="C197" r:id="rId558" xr:uid="{63BBE702-55C8-4458-8A67-C5591C5F9247}"/>
-    <hyperlink ref="D197" r:id="rId559" xr:uid="{A666B7EF-0CBD-4183-BF04-FD5B6DDCF6FD}"/>
-    <hyperlink ref="D99" r:id="rId560" xr:uid="{BB5402C0-11CF-4FB7-9D11-E4E06DA8E09D}"/>
-    <hyperlink ref="C99" r:id="rId561" xr:uid="{5098A259-C902-4545-A7E1-E636AB33D5F8}"/>
-    <hyperlink ref="D86" r:id="rId562" display="https://www.camara.leg.br/internet/sitaqweb/TextoHTML.asp?etapa=11&amp;tpReuniaoEvento=AP%20c/%20Convidado&amp;dtReuniao=15/08/2017&amp;hrInicio=14:50:00&amp;hrFim=17:12:00&amp;origemDiscurso=&amp;nmLocal=Plen%C3%A1rio%20Principal%20-%20CD&amp;nuSessao=1047/17&amp;nuQuarto=0&amp;nuOrador=0&amp;nuInsercao=0&amp;dtHorarioQuarto=14:50&amp;sgFaseSessao=&amp;Data=15/08/2017&amp;txApelido=&amp;txFaseSessao=&amp;txTipoSessao=Permanente&amp;dtHoraQuarto=14:50&amp;txEtapa=" xr:uid="{885EDDC5-59F7-4E1C-AF16-381A4A38D774}"/>
-    <hyperlink ref="C86" r:id="rId563" xr:uid="{4A17DC70-EC44-4004-B071-6F5D899C8CA5}"/>
-    <hyperlink ref="D71" r:id="rId564" xr:uid="{D677B959-EB3C-4DDB-8AEF-E8EAE6D6D45E}"/>
-    <hyperlink ref="C71" r:id="rId565" xr:uid="{0AD8437A-2704-40CD-866A-26901C1B53CE}"/>
-    <hyperlink ref="D63" r:id="rId566" xr:uid="{5F59921F-E727-4A1F-AE6F-37476A2F81C2}"/>
-    <hyperlink ref="C63" r:id="rId567" xr:uid="{4B817215-AB66-422A-B2EE-745DCCE2715E}"/>
-    <hyperlink ref="C62" r:id="rId568" xr:uid="{2DA64800-7A72-4482-919D-DFF1D13D4B55}"/>
-    <hyperlink ref="D62" r:id="rId569" xr:uid="{E8EC2437-F030-4E8C-B6AC-917AA71D6D2D}"/>
-    <hyperlink ref="D40" r:id="rId570" xr:uid="{6C41F5BF-C09E-47D4-A816-D0E540BD6149}"/>
-    <hyperlink ref="C40" r:id="rId571" xr:uid="{CBA2CB5F-E42B-4632-83EE-22826ADE1E04}"/>
-    <hyperlink ref="E197" r:id="rId572" xr:uid="{136FF705-8DCE-4116-BE70-5F1542A088B0}"/>
-    <hyperlink ref="C198" r:id="rId573" xr:uid="{3FB904D1-0936-422F-96AB-F3B96921D779}"/>
-    <hyperlink ref="D198" r:id="rId574" xr:uid="{7A54B018-01DB-4819-9FD1-68863145C0A1}"/>
-    <hyperlink ref="E198" r:id="rId575" xr:uid="{E3C9E074-5A18-4A4E-8CA3-EEB4F330DFC6}"/>
-    <hyperlink ref="C199" r:id="rId576" xr:uid="{E2D42ECE-DCF2-4092-B7EF-C717EECA06D7}"/>
-    <hyperlink ref="D199" r:id="rId577" xr:uid="{D3B0D91F-A5F5-489B-B4BF-5B6ADA49D078}"/>
-    <hyperlink ref="E199" r:id="rId578" xr:uid="{9E3CF267-2270-4A5E-BF99-A49458146C5C}"/>
-    <hyperlink ref="C200" r:id="rId579" xr:uid="{39D382AA-57C1-42F8-ABF7-11A7F0B35567}"/>
-    <hyperlink ref="D200" r:id="rId580" xr:uid="{8CE8A2BD-98A2-45D9-B373-7C90E69ADB93}"/>
-    <hyperlink ref="E200" r:id="rId581" xr:uid="{DE229DE6-DE64-42DD-97A1-D38A12923FD3}"/>
-    <hyperlink ref="C201" r:id="rId582" xr:uid="{189D0765-1C92-4FC1-A376-28B52EA2BFAF}"/>
-    <hyperlink ref="D201" r:id="rId583" xr:uid="{2532C84C-8DB5-4D9F-8FFB-F09727EC3D64}"/>
-    <hyperlink ref="E201" r:id="rId584" xr:uid="{A9C00FED-2E5B-4151-A8D6-2CBF429036A5}"/>
-    <hyperlink ref="C202" r:id="rId585" xr:uid="{0FB758F3-8CEC-44F8-AB0B-FB5749251F72}"/>
-    <hyperlink ref="D202" r:id="rId586" xr:uid="{14790960-D653-4274-8C1A-87D26826D0D0}"/>
-    <hyperlink ref="E202" r:id="rId587" xr:uid="{669AE71B-0710-4E47-9B20-28C6E0D2A24C}"/>
-    <hyperlink ref="C203" r:id="rId588" xr:uid="{6C1C977A-8104-4C5D-BED7-C833FD88FC10}"/>
-    <hyperlink ref="D203" r:id="rId589" xr:uid="{FA52D527-723E-449E-AE77-53A711E8B5F4}"/>
-    <hyperlink ref="E203" r:id="rId590" xr:uid="{7D40609C-37B6-4DA5-86FD-A779CCE9CF33}"/>
-    <hyperlink ref="D204" r:id="rId591" xr:uid="{E1F2A5BF-32A9-48D5-81EE-19ABF3643DD2}"/>
-    <hyperlink ref="E204" r:id="rId592" xr:uid="{E561AB7E-F883-4B46-9BD4-A1A7658BB442}"/>
-    <hyperlink ref="C204" r:id="rId593" xr:uid="{0B823933-67DE-41F8-B9F5-D78FB031387C}"/>
-    <hyperlink ref="C205" r:id="rId594" xr:uid="{26F9A583-2496-4B17-A929-300CBDA2E24D}"/>
-    <hyperlink ref="D205" r:id="rId595" xr:uid="{6719EDC2-583C-49D3-9ECA-9AAEAB5A1AF8}"/>
-    <hyperlink ref="E205" r:id="rId596" xr:uid="{3243DF7A-EE24-42C4-9051-EF34793BE812}"/>
-    <hyperlink ref="C206" r:id="rId597" xr:uid="{4C45050E-CAB2-4E91-876A-26ACF94DB8B2}"/>
-    <hyperlink ref="D206" r:id="rId598" xr:uid="{4FE2A5B0-C928-4394-8042-D3AA021DA4D8}"/>
-    <hyperlink ref="E206" r:id="rId599" xr:uid="{CAB1117F-895B-408D-BFB0-CC8642447B67}"/>
-    <hyperlink ref="C207" r:id="rId600" xr:uid="{3497FE2B-F080-4F0F-9454-A2F8E2BCEA79}"/>
-    <hyperlink ref="D207" r:id="rId601" xr:uid="{C1B80CC4-8153-4B20-A3F2-B283168811C5}"/>
-    <hyperlink ref="E207" r:id="rId602" xr:uid="{BF0434BE-354E-4789-9E21-F298661908C9}"/>
-    <hyperlink ref="C208" r:id="rId603" xr:uid="{E432FEE7-0CE3-4671-A6DE-A89067FE71F8}"/>
-    <hyperlink ref="D208" r:id="rId604" xr:uid="{9B118C1B-E5E7-4F47-BFA5-206491EA6ED8}"/>
-    <hyperlink ref="E208" r:id="rId605" xr:uid="{9EA9596A-CB3D-4B30-8E07-CA8A3FF7C508}"/>
-    <hyperlink ref="C209" r:id="rId606" xr:uid="{46C6222B-B670-40C3-A605-FABE1731989A}"/>
-    <hyperlink ref="D209" r:id="rId607" xr:uid="{C653707F-D543-43CC-A01D-24A54A6A319B}"/>
-    <hyperlink ref="E209" r:id="rId608" xr:uid="{60116EA4-2834-4C7A-B4DB-1CE223CB90BB}"/>
-    <hyperlink ref="C96" r:id="rId609" xr:uid="{20EC698E-A69F-497B-8D14-1C5CA444BC21}"/>
-    <hyperlink ref="D96" r:id="rId610" xr:uid="{AFAB7C9A-C544-47BD-8645-5C31CE7C5CF3}"/>
-    <hyperlink ref="E96" r:id="rId611" xr:uid="{F53AF2AB-0CE9-45A6-B905-24C7FEEA3E52}"/>
-    <hyperlink ref="C95" r:id="rId612" xr:uid="{30CD9287-A385-456E-9D5E-59944E3156E1}"/>
-    <hyperlink ref="D95" r:id="rId613" xr:uid="{C9FDF5BB-9B0E-442F-AE18-EBCAF9FA12BA}"/>
-    <hyperlink ref="E95" r:id="rId614" xr:uid="{E3661C98-D989-4879-A8FC-B6166662C8D7}"/>
-    <hyperlink ref="C55" r:id="rId615" xr:uid="{2102EDB4-6981-4633-9FD3-E647448181FC}"/>
-    <hyperlink ref="D55" r:id="rId616" xr:uid="{0DB9D726-23FB-4B78-94AC-DFD7B21AB5AE}"/>
-    <hyperlink ref="E55" r:id="rId617" xr:uid="{BF7B36EC-2642-4F9B-A942-FC7DA39117FB}"/>
+    <hyperlink ref="C172" r:id="rId480" xr:uid="{7627DCB7-8878-43A8-B6E9-AA0B9A8AA69D}"/>
+    <hyperlink ref="D172" r:id="rId481" xr:uid="{FCCBB0CF-B9DD-4759-BBA3-76BD72CDE47E}"/>
+    <hyperlink ref="E172" r:id="rId482" xr:uid="{3E811DA2-3C40-4364-9266-6773CDEE5611}"/>
+    <hyperlink ref="C173" r:id="rId483" xr:uid="{FC27C7F6-56D3-4353-B218-AEDBD69411BE}"/>
+    <hyperlink ref="D173" r:id="rId484" xr:uid="{1FAEEA19-C0F2-4B64-AB53-5CE1FCFD3EED}"/>
+    <hyperlink ref="E173" r:id="rId485" xr:uid="{9AFEB9F6-C42C-4F69-BAB9-0F96228BAB75}"/>
+    <hyperlink ref="C174" r:id="rId486" xr:uid="{782E6140-94C3-407F-BEAF-9C0D976620EB}"/>
+    <hyperlink ref="D174" r:id="rId487" xr:uid="{B6A4BB4A-CEE1-4126-85FD-8A0A92A86F6C}"/>
+    <hyperlink ref="E174" r:id="rId488" xr:uid="{4DE847BB-899E-400F-B0A1-5368BD326435}"/>
+    <hyperlink ref="C175" r:id="rId489" xr:uid="{550B60D7-37BE-42DF-A0A6-234EE2ABEC88}"/>
+    <hyperlink ref="D175" r:id="rId490" xr:uid="{FE54EAA5-5BCB-4AE8-B0F0-DF219D75D2FA}"/>
+    <hyperlink ref="E175" r:id="rId491" xr:uid="{5F404BDE-7004-4B15-8063-6FFDD0232C10}"/>
+    <hyperlink ref="D176" r:id="rId492" xr:uid="{04847EC6-CA8E-40B5-A255-4AA69821E9CD}"/>
+    <hyperlink ref="E176" r:id="rId493" xr:uid="{C5321455-60AF-4B1F-B2EB-9C48ABE6CF88}"/>
+    <hyperlink ref="C176" r:id="rId494" xr:uid="{F487FA1F-6345-4747-9B2D-E8B2F3CA8F64}"/>
+    <hyperlink ref="C177" r:id="rId495" xr:uid="{0BB76D84-05E9-403F-B67C-C3BFFCCC1DE9}"/>
+    <hyperlink ref="D177" r:id="rId496" xr:uid="{E68DE772-C262-43D4-BAB1-57B7508710F5}"/>
+    <hyperlink ref="E177" r:id="rId497" xr:uid="{E2FD5107-217F-4912-8F1C-CBCA0456D0B1}"/>
+    <hyperlink ref="C178" r:id="rId498" xr:uid="{0709A472-9980-4F85-A449-8A5D6EABD5F4}"/>
+    <hyperlink ref="D178" r:id="rId499" xr:uid="{31C86E75-E56D-4C5A-965A-002F4B567CEA}"/>
+    <hyperlink ref="E178" r:id="rId500" xr:uid="{A44C8FE0-0122-4430-BB7B-95FC5AC20FD1}"/>
+    <hyperlink ref="C179" r:id="rId501" xr:uid="{6CA3E827-405F-40BE-9BA0-7F75BE64C3EF}"/>
+    <hyperlink ref="D179" r:id="rId502" xr:uid="{1AB16091-69AE-4105-9BA6-B775B46361F8}"/>
+    <hyperlink ref="E179" r:id="rId503" xr:uid="{2B7A126E-8D1B-4E8F-93A6-C98453F4B0CD}"/>
+    <hyperlink ref="C180" r:id="rId504" xr:uid="{FF9DC8D1-E300-4D00-8478-B4C4465463B0}"/>
+    <hyperlink ref="D180" r:id="rId505" xr:uid="{C7FB4928-100E-4F31-AA8B-9BB5386BD6E2}"/>
+    <hyperlink ref="E180" r:id="rId506" xr:uid="{33E88EF2-069C-4A8A-A4B9-407D561D9FA7}"/>
+    <hyperlink ref="C181" r:id="rId507" xr:uid="{AD27F6F9-722F-4772-BAD3-292259E599AE}"/>
+    <hyperlink ref="D181" r:id="rId508" xr:uid="{9855AD87-CCE8-4B4A-9D90-654E9CB9A884}"/>
+    <hyperlink ref="E181" r:id="rId509" xr:uid="{DABA9FDA-64E2-49EB-A86C-6A285B8ED457}"/>
+    <hyperlink ref="C182" r:id="rId510" xr:uid="{08DC194C-ADC7-4BD9-B1FA-D02B1EB30413}"/>
+    <hyperlink ref="D182" r:id="rId511" xr:uid="{BDCC0E77-3EA0-4F00-B40F-EB3744C4B10A}"/>
+    <hyperlink ref="E182" r:id="rId512" xr:uid="{0C11EA0B-B2D0-438E-81C0-C400F6D0799A}"/>
+    <hyperlink ref="C183" r:id="rId513" xr:uid="{13991465-B6B8-432B-B460-78ABB1DED868}"/>
+    <hyperlink ref="D183" r:id="rId514" xr:uid="{A036A9F5-033D-4A23-B1E3-B321FB1A1D5C}"/>
+    <hyperlink ref="E183" r:id="rId515" xr:uid="{D1FD862C-B5D6-4B13-931B-57B7FFF1059A}"/>
+    <hyperlink ref="C184" r:id="rId516" xr:uid="{5217B7E5-50F7-4581-9109-F6A8BC875186}"/>
+    <hyperlink ref="D184" r:id="rId517" xr:uid="{C3F790CF-A478-40B7-99F6-7D2667CBC146}"/>
+    <hyperlink ref="E184" r:id="rId518" xr:uid="{A5F80E79-506C-4A15-AACD-68F53D61E373}"/>
+    <hyperlink ref="C185" r:id="rId519" xr:uid="{62E029C0-61D3-4187-A49A-6F8E847B07E9}"/>
+    <hyperlink ref="D185" r:id="rId520" xr:uid="{682FAA6B-7ADD-4D0B-9D48-124102D3B8C4}"/>
+    <hyperlink ref="E185" r:id="rId521" xr:uid="{CB64775F-93CB-4F3C-A7B2-61AA1EEC9FF4}"/>
+    <hyperlink ref="D186" r:id="rId522" xr:uid="{33DB2910-4B9B-4EBD-94DB-9D1D8BA1A60A}"/>
+    <hyperlink ref="E186" r:id="rId523" xr:uid="{D816F0E8-5CA4-4FBA-A574-65EB5C502159}"/>
+    <hyperlink ref="C186" r:id="rId524" xr:uid="{7BED455F-4DC7-4B45-AD26-E1286840DEBE}"/>
+    <hyperlink ref="C187" r:id="rId525" xr:uid="{B17E7A06-B7A3-43DE-959C-80217F4C7404}"/>
+    <hyperlink ref="D187" r:id="rId526" xr:uid="{108A2D11-51B8-4F46-B0AE-357FA3F6BDB6}"/>
+    <hyperlink ref="E187" r:id="rId527" xr:uid="{16666982-1A83-4A62-BFC7-C4F40E6C916E}"/>
+    <hyperlink ref="C188" r:id="rId528" xr:uid="{053DBA08-46A7-4A97-9457-F0E304824F8E}"/>
+    <hyperlink ref="D188" r:id="rId529" xr:uid="{DB4ECA15-195B-4A54-858F-239BA708B125}"/>
+    <hyperlink ref="E188" r:id="rId530" xr:uid="{17CC691E-0C7E-443C-B3E1-54C8BFC12D95}"/>
+    <hyperlink ref="C189" r:id="rId531" xr:uid="{488BAF16-AD49-4FAE-8E4C-CE7962082CBA}"/>
+    <hyperlink ref="D189" r:id="rId532" xr:uid="{0B038405-DDEA-461D-994B-7F271E9120F4}"/>
+    <hyperlink ref="E189" r:id="rId533" xr:uid="{7BACCCB4-5CF4-4224-9201-E647233DE274}"/>
+    <hyperlink ref="C190" r:id="rId534" xr:uid="{E9108E47-563C-4F4D-8B1F-CB863619C501}"/>
+    <hyperlink ref="D190" r:id="rId535" xr:uid="{ECB18330-35A1-421E-8B98-A38AB1F12F4B}"/>
+    <hyperlink ref="E190" r:id="rId536" xr:uid="{594B3616-5B4C-4902-90E8-B56CF4ADD901}"/>
+    <hyperlink ref="C191" r:id="rId537" xr:uid="{BEC6DA00-205E-4FA8-BF78-644278A12620}"/>
+    <hyperlink ref="D191" r:id="rId538" xr:uid="{66E4959D-D2E5-40E0-9A50-3E9722C83879}"/>
+    <hyperlink ref="E191" r:id="rId539" xr:uid="{165E3072-0F8C-4D07-A8EE-AFB2E92D10D0}"/>
+    <hyperlink ref="C192" r:id="rId540" xr:uid="{8BDFFA66-526B-49E6-A9EF-74BACEF2FC3A}"/>
+    <hyperlink ref="D192" r:id="rId541" xr:uid="{23452AE3-198E-4555-8556-92D1EB9C8F2F}"/>
+    <hyperlink ref="E192" r:id="rId542" xr:uid="{1C8BB96E-E2D2-41A2-B51E-CA1C94882C45}"/>
+    <hyperlink ref="C193" r:id="rId543" xr:uid="{78499224-1133-4CA4-8141-97A18D48B873}"/>
+    <hyperlink ref="D193" r:id="rId544" xr:uid="{B9B02DD2-D017-4DBC-9327-5DF3E8B353CB}"/>
+    <hyperlink ref="E193" r:id="rId545" xr:uid="{4CDCE363-4F15-4C8E-88A0-16B4ACE31706}"/>
+    <hyperlink ref="D194" r:id="rId546" xr:uid="{9672DF3D-1B42-4B06-BE7E-8C371290DDD8}"/>
+    <hyperlink ref="E194" r:id="rId547" xr:uid="{A6A6609E-1ACE-4AE1-8630-67EC2A09BB1B}"/>
+    <hyperlink ref="C194" r:id="rId548" xr:uid="{2945D925-89ED-4A50-9C8A-33FAE3D9B663}"/>
+    <hyperlink ref="C195" r:id="rId549" xr:uid="{B2232121-8FC5-4AFB-B4A5-EAFCA6F8BF55}"/>
+    <hyperlink ref="D195" r:id="rId550" xr:uid="{BDB9895C-3A01-437E-B535-262F78163F79}"/>
+    <hyperlink ref="E195" r:id="rId551" xr:uid="{7E8CB580-3C77-4108-A7BB-241E5DD2F8F8}"/>
+    <hyperlink ref="C196" r:id="rId552" xr:uid="{0E762398-C5ED-49DE-9BD7-D01671B4E18A}"/>
+    <hyperlink ref="D196" r:id="rId553" xr:uid="{7FC49659-FA8F-434A-B4B6-95508B1B4D35}"/>
+    <hyperlink ref="E196" r:id="rId554" xr:uid="{5FD4642D-66C0-4BCC-9C59-E55B95CFBFBB}"/>
+    <hyperlink ref="C197" r:id="rId555" xr:uid="{63BBE702-55C8-4458-8A67-C5591C5F9247}"/>
+    <hyperlink ref="D197" r:id="rId556" xr:uid="{A666B7EF-0CBD-4183-BF04-FD5B6DDCF6FD}"/>
+    <hyperlink ref="D99" r:id="rId557" xr:uid="{BB5402C0-11CF-4FB7-9D11-E4E06DA8E09D}"/>
+    <hyperlink ref="C99" r:id="rId558" xr:uid="{5098A259-C902-4545-A7E1-E636AB33D5F8}"/>
+    <hyperlink ref="D71" r:id="rId559" xr:uid="{D677B959-EB3C-4DDB-8AEF-E8EAE6D6D45E}"/>
+    <hyperlink ref="C71" r:id="rId560" xr:uid="{0AD8437A-2704-40CD-866A-26901C1B53CE}"/>
+    <hyperlink ref="D63" r:id="rId561" xr:uid="{5F59921F-E727-4A1F-AE6F-37476A2F81C2}"/>
+    <hyperlink ref="C63" r:id="rId562" xr:uid="{4B817215-AB66-422A-B2EE-745DCCE2715E}"/>
+    <hyperlink ref="C62" r:id="rId563" xr:uid="{2DA64800-7A72-4482-919D-DFF1D13D4B55}"/>
+    <hyperlink ref="D62" r:id="rId564" xr:uid="{E8EC2437-F030-4E8C-B6AC-917AA71D6D2D}"/>
+    <hyperlink ref="D40" r:id="rId565" xr:uid="{6C41F5BF-C09E-47D4-A816-D0E540BD6149}"/>
+    <hyperlink ref="C40" r:id="rId566" xr:uid="{CBA2CB5F-E42B-4632-83EE-22826ADE1E04}"/>
+    <hyperlink ref="E197" r:id="rId567" xr:uid="{136FF705-8DCE-4116-BE70-5F1542A088B0}"/>
+    <hyperlink ref="C198" r:id="rId568" xr:uid="{3FB904D1-0936-422F-96AB-F3B96921D779}"/>
+    <hyperlink ref="D198" r:id="rId569" xr:uid="{7A54B018-01DB-4819-9FD1-68863145C0A1}"/>
+    <hyperlink ref="E198" r:id="rId570" xr:uid="{E3C9E074-5A18-4A4E-8CA3-EEB4F330DFC6}"/>
+    <hyperlink ref="C199" r:id="rId571" xr:uid="{E2D42ECE-DCF2-4092-B7EF-C717EECA06D7}"/>
+    <hyperlink ref="D199" r:id="rId572" xr:uid="{D3B0D91F-A5F5-489B-B4BF-5B6ADA49D078}"/>
+    <hyperlink ref="E199" r:id="rId573" xr:uid="{9E3CF267-2270-4A5E-BF99-A49458146C5C}"/>
+    <hyperlink ref="C200" r:id="rId574" xr:uid="{39D382AA-57C1-42F8-ABF7-11A7F0B35567}"/>
+    <hyperlink ref="D200" r:id="rId575" xr:uid="{8CE8A2BD-98A2-45D9-B373-7C90E69ADB93}"/>
+    <hyperlink ref="E200" r:id="rId576" xr:uid="{DE229DE6-DE64-42DD-97A1-D38A12923FD3}"/>
+    <hyperlink ref="C201" r:id="rId577" xr:uid="{189D0765-1C92-4FC1-A376-28B52EA2BFAF}"/>
+    <hyperlink ref="D201" r:id="rId578" xr:uid="{2532C84C-8DB5-4D9F-8FFB-F09727EC3D64}"/>
+    <hyperlink ref="E201" r:id="rId579" xr:uid="{A9C00FED-2E5B-4151-A8D6-2CBF429036A5}"/>
+    <hyperlink ref="C202" r:id="rId580" xr:uid="{0FB758F3-8CEC-44F8-AB0B-FB5749251F72}"/>
+    <hyperlink ref="D202" r:id="rId581" xr:uid="{14790960-D653-4274-8C1A-87D26826D0D0}"/>
+    <hyperlink ref="E202" r:id="rId582" xr:uid="{669AE71B-0710-4E47-9B20-28C6E0D2A24C}"/>
+    <hyperlink ref="C203" r:id="rId583" xr:uid="{6C1C977A-8104-4C5D-BED7-C833FD88FC10}"/>
+    <hyperlink ref="D203" r:id="rId584" xr:uid="{FA52D527-723E-449E-AE77-53A711E8B5F4}"/>
+    <hyperlink ref="E203" r:id="rId585" xr:uid="{7D40609C-37B6-4DA5-86FD-A779CCE9CF33}"/>
+    <hyperlink ref="D204" r:id="rId586" xr:uid="{E1F2A5BF-32A9-48D5-81EE-19ABF3643DD2}"/>
+    <hyperlink ref="E204" r:id="rId587" xr:uid="{E561AB7E-F883-4B46-9BD4-A1A7658BB442}"/>
+    <hyperlink ref="C204" r:id="rId588" xr:uid="{0B823933-67DE-41F8-B9F5-D78FB031387C}"/>
+    <hyperlink ref="C205" r:id="rId589" xr:uid="{26F9A583-2496-4B17-A929-300CBDA2E24D}"/>
+    <hyperlink ref="D205" r:id="rId590" xr:uid="{6719EDC2-583C-49D3-9ECA-9AAEAB5A1AF8}"/>
+    <hyperlink ref="E205" r:id="rId591" xr:uid="{3243DF7A-EE24-42C4-9051-EF34793BE812}"/>
+    <hyperlink ref="C206" r:id="rId592" xr:uid="{4C45050E-CAB2-4E91-876A-26ACF94DB8B2}"/>
+    <hyperlink ref="D206" r:id="rId593" xr:uid="{4FE2A5B0-C928-4394-8042-D3AA021DA4D8}"/>
+    <hyperlink ref="E206" r:id="rId594" xr:uid="{CAB1117F-895B-408D-BFB0-CC8642447B67}"/>
+    <hyperlink ref="C207" r:id="rId595" xr:uid="{3497FE2B-F080-4F0F-9454-A2F8E2BCEA79}"/>
+    <hyperlink ref="D207" r:id="rId596" xr:uid="{C1B80CC4-8153-4B20-A3F2-B283168811C5}"/>
+    <hyperlink ref="E207" r:id="rId597" xr:uid="{BF0434BE-354E-4789-9E21-F298661908C9}"/>
+    <hyperlink ref="C171" r:id="rId598" xr:uid="{E432FEE7-0CE3-4671-A6DE-A89067FE71F8}"/>
+    <hyperlink ref="D171" r:id="rId599" xr:uid="{9B118C1B-E5E7-4F47-BFA5-206491EA6ED8}"/>
+    <hyperlink ref="E171" r:id="rId600" xr:uid="{9EA9596A-CB3D-4B30-8E07-CA8A3FF7C508}"/>
+    <hyperlink ref="C86" r:id="rId601" xr:uid="{46C6222B-B670-40C3-A605-FABE1731989A}"/>
+    <hyperlink ref="D86" r:id="rId602" xr:uid="{C653707F-D543-43CC-A01D-24A54A6A319B}"/>
+    <hyperlink ref="E86" r:id="rId603" xr:uid="{60116EA4-2834-4C7A-B4DB-1CE223CB90BB}"/>
+    <hyperlink ref="C96" r:id="rId604" xr:uid="{20EC698E-A69F-497B-8D14-1C5CA444BC21}"/>
+    <hyperlink ref="D96" r:id="rId605" xr:uid="{AFAB7C9A-C544-47BD-8645-5C31CE7C5CF3}"/>
+    <hyperlink ref="E96" r:id="rId606" xr:uid="{F53AF2AB-0CE9-45A6-B905-24C7FEEA3E52}"/>
+    <hyperlink ref="C95" r:id="rId607" xr:uid="{30CD9287-A385-456E-9D5E-59944E3156E1}"/>
+    <hyperlink ref="D95" r:id="rId608" xr:uid="{C9FDF5BB-9B0E-442F-AE18-EBCAF9FA12BA}"/>
+    <hyperlink ref="E95" r:id="rId609" xr:uid="{E3661C98-D989-4879-A8FC-B6166662C8D7}"/>
+    <hyperlink ref="C55" r:id="rId610" xr:uid="{2102EDB4-6981-4633-9FD3-E647448181FC}"/>
+    <hyperlink ref="D55" r:id="rId611" xr:uid="{0DB9D726-23FB-4B78-94AC-DFD7B21AB5AE}"/>
+    <hyperlink ref="E55" r:id="rId612" xr:uid="{BF7B36EC-2642-4F9B-A942-FC7DA39117FB}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId618"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId613"/>
 </worksheet>
 </file>
 
@@ -6187,13 +6458,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>